<commit_message>
Added to prod document
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F54822D-A434-4823-9519-84BE7CDC8451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197B052B-7ED0-455F-851C-28D2EEF714FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Gantt Chart" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Task Tracking'!$A$1:$R$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Task Tracking'!$A$1:$R$72</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -141,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="155">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -464,9 +466,6 @@
     <t>Create Act 2 level 3</t>
   </si>
   <si>
-    <t>Create Act 2 level 4</t>
-  </si>
-  <si>
     <t>Create Act 3 level 1</t>
   </si>
   <si>
@@ -476,15 +475,9 @@
     <t>Create Act 3 level 3</t>
   </si>
   <si>
-    <t>Create Act 3 level 4</t>
-  </si>
-  <si>
     <t>Levels are to demonstrate more complexity, also requiring final capabilities</t>
   </si>
   <si>
-    <t>Filter Act 1 into only 4 best levels</t>
-  </si>
-  <si>
     <t>Do as said</t>
   </si>
   <si>
@@ -531,6 +524,90 @@
   </si>
   <si>
     <t>Lauren has a vision</t>
+  </si>
+  <si>
+    <t>Filter Act 1 into only 3 best levels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bulk out the levels in each act </t>
+  </si>
+  <si>
+    <t>Use floating coloured spirit masks on goals to make them read better</t>
+  </si>
+  <si>
+    <t>Lever on mushroom level moves but does not actually execute its function</t>
+  </si>
+  <si>
+    <t>Straight forward</t>
+  </si>
+  <si>
+    <t>Texture everything in act 2. Colab with Angus on socials.</t>
+  </si>
+  <si>
+    <t>Particle effects, start implementing from game, think about using the magic masks. Make the eyes glow with a slight trail.</t>
+  </si>
+  <si>
+    <t>Glowing eyes with slight trail</t>
+  </si>
+  <si>
+    <t>Shader for puppets when they go behind obstacles</t>
+  </si>
+  <si>
+    <t>Make them the same colour as the player, consider using plugin which makes it work</t>
+  </si>
+  <si>
+    <t>No jumping up, especially on player jumps</t>
+  </si>
+  <si>
+    <t>Restrict the camera pan</t>
+  </si>
+  <si>
+    <t>Waiting for sound files, if not replied in 3 days, will start designing mp3 for level track.</t>
+  </si>
+  <si>
+    <t>Level selection screen, broken into 3 acts and 3 level boxes</t>
+  </si>
+  <si>
+    <t>Redo the game soundtrack and music effects</t>
+  </si>
+  <si>
+    <t>Scrap the old one or just keep the percussion and rebuild from there</t>
+  </si>
+  <si>
+    <t>Make the gridded  movement more tolerant</t>
+  </si>
+  <si>
+    <t>Junctions are a bit janky, have to ensure player is able to turn easily enough</t>
+  </si>
+  <si>
+    <t>Implement gridded movement system into the main branch</t>
+  </si>
+  <si>
+    <t>Use Tim's grid engine, must breif team on how to effectively use it when constructing levels</t>
+  </si>
+  <si>
+    <t>Restructure old levels using the grid based system</t>
+  </si>
+  <si>
+    <t>Chance here to also improve narrative and progressive teaching of mechanics, consider moving tangling earlier in the piece.</t>
+  </si>
+  <si>
+    <t>Import new stage model</t>
+  </si>
+  <si>
+    <t>Replace the old model, optimise the grid to get a blance of enough lines to move on</t>
+  </si>
+  <si>
+    <t>Add more props and general items as well as backdrop to enhance the stag effect</t>
+  </si>
+  <si>
+    <t>Make the camera start very zoomed in the first level</t>
+  </si>
+  <si>
+    <t>Better displays the characters and gets the player into the narrative, also can be used to teach about the strings and actually make sense cause they'll be able to read the puppets</t>
+  </si>
+  <si>
+    <t>Particle effects needed here as well as the actual model for each mask but made transparent</t>
   </si>
 </sst>
 </file>
@@ -693,7 +770,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -751,12 +828,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -773,11 +844,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="11">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -869,316 +949,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAF8A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAF8A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1507,24 +1277,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
-  <dimension ref="A1:R62"/>
+  <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="18" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="18" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>90</v>
       </c>
@@ -1567,7 +1337,7 @@
       <c r="N1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="O1" s="30" t="s">
+      <c r="O1" s="28" t="s">
         <v>50</v>
       </c>
       <c r="P1" s="2" t="s">
@@ -1580,25 +1350,25 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>105</v>
+        <v>146</v>
       </c>
       <c r="D2" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="1" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>96</v>
@@ -1607,147 +1377,111 @@
         <v>96</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>104</v>
+        <v>147</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>105</v>
+        <v>148</v>
       </c>
       <c r="D3" s="4">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="1" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="D4" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="1" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>105</v>
@@ -1769,49 +1503,49 @@
         <v>96</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D6" s="4">
         <v>4</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="1" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>96</v>
@@ -1823,49 +1557,49 @@
         <v>96</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D7" s="4">
         <v>4</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="1" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>96</v>
@@ -1877,42 +1611,42 @@
         <v>96</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="D8" s="4">
         <v>4</v>
@@ -1931,42 +1665,42 @@
         <v>96</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D9" s="4">
         <v>4</v>
@@ -1976,7 +1710,7 @@
         <v>73</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>96</v>
@@ -1985,42 +1719,42 @@
         <v>96</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D10" s="4">
         <v>4</v>
@@ -2033,55 +1767,55 @@
         <v>95</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>9</v>
+      <c r="B11" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="1">
-        <v>10</v>
-      </c>
-      <c r="E11" s="1"/>
+        <v>111</v>
+      </c>
+      <c r="D11" s="4">
+        <v>4</v>
+      </c>
+      <c r="E11" s="4"/>
       <c r="F11" s="1" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>95</v>
@@ -2093,103 +1827,83 @@
         <v>95</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>128</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>143</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D12" s="1">
-        <v>12</v>
-      </c>
-      <c r="E12" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>91</v>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>23</v>
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="D13" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>95</v>
@@ -2201,47 +1915,49 @@
         <v>95</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>34</v>
+      <c r="B14" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="1"/>
+        <v>153</v>
+      </c>
+      <c r="D14" s="1">
+        <v>4</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>95</v>
@@ -2252,427 +1968,411 @@
       <c r="I14" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+    </row>
+    <row r="15" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>117</v>
+        <v>128</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="D15" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="H15" s="25" t="s">
+      <c r="F15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" s="1">
+        <v>12</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="1">
+        <v>4</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D20" s="1">
         <v>0.5</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E20" s="1">
         <v>0.5</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F20" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="G20" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="J20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C21" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D21" s="5">
         <v>2</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="29" t="s">
+      <c r="E21" s="5"/>
+      <c r="F21" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R17" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="G21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D22" s="5">
         <v>2</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="1" t="s">
+      <c r="E22" s="5"/>
+      <c r="F22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D20" s="1">
-        <v>4</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="1">
-        <v>4</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="1">
-        <v>8</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="G22" s="1" t="s">
         <v>95</v>
       </c>
@@ -2683,102 +2383,100 @@
         <v>95</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>21</v>
+      <c r="B23" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="5">
+        <v>6</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="25" t="s">
+        <v>37</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>95</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="1">
-        <v>2</v>
-      </c>
+      <c r="B24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="25" t="s">
         <v>25</v>
       </c>
       <c r="G24" s="1" t="s">
@@ -2791,101 +2489,103 @@
         <v>95</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>28</v>
+      <c r="B25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="D25" s="1">
         <v>4</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>95</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="3"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="D26" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>95</v>
@@ -2897,47 +2597,47 @@
         <v>95</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>38</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>95</v>
@@ -2949,103 +2649,103 @@
         <v>95</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>101</v>
-      </c>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="4"/>
       <c r="D28" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="1">
         <v>2</v>
       </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E29" s="4"/>
+      <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>95</v>
@@ -3057,49 +2757,49 @@
         <v>95</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>15</v>
+        <v>92</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="D30" s="1">
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>95</v>
@@ -3111,160 +2811,654 @@
         <v>95</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="1">
         <v>2</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1">
-        <v>3</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="1">
         <v>6</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="N31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="E35" s="1"/>
+      <c r="F35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D36" s="1">
+        <v>2</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D37" s="1">
+        <v>3</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R38" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="1">
+        <v>3</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R40" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>102</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F64" t="s">
         <v>7</v>
       </c>
-      <c r="G55" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="G64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>91</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F65" t="s">
         <v>21</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G65" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>92</v>
+      </c>
+      <c r="F66" t="s">
+        <v>25</v>
+      </c>
+      <c r="G66" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>92</v>
-      </c>
-      <c r="F57" t="s">
-        <v>25</v>
-      </c>
-      <c r="G57" t="s">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>93</v>
+      </c>
+      <c r="F67" t="s">
+        <v>5</v>
+      </c>
+      <c r="G67" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>93</v>
-      </c>
-      <c r="F58" t="s">
-        <v>5</v>
-      </c>
-      <c r="G58" t="s">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F68" t="s">
+        <v>80</v>
+      </c>
+      <c r="G68" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F59" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F60" t="s">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F69" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F61" t="s">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F70" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F62" t="s">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F71" t="s">
         <v>73</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R63" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}"/>
-  <conditionalFormatting sqref="A2:A31">
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+  <autoFilter ref="A1:R72" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}"/>
+  <conditionalFormatting sqref="A2:A40">
+    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:R31">
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="G69:R1048576 H64:R68 G65:G68 G1:R63">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",G1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+      <formula>"Done (Needs Testing)"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
+      <formula>"Started"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3273,19 +3467,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:R1048576">
-    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",G1)))</formula>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",B20)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"Done (Needs Testing)"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="G5:R40">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3294,29 +3488,28 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",B16)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
-      <formula>"Done (Needs Testing)"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
-      <formula>"Started"</formula>
+  <conditionalFormatting sqref="G2:R4">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F30:F31 F11:F28" xr:uid="{1BB046FB-46C3-40BC-B6E1-E30D1F0B9ED1}">
-      <formula1>$F$55:$F$63</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F39:F40 F13:F37" xr:uid="{1BB046FB-46C3-40BC-B6E1-E30D1F0B9ED1}">
+      <formula1>$F$64:$F$72</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F13 F29" xr:uid="{7C14EC72-7C28-4BF3-AF6C-60555A8DBEF9}">
-      <formula1>$F$55:$F$62</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F38 F2:F17" xr:uid="{7C14EC72-7C28-4BF3-AF6C-60555A8DBEF9}">
+      <formula1>$F$64:$F$71</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:R31" xr:uid="{74781059-03CD-4747-BF6A-E35BF8F2BF2E}">
-      <formula1>$G$55:$G$58</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A40" xr:uid="{D3DB8CA4-CF09-459F-A4BC-4F324FE8B47E}">
+      <formula1>$A$64:$A$67</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A31" xr:uid="{D3DB8CA4-CF09-459F-A4BC-4F324FE8B47E}">
-      <formula1>$A$55:$A$58</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:R40" xr:uid="{74781059-03CD-4747-BF6A-E35BF8F2BF2E}">
+      <formula1>$G$64:$G$68</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3327,20 +3520,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B9" sqref="B9:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="48.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="48.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>90</v>
       </c>
@@ -3348,117 +3541,134 @@
         <v>94</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D27" t="s">
+      <c r="B4" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>91</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>21</v>
       </c>
-      <c r="E28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="E29" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>92</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>25</v>
       </c>
-      <c r="E29" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="E30" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>93</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
         <v>73</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A3">
+  <conditionalFormatting sqref="A2:A4">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E3">
+  <conditionalFormatting sqref="E2:E4">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
@@ -3470,14 +3680,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
-      <formula1>$D$27:$D$34</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
+      <formula1>$D$28:$D$35</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A3" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
-      <formula1>$A$27:$A$30</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
+      <formula1>$A$28:$A$31</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
-      <formula1>$E$27:$E$29</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
+      <formula1>$E$28:$E$30</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3489,47 +3699,47 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="16" customWidth="1"/>
-    <col min="4" max="5" width="17.85546875" style="16" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" style="17" customWidth="1"/>
-    <col min="7" max="11" width="17.85546875" style="16" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" style="16" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" style="16" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="16"/>
+    <col min="1" max="1" width="24.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="16" customWidth="1"/>
+    <col min="4" max="5" width="17.88671875" style="16" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="17" customWidth="1"/>
+    <col min="7" max="11" width="17.88671875" style="16" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" style="16" customWidth="1"/>
+    <col min="13" max="13" width="16.88671875" style="16" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9"/>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-    </row>
-    <row r="2" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+    </row>
+    <row r="2" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>89</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="30" t="s">
         <v>43</v>
       </c>
       <c r="D2" s="9" t="s">
@@ -3563,7 +3773,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>25</v>
       </c>
@@ -3584,7 +3794,7 @@
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
     </row>
-    <row r="4" spans="1:13" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>21</v>
       </c>
@@ -3605,7 +3815,7 @@
       <c r="L4" s="18"/>
       <c r="M4" s="18"/>
     </row>
-    <row r="5" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>5</v>
       </c>
@@ -3615,7 +3825,9 @@
       <c r="C5" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="18"/>
+      <c r="D5" s="18" t="s">
+        <v>133</v>
+      </c>
       <c r="E5" s="18"/>
       <c r="F5" s="19"/>
       <c r="G5" s="18"/>
@@ -3626,7 +3838,7 @@
       <c r="L5" s="18"/>
       <c r="M5" s="18"/>
     </row>
-    <row r="6" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>37</v>
       </c>
@@ -3636,7 +3848,9 @@
       <c r="C6" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="18"/>
+      <c r="D6" s="18" t="s">
+        <v>139</v>
+      </c>
       <c r="E6" s="18"/>
       <c r="F6" s="19"/>
       <c r="G6" s="18"/>
@@ -3647,7 +3861,7 @@
       <c r="L6" s="18"/>
       <c r="M6" s="18"/>
     </row>
-    <row r="7" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>80</v>
       </c>
@@ -3657,7 +3871,9 @@
       <c r="C7" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="18"/>
+      <c r="D7" s="18" t="s">
+        <v>132</v>
+      </c>
       <c r="E7" s="18"/>
       <c r="F7" s="19"/>
       <c r="G7" s="18"/>
@@ -3668,7 +3884,7 @@
       <c r="L7" s="18"/>
       <c r="M7" s="18"/>
     </row>
-    <row r="8" spans="1:13" ht="180" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="144" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>6</v>
       </c>
@@ -3689,7 +3905,7 @@
       <c r="L8" s="18"/>
       <c r="M8" s="18"/>
     </row>
-    <row r="9" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>7</v>
       </c>
@@ -3710,7 +3926,7 @@
       <c r="L9" s="18"/>
       <c r="M9" s="18"/>
     </row>
-    <row r="10" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>73</v>
       </c>
@@ -3731,7 +3947,7 @@
       <c r="L10" s="18"/>
       <c r="M10" s="18"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>70</v>
       </c>
@@ -3741,7 +3957,9 @@
       <c r="C11" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="18"/>
+      <c r="D11" s="18" t="s">
+        <v>140</v>
+      </c>
       <c r="E11" s="18"/>
       <c r="F11" s="19"/>
       <c r="G11" s="18"/>
@@ -3769,33 +3987,33 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="9"/>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="30" t="s">
         <v>43</v>
       </c>
       <c r="D2" s="10" t="s">
@@ -3829,24 +4047,24 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>55</v>
       </c>
@@ -3863,7 +4081,7 @@
       <c r="L4" s="15"/>
       <c r="M4" s="15"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>56</v>
       </c>
@@ -3880,24 +4098,24 @@
       <c r="L5" s="14"/>
       <c r="M5" s="14"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>58</v>
       </c>
@@ -3914,7 +4132,7 @@
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>59</v>
       </c>
@@ -3931,7 +4149,7 @@
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>60</v>
       </c>
@@ -3948,7 +4166,7 @@
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>61</v>
       </c>
@@ -3965,24 +4183,24 @@
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>63</v>
       </c>
@@ -3999,7 +4217,7 @@
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>64</v>
       </c>
@@ -4016,7 +4234,7 @@
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>65</v>
       </c>
@@ -4033,24 +4251,24 @@
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>67</v>
       </c>
@@ -4067,7 +4285,7 @@
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
Added a fresh title screen, get keen
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197B052B-7ED0-455F-851C-28D2EEF714FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0804138F-879E-4EFC-B415-910E63489186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Gantt Chart" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Task Tracking'!$A$1:$R$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Task Tracking'!$A$1:$R$73</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="156">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -574,9 +574,6 @@
     <t>Scrap the old one or just keep the percussion and rebuild from there</t>
   </si>
   <si>
-    <t>Make the gridded  movement more tolerant</t>
-  </si>
-  <si>
     <t>Junctions are a bit janky, have to ensure player is able to turn easily enough</t>
   </si>
   <si>
@@ -608,6 +605,12 @@
   </si>
   <si>
     <t>Particle effects needed here as well as the actual model for each mask but made transparent</t>
+  </si>
+  <si>
+    <t>Change dying image to somethiong else</t>
+  </si>
+  <si>
+    <t>Make the gridded movement more tolerant</t>
   </si>
 </sst>
 </file>
@@ -844,14 +847,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1277,24 +1280,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
-  <dimension ref="A1:R71"/>
+  <dimension ref="A1:R72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.88671875" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="18" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="18" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>90</v>
       </c>
@@ -1350,15 +1353,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="D2" s="4">
         <v>8</v>
@@ -1404,15 +1407,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="D3" s="4">
         <v>10</v>
@@ -1430,25 +1433,43 @@
       <c r="I3" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-    </row>
-    <row r="4" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -1466,17 +1487,35 @@
       <c r="I4" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-    </row>
-    <row r="5" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>102</v>
       </c>
@@ -1530,7 +1569,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>102</v>
       </c>
@@ -1584,7 +1623,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>102</v>
       </c>
@@ -1638,7 +1677,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>102</v>
       </c>
@@ -1692,7 +1731,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>102</v>
       </c>
@@ -1746,7 +1785,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>102</v>
       </c>
@@ -1800,7 +1839,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>102</v>
       </c>
@@ -1854,15 +1893,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>144</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1878,17 +1917,35 @@
       <c r="I12" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>102</v>
       </c>
@@ -1942,15 +1999,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="D14" s="1">
         <v>4</v>
@@ -1968,17 +2025,35 @@
       <c r="I14" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-    </row>
-    <row r="15" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>91</v>
       </c>
@@ -1986,7 +2061,7 @@
         <v>128</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D15" s="1">
         <v>12</v>
@@ -2032,7 +2107,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>91</v>
       </c>
@@ -2086,7 +2161,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>91</v>
       </c>
@@ -2140,7 +2215,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>91</v>
       </c>
@@ -2192,7 +2267,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>91</v>
       </c>
@@ -2246,7 +2321,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>91</v>
       </c>
@@ -2302,21 +2377,21 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="26" t="s">
-        <v>31</v>
+        <v>154</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="D21" s="5">
         <v>2</v>
       </c>
       <c r="E21" s="5"/>
-      <c r="F21" s="27" t="s">
+      <c r="F21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G21" s="1" t="s">
@@ -2356,21 +2431,21 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>31</v>
       </c>
       <c r="D22" s="5">
         <v>2</v>
       </c>
       <c r="E22" s="5"/>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="27" t="s">
         <v>7</v>
       </c>
       <c r="G22" s="1" t="s">
@@ -2410,84 +2485,86 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:18" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="5">
+        <v>2</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C23" s="33" t="s">
+      <c r="C24" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D24" s="5">
         <v>6</v>
       </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="25" t="s">
+      <c r="E24" s="5"/>
+      <c r="F24" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I23" s="1" t="s">
+      <c r="G24" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J23" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="J24" s="1" t="s">
         <v>69</v>
       </c>
@@ -2516,85 +2593,83 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="D25" s="1">
-        <v>4</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="D26" s="1">
         <v>4</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>95</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>69</v>
@@ -2624,20 +2699,22 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="D27" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>95</v>
@@ -2676,86 +2753,84 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="1">
+        <v>8</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="1">
+      <c r="C29" s="4"/>
+      <c r="D29" s="1">
         <v>0.5</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E29" s="1">
         <v>0.5</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H28" s="1" t="s">
+      <c r="G29" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="1">
-        <v>2</v>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="J29" s="1" t="s">
         <v>69</v>
       </c>
@@ -2784,22 +2859,22 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D30" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>95</v>
@@ -2838,20 +2913,22 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C31" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="D31" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>95</v>
@@ -2860,7 +2937,7 @@
         <v>95</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>69</v>
@@ -2890,16 +2967,14 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>136</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="C32" s="4"/>
       <c r="D32" s="1">
         <v>2</v>
       </c>
@@ -2914,7 +2989,7 @@
         <v>95</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>69</v>
@@ -2944,22 +3019,22 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D33" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>95</v>
@@ -2998,20 +3073,22 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="3"/>
+      <c r="B34" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>137</v>
+      </c>
       <c r="D34" s="1">
         <v>1</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>95</v>
@@ -3050,20 +3127,20 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>95</v>
@@ -3102,22 +3179,20 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>101</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C36" s="3"/>
       <c r="D36" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>95</v>
@@ -3156,22 +3231,22 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>129</v>
+        <v>39</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
       <c r="D37" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>95</v>
@@ -3180,7 +3255,7 @@
         <v>95</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>69</v>
@@ -3210,20 +3285,20 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E38" s="4"/>
+        <v>153</v>
+      </c>
+      <c r="D38" s="1">
+        <v>3</v>
+      </c>
+      <c r="E38" s="1"/>
       <c r="F38" s="1" t="s">
         <v>5</v>
       </c>
@@ -3234,7 +3309,7 @@
         <v>95</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>69</v>
@@ -3264,20 +3339,20 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" s="1">
+        <v>14</v>
+      </c>
+      <c r="D39" s="4">
         <v>0.5</v>
       </c>
-      <c r="E39" s="1"/>
+      <c r="E39" s="4"/>
       <c r="F39" s="1" t="s">
         <v>5</v>
       </c>
@@ -3318,135 +3393,189 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D40" s="1">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R40" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="1">
+        <v>3</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="N40" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="O40" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q40" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="R40" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+      <c r="G41" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R41" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>102</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F65" t="s">
         <v>7</v>
       </c>
-      <c r="G64" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+      <c r="G65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>91</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F66" t="s">
         <v>21</v>
       </c>
-      <c r="G65" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+      <c r="G66" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>92</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F67" t="s">
         <v>25</v>
       </c>
-      <c r="G66" t="s">
+      <c r="G67" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>93</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F68" t="s">
         <v>5</v>
       </c>
-      <c r="G67" t="s">
+      <c r="G68" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F68" t="s">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F69" t="s">
         <v>80</v>
       </c>
-      <c r="G68" t="s">
+      <c r="G69" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F69" t="s">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F70" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F70" t="s">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F71" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F71" t="s">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F72" t="s">
         <v>73</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R72" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}"/>
-  <conditionalFormatting sqref="A2:A40">
+  <autoFilter ref="A1:R73" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}"/>
+  <conditionalFormatting sqref="A2:A41">
     <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G69:R1048576 H64:R68 G65:G68 G1:R63">
+  <conditionalFormatting sqref="G70:R1048576 H65:R69 G66:G69 G1:R64">
     <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",G1)))</formula>
     </cfRule>
@@ -3478,7 +3607,7 @@
       <formula>"Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5:R40">
+  <conditionalFormatting sqref="G5:R41">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -3499,17 +3628,17 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F39:F40 F13:F37" xr:uid="{1BB046FB-46C3-40BC-B6E1-E30D1F0B9ED1}">
-      <formula1>$F$64:$F$72</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F40:F41 F13:F38" xr:uid="{1BB046FB-46C3-40BC-B6E1-E30D1F0B9ED1}">
+      <formula1>$F$65:$F$73</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F38 F2:F17" xr:uid="{7C14EC72-7C28-4BF3-AF6C-60555A8DBEF9}">
-      <formula1>$F$64:$F$71</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F39 F2:F17" xr:uid="{7C14EC72-7C28-4BF3-AF6C-60555A8DBEF9}">
+      <formula1>$F$65:$F$72</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A40" xr:uid="{D3DB8CA4-CF09-459F-A4BC-4F324FE8B47E}">
-      <formula1>$A$64:$A$67</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A41" xr:uid="{D3DB8CA4-CF09-459F-A4BC-4F324FE8B47E}">
+      <formula1>$A$65:$A$68</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:R40" xr:uid="{74781059-03CD-4747-BF6A-E35BF8F2BF2E}">
-      <formula1>$G$64:$G$68</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:R41" xr:uid="{74781059-03CD-4747-BF6A-E35BF8F2BF2E}">
+      <formula1>$G$65:$G$69</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3523,17 +3652,17 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="48.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="48.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>90</v>
       </c>
@@ -3550,7 +3679,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
@@ -3567,7 +3696,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>92</v>
       </c>
@@ -3584,7 +3713,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>102</v>
       </c>
@@ -3601,7 +3730,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -3612,7 +3741,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>91</v>
       </c>
@@ -3623,7 +3752,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>92</v>
       </c>
@@ -3634,7 +3763,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>93</v>
       </c>
@@ -3642,22 +3771,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>73</v>
       </c>
@@ -3702,37 +3831,37 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="16" customWidth="1"/>
-    <col min="4" max="5" width="17.88671875" style="16" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="17" customWidth="1"/>
-    <col min="7" max="11" width="17.88671875" style="16" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" style="16" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" style="16" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="16"/>
+    <col min="1" max="1" width="24.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="16" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" style="16" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="17" customWidth="1"/>
+    <col min="7" max="11" width="17.85546875" style="16" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="16" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="16" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-    </row>
-    <row r="2" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+    </row>
+    <row r="2" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>89</v>
       </c>
@@ -3773,7 +3902,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>25</v>
       </c>
@@ -3794,7 +3923,7 @@
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
     </row>
-    <row r="4" spans="1:13" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>21</v>
       </c>
@@ -3815,7 +3944,7 @@
       <c r="L4" s="18"/>
       <c r="M4" s="18"/>
     </row>
-    <row r="5" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>5</v>
       </c>
@@ -3838,7 +3967,7 @@
       <c r="L5" s="18"/>
       <c r="M5" s="18"/>
     </row>
-    <row r="6" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>37</v>
       </c>
@@ -3861,7 +3990,7 @@
       <c r="L6" s="18"/>
       <c r="M6" s="18"/>
     </row>
-    <row r="7" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>80</v>
       </c>
@@ -3884,7 +4013,7 @@
       <c r="L7" s="18"/>
       <c r="M7" s="18"/>
     </row>
-    <row r="8" spans="1:13" ht="144" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>6</v>
       </c>
@@ -3905,7 +4034,7 @@
       <c r="L8" s="18"/>
       <c r="M8" s="18"/>
     </row>
-    <row r="9" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>7</v>
       </c>
@@ -3926,7 +4055,7 @@
       <c r="L9" s="18"/>
       <c r="M9" s="18"/>
     </row>
-    <row r="10" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>73</v>
       </c>
@@ -3947,7 +4076,7 @@
       <c r="L10" s="18"/>
       <c r="M10" s="18"/>
     </row>
-    <row r="11" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>70</v>
       </c>
@@ -3987,26 +4116,26 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>41</v>
       </c>
@@ -4047,24 +4176,24 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>55</v>
       </c>
@@ -4081,7 +4210,7 @@
       <c r="L4" s="15"/>
       <c r="M4" s="15"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>56</v>
       </c>
@@ -4098,24 +4227,24 @@
       <c r="L5" s="14"/>
       <c r="M5" s="14"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>58</v>
       </c>
@@ -4132,7 +4261,7 @@
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>59</v>
       </c>
@@ -4149,7 +4278,7 @@
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>60</v>
       </c>
@@ -4166,7 +4295,7 @@
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>61</v>
       </c>
@@ -4183,24 +4312,24 @@
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="32" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>63</v>
       </c>
@@ -4217,7 +4346,7 @@
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>64</v>
       </c>
@@ -4234,7 +4363,7 @@
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>65</v>
       </c>
@@ -4251,24 +4380,24 @@
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="32" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="33"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>67</v>
       </c>
@@ -4285,7 +4414,7 @@
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
Fixed music transition with fade out
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0804138F-879E-4EFC-B415-910E63489186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E49816-4F50-4E32-AE8A-2E0771064BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="1785" yWindow="1245" windowWidth="21600" windowHeight="11235" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -607,10 +607,10 @@
     <t>Particle effects needed here as well as the actual model for each mask but made transparent</t>
   </si>
   <si>
-    <t>Change dying image to somethiong else</t>
-  </si>
-  <si>
     <t>Make the gridded movement more tolerant</t>
+  </si>
+  <si>
+    <t>Change dying image to something else</t>
   </si>
 </sst>
 </file>
@@ -773,7 +773,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -855,6 +855,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1282,8 +1285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1898,7 +1901,7 @@
         <v>102</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>143</v>
@@ -2382,7 +2385,7 @@
         <v>91</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>33</v>
@@ -2392,7 +2395,7 @@
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>95</v>
@@ -2435,7 +2438,7 @@
       <c r="A22" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="34" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="26" t="s">
@@ -2452,10 +2455,10 @@
         <v>95</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
Added grid changes to prod doc
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C32872-364A-43CE-9B42-D82206F8DDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B8C50A-07BB-4403-9A16-B5F0ECD1B0DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Gantt Chart" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Task Tracking'!$A$1:$R$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Task Tracking'!$A$1:$R$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="163">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -620,6 +620,18 @@
   </si>
   <si>
     <t>Done (Needs Review)</t>
+  </si>
+  <si>
+    <t>Make grid separate for each level</t>
+  </si>
+  <si>
+    <t>Decide on standard grid dimensions going forward</t>
+  </si>
+  <si>
+    <t>Hiding the entire object of a level doesn't actually skip it</t>
+  </si>
+  <si>
+    <t>Left in an empty scene, also happens when you skip level 1 but level 2 is greyed out</t>
   </si>
 </sst>
 </file>
@@ -872,21 +884,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="12">
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAF8A4"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -911,39 +916,12 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAF8A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4FBA9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1003,41 +981,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color theme="9" tint="-0.499984740745262"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFC4FBA9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1367,10 +1315,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
-  <dimension ref="A1:R72"/>
+  <dimension ref="A1:R74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1464,7 +1412,7 @@
         <v>93</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>66</v>
@@ -1494,22 +1442,20 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>144</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="C3" s="3"/>
       <c r="D3" s="4">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="1" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>92</v>
@@ -1607,23 +1553,21 @@
         <v>99</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>102</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="C5" s="3"/>
       <c r="D5" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="1" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>93</v>
@@ -1656,28 +1600,28 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>102</v>
+        <v>144</v>
       </c>
       <c r="D6" s="4">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="1" t="s">
         <v>70</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>93</v>
@@ -1715,7 +1659,7 @@
         <v>99</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>102</v>
@@ -1769,10 +1713,10 @@
         <v>99</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D8" s="4">
         <v>4</v>
@@ -1823,10 +1767,10 @@
         <v>99</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D9" s="4">
         <v>4</v>
@@ -1836,7 +1780,7 @@
         <v>70</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>93</v>
@@ -1877,7 +1821,7 @@
         <v>99</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>107</v>
@@ -1890,7 +1834,7 @@
         <v>70</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>93</v>
@@ -1931,10 +1875,10 @@
         <v>99</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D11" s="4">
         <v>4</v>
@@ -1947,10 +1891,10 @@
         <v>92</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>66</v>
@@ -1985,21 +1929,23 @@
         <v>99</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>151</v>
+        <v>106</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D12" s="4"/>
+        <v>107</v>
+      </c>
+      <c r="D12" s="4">
+        <v>4</v>
+      </c>
       <c r="E12" s="4"/>
       <c r="F12" s="1" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>92</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>93</v>
@@ -2032,142 +1978,140 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="4">
+        <v>4</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C15" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D15" s="5">
         <v>5</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E15" s="5">
         <v>6.5</v>
       </c>
-      <c r="F13" s="27" t="s">
+      <c r="F15" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H13" s="1" t="s">
+      <c r="G15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="D14" s="1">
-        <v>4</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D15" s="1">
-        <v>12</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="J15" s="1" t="s">
         <v>66</v>
       </c>
@@ -2196,31 +2140,31 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
       <c r="D16" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>92</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>66</v>
@@ -2251,21 +2195,21 @@
       </c>
     </row>
     <row r="17" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>21</v>
+        <v>125</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>147</v>
       </c>
       <c r="D17" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>92</v>
@@ -2304,139 +2248,137 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>31</v>
+      <c r="B18" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="1"/>
+        <v>123</v>
+      </c>
+      <c r="D18" s="1">
+        <v>12</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D19" s="1">
-        <v>4</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G19" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="H19" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B20" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>93</v>
+      <c r="G20" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>66</v>
@@ -2466,31 +2408,31 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:18" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>152</v>
+        <v>110</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="5">
-        <v>2</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H21" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" s="1">
+        <v>4</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="23" t="s">
         <v>92</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>66</v>
@@ -2520,31 +2462,33 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>29</v>
+      <c r="B22" s="29" t="s">
+        <v>8</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="5">
-        <v>2</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>92</v>
+      <c r="G22" s="23" t="s">
+        <v>93</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>66</v>
@@ -2576,132 +2520,134 @@
     </row>
     <row r="23" spans="1:18" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="5">
+        <v>2</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="5">
+        <v>2</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C25" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D25" s="5">
         <v>6</v>
       </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="25" t="s">
+      <c r="E25" s="5"/>
+      <c r="F25" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D25" s="1">
-        <v>4</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="G25" s="1" t="s">
         <v>92</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>93</v>
@@ -2734,22 +2680,20 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="1">
+      <c r="B26" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="C26" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1" t="s">
-        <v>19</v>
+      <c r="F26" s="25" t="s">
+        <v>23</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>92</v>
@@ -2788,29 +2732,31 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+    <row r="27" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="3"/>
+      <c r="B27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="D27" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>92</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>66</v>
@@ -2840,31 +2786,31 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B28" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="4"/>
+      <c r="B28" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="D28" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E28" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="F28" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>92</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>66</v>
@@ -2894,139 +2840,137 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="1">
+        <v>8</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D31" s="1">
         <v>3</v>
       </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="5" t="s">
+      <c r="E31" s="1"/>
+      <c r="F31" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I29" s="1" t="s">
+      <c r="G31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R29" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="1">
-        <v>2</v>
-      </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R30" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D31" s="1">
-        <v>4</v>
-      </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>66</v>
@@ -3058,18 +3002,20 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C32" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="D32" s="1">
         <v>2</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>92</v>
@@ -3078,7 +3024,7 @@
         <v>92</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>66</v>
@@ -3108,22 +3054,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>132</v>
+        <v>25</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>133</v>
+        <v>26</v>
       </c>
       <c r="D33" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>92</v>
@@ -3167,17 +3113,15 @@
         <v>90</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>134</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="C34" s="4"/>
       <c r="D34" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>92</v>
@@ -3186,7 +3130,7 @@
         <v>92</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>66</v>
@@ -3220,16 +3164,18 @@
       <c r="A35" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="3"/>
+      <c r="B35" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="D35" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>92</v>
@@ -3268,20 +3214,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="3"/>
+      <c r="B36" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="D36" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>92</v>
@@ -3325,17 +3273,15 @@
         <v>90</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>98</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C37" s="3"/>
       <c r="D37" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>92</v>
@@ -3379,13 +3325,11 @@
         <v>90</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>150</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C38" s="3"/>
       <c r="D38" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1" t="s">
@@ -3398,7 +3342,7 @@
         <v>92</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>66</v>
@@ -3428,22 +3372,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E39" s="4"/>
+        <v>98</v>
+      </c>
+      <c r="D39" s="1">
+        <v>2</v>
+      </c>
+      <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>92</v>
@@ -3482,18 +3426,18 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1</v>
+        <v>126</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>14</v>
+        <v>150</v>
       </c>
       <c r="D40" s="1">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1" t="s">
@@ -3506,7 +3450,7 @@
         <v>92</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>66</v>
@@ -3536,167 +3480,275 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E41" s="4"/>
+      <c r="F41" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R41" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R42" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D43" s="1">
         <v>3</v>
       </c>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1" t="s">
+      <c r="E43" s="1"/>
+      <c r="F43" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L41" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M41" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N41" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O41" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P41" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q41" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R41" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K47" t="s">
+      <c r="G43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R43" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K49" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K48" t="s">
+    <row r="50" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K50" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="64" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F64" t="s">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F66" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>99</v>
-      </c>
-      <c r="F65" t="s">
-        <v>7</v>
-      </c>
-      <c r="G65" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>88</v>
-      </c>
-      <c r="F66" t="s">
-        <v>19</v>
-      </c>
-      <c r="G66" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="F67" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="G67" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>88</v>
+      </c>
+      <c r="F68" t="s">
+        <v>19</v>
+      </c>
+      <c r="G68" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>89</v>
+      </c>
+      <c r="F69" t="s">
+        <v>23</v>
+      </c>
+      <c r="G69" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>90</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F70" t="s">
         <v>5</v>
       </c>
-      <c r="G68" t="s">
+      <c r="G70" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F69" t="s">
-        <v>77</v>
-      </c>
-      <c r="G69" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F70" t="s">
-        <v>34</v>
-      </c>
-      <c r="G70" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F71" t="s">
-        <v>6</v>
+        <v>77</v>
+      </c>
+      <c r="G71" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F72" t="s">
+        <v>34</v>
+      </c>
+      <c r="G72" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F73" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F74" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R73" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}"/>
-  <conditionalFormatting sqref="A2:A41">
-    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
+  <autoFilter ref="A1:R75" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}"/>
+  <conditionalFormatting sqref="A2:A43">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H65:R69 G1:R48 G50:R64 G49:H49 J49:R49 G70:R1048576 G66:G69">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Complete">
+  <conditionalFormatting sqref="H67:R71 G52:R66 G51:H51 J51:R51 G72:R1048576 G68:G71 G1:R50">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+      <formula>"Done (Needs Review)"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",G1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
       <formula>"Done (Needs Testing)"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
       <formula>"Started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
-      <formula>"Done (Needs Review)"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B20">
+  <conditionalFormatting sqref="B22">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -3706,18 +3758,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B20">
-    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",B20)))</formula>
+  <conditionalFormatting sqref="B22">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",B22)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Done (Needs Testing)"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5:R41">
+  <conditionalFormatting sqref="G7:R43">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
@@ -3727,8 +3779,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:R4">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="G2:R6">
+    <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3738,14 +3790,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A41" xr:uid="{D3DB8CA4-CF09-459F-A4BC-4F324FE8B47E}">
-      <formula1>$A$65:$A$68</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A43" xr:uid="{D3DB8CA4-CF09-459F-A4BC-4F324FE8B47E}">
+      <formula1>$A$67:$A$70</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F41" xr:uid="{8F276E49-902F-4BBD-9E0B-A51B9A15EC6B}">
-      <formula1>$F$64:$F$72</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F43" xr:uid="{8F276E49-902F-4BBD-9E0B-A51B9A15EC6B}">
+      <formula1>$F$66:$F$74</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:R41" xr:uid="{74781059-03CD-4747-BF6A-E35BF8F2BF2E}">
-      <formula1>$G$65:$G$70</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:R43" xr:uid="{74781059-03CD-4747-BF6A-E35BF8F2BF2E}">
+      <formula1>$G$67:$G$72</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3758,7 +3810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -3837,6 +3889,23 @@
         <v>117</v>
       </c>
     </row>
+    <row r="5" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>99</v>
@@ -3899,30 +3968,30 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A4">
-    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
+  <conditionalFormatting sqref="A2:A5">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E4">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+  <conditionalFormatting sqref="E2:E5">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Unfixed"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
       <formula1>$D$28:$D$35</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A5" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
       <formula1>$A$28:$A$31</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E5" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
       <formula1>$E$28:$E$30</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fixed bugs: mushie level lever, skipping hidden level objects
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D17DA8-0553-4E25-A795-74A3E26C328A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127DB6B2-E13C-474C-B570-832408B18EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="167">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -639,6 +639,9 @@
   </si>
   <si>
     <t>Each level will have it's own specific grid, so the level switcher will have to correctly load and unload each grid alongside the level.</t>
+  </si>
+  <si>
+    <t>Last Update</t>
   </si>
 </sst>
 </file>
@@ -801,7 +804,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -879,6 +882,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1324,7 +1330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R75"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -2387,7 +2393,7 @@
         <v>92</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>66</v>
@@ -3869,10 +3875,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3881,9 +3887,10 @@
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>87</v>
       </c>
@@ -3902,8 +3909,11 @@
       <c r="F1" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>88</v>
       </c>
@@ -3920,8 +3930,9 @@
       <c r="F2" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>89</v>
       </c>
@@ -3934,14 +3945,13 @@
       <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="E3" s="1"/>
       <c r="F3" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="G3" s="33"/>
+    </row>
+    <row r="4" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>99</v>
       </c>
@@ -3958,10 +3968,13 @@
         <v>19</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="G4" s="33">
+        <v>44792</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>88</v>
       </c>
@@ -3978,7 +3991,10 @@
         <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
+      </c>
+      <c r="G5" s="33">
+        <v>44792</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -4097,20 +4113,20 @@
   <sheetData>
     <row r="1" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
     </row>
     <row r="2" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -4371,20 +4387,20 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -4428,21 +4444,21 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -4479,21 +4495,21 @@
       <c r="M5" s="14"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
@@ -4564,21 +4580,21 @@
       <c r="M10" s="13"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
@@ -4632,21 +4648,21 @@
       <c r="M14" s="13"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">

</xml_diff>

<commit_message>
Implemented the grid system into each level yeeha
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D17DA8-0553-4E25-A795-74A3E26C328A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA6F6C1-7559-46E1-A383-06EF9EDCC27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="1785" yWindow="1245" windowWidth="21600" windowHeight="11235" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Gantt Chart" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Task Tracking'!$A$1:$R$76</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Task Tracking'!$A$1:$R$78</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="171">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -639,6 +639,21 @@
   </si>
   <si>
     <t>Each level will have it's own specific grid, so the level switcher will have to correctly load and unload each grid alongside the level.</t>
+  </si>
+  <si>
+    <t>Climbing string made player invulnerable to being killed by vines</t>
+  </si>
+  <si>
+    <t>After climbing, happens because puppet changes layer so can't be hit by vines</t>
+  </si>
+  <si>
+    <t>Make "Take 1" sign appear at level start, same as when you die</t>
+  </si>
+  <si>
+    <t>Make quit button return to title screen</t>
+  </si>
+  <si>
+    <t>As stated</t>
   </si>
 </sst>
 </file>
@@ -1322,10 +1337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
-  <dimension ref="A1:R75"/>
+  <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,16 +1468,18 @@
       <c r="A3" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>159</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="4">
         <v>1</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4">
+        <v>0.5</v>
+      </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>92</v>
@@ -1471,7 +1488,7 @@
         <v>92</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>66</v>
@@ -1505,7 +1522,7 @@
       <c r="A4" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>145</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1514,7 +1531,9 @@
       <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4">
+        <v>0.5</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>77</v>
       </c>
@@ -1525,7 +1544,7 @@
         <v>92</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>66</v>
@@ -2147,22 +2166,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="D16" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>92</v>
@@ -2171,7 +2190,7 @@
         <v>92</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>66</v>
@@ -2201,22 +2220,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="D17" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>92</v>
@@ -2225,7 +2244,7 @@
         <v>92</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>66</v>
@@ -2255,22 +2274,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D18" s="1">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>92</v>
@@ -2309,31 +2328,31 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="D19" s="1">
         <v>12</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>92</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>66</v>
@@ -2363,31 +2382,31 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>21</v>
+        <v>122</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="D20" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>92</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>66</v>
@@ -2421,79 +2440,79 @@
       <c r="A21" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="1"/>
+      <c r="B21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2</v>
+      </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D22" s="1">
-        <v>4</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G22" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="H22" s="23" t="s">
+      <c r="G22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>92</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>66</v>
@@ -2523,34 +2542,32 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="29" t="s">
-        <v>8</v>
+      <c r="B23" s="4" t="s">
+        <v>110</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="D23" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0.5</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E23" s="1"/>
       <c r="F23" s="5" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="G23" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="J23" s="1" t="s">
         <v>66</v>
       </c>
@@ -2579,31 +2596,33 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:18" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>152</v>
+      <c r="B24" s="29" t="s">
+        <v>8</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="5">
-        <v>2</v>
-      </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>92</v>
+      <c r="G24" s="23" t="s">
+        <v>93</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>158</v>
+        <v>95</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>66</v>
@@ -2633,12 +2652,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>29</v>
+        <v>152</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>30</v>
@@ -2657,7 +2676,7 @@
         <v>92</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>92</v>
+        <v>158</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>66</v>
@@ -2687,84 +2706,86 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="5">
+        <v>2</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C26" s="31" t="s">
+      <c r="C27" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D27" s="5">
         <v>6</v>
       </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="25" t="s">
+      <c r="E27" s="5"/>
+      <c r="F27" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I26" s="1" t="s">
+      <c r="G27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q26" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="J27" s="1" t="s">
         <v>66</v>
       </c>
@@ -2793,85 +2814,83 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="D28" s="1">
-        <v>4</v>
-      </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="D29" s="1">
         <v>4</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>92</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>66</v>
@@ -2901,20 +2920,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="D30" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>92</v>
@@ -2953,31 +2974,29 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B31" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="4"/>
+      <c r="B31" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C31" s="3"/>
       <c r="D31" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E31" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="F31" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>92</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>66</v>
@@ -3007,139 +3026,137 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="1">
+        <v>8</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D34" s="1">
         <v>3</v>
       </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="5" t="s">
+      <c r="E34" s="1"/>
+      <c r="F34" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I32" s="1" t="s">
+      <c r="G34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R32" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D33" s="1">
-        <v>2</v>
-      </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O33" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P33" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q33" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R33" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D34" s="1">
-        <v>4</v>
-      </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>66</v>
@@ -3171,18 +3188,20 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C35" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="D35" s="1">
         <v>2</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>92</v>
@@ -3191,7 +3210,7 @@
         <v>92</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>66</v>
@@ -3221,22 +3240,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>132</v>
+        <v>25</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>133</v>
+        <v>26</v>
       </c>
       <c r="D36" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>92</v>
@@ -3280,17 +3299,15 @@
         <v>90</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>134</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="C37" s="4"/>
       <c r="D37" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>92</v>
@@ -3299,7 +3316,7 @@
         <v>92</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>66</v>
@@ -3333,16 +3350,18 @@
       <c r="A38" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" s="3"/>
+      <c r="B38" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="D38" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>92</v>
@@ -3381,20 +3400,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" s="3"/>
+      <c r="B39" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="D39" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>92</v>
@@ -3438,17 +3459,15 @@
         <v>90</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>98</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C40" s="3"/>
       <c r="D40" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>92</v>
@@ -3487,18 +3506,16 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>150</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C41" s="3"/>
       <c r="D41" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1" t="s">
@@ -3511,7 +3528,7 @@
         <v>92</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>66</v>
@@ -3541,22 +3558,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E42" s="4"/>
+        <v>98</v>
+      </c>
+      <c r="D42" s="1">
+        <v>2</v>
+      </c>
+      <c r="E42" s="1"/>
       <c r="F42" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>92</v>
@@ -3595,18 +3612,18 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>1</v>
+        <v>126</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>14</v>
+        <v>150</v>
       </c>
       <c r="D43" s="1">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1" t="s">
@@ -3619,7 +3636,7 @@
         <v>92</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>66</v>
@@ -3649,153 +3666,261 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E44" s="4"/>
+      <c r="F44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R44" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R45" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D46" s="1">
         <v>3</v>
       </c>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1" t="s">
+      <c r="E46" s="1"/>
+      <c r="F46" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L44" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M44" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N44" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O44" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P44" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q44" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R44" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="50" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K50" t="s">
+      <c r="G46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q46" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R46" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K52" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="51" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K51" t="s">
+    <row r="53" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K53" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F67" t="s">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F69" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>99</v>
-      </c>
-      <c r="F68" t="s">
-        <v>7</v>
-      </c>
-      <c r="G68" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>88</v>
-      </c>
-      <c r="F69" t="s">
-        <v>19</v>
-      </c>
-      <c r="G69" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="F70" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="G70" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>88</v>
+      </c>
+      <c r="F71" t="s">
+        <v>19</v>
+      </c>
+      <c r="G71" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>89</v>
+      </c>
+      <c r="F72" t="s">
+        <v>23</v>
+      </c>
+      <c r="G72" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>90</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F73" t="s">
         <v>5</v>
       </c>
-      <c r="G71" t="s">
+      <c r="G73" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F72" t="s">
-        <v>77</v>
-      </c>
-      <c r="G72" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F73" t="s">
-        <v>34</v>
-      </c>
-      <c r="G73" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F74" t="s">
-        <v>6</v>
+        <v>77</v>
+      </c>
+      <c r="G74" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F75" t="s">
+        <v>34</v>
+      </c>
+      <c r="G75" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F77" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R76" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}"/>
-  <conditionalFormatting sqref="A2:A44">
+  <autoFilter ref="A1:R78" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}"/>
+  <conditionalFormatting sqref="A2:A46">
     <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H68:R72 G53:R67 G52:H52 J52:R52 G73:R1048576 G69:G72 G1:R51">
+  <conditionalFormatting sqref="H70:R74 G55:R69 G54:H54 J54:R54 G75:R1048576 G71:G74 G1:R53">
     <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"Done (Needs Review)"</formula>
     </cfRule>
@@ -3809,7 +3934,7 @@
       <formula>"Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B23">
+  <conditionalFormatting sqref="B24">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -3819,9 +3944,9 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B23">
+  <conditionalFormatting sqref="B24">
     <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",B23)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Complete",B24)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Done (Needs Testing)"</formula>
@@ -3840,7 +3965,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7:R44">
+  <conditionalFormatting sqref="G7:R46">
     <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
@@ -3851,14 +3976,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A44" xr:uid="{D3DB8CA4-CF09-459F-A4BC-4F324FE8B47E}">
-      <formula1>$A$68:$A$71</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A46" xr:uid="{D3DB8CA4-CF09-459F-A4BC-4F324FE8B47E}">
+      <formula1>$A$70:$A$73</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F44" xr:uid="{8F276E49-902F-4BBD-9E0B-A51B9A15EC6B}">
-      <formula1>$F$67:$F$75</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F46" xr:uid="{8F276E49-902F-4BBD-9E0B-A51B9A15EC6B}">
+      <formula1>$F$69:$F$77</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:R44" xr:uid="{74781059-03CD-4747-BF6A-E35BF8F2BF2E}">
-      <formula1>$G$68:$G$73</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:R46" xr:uid="{74781059-03CD-4747-BF6A-E35BF8F2BF2E}">
+      <formula1>$G$70:$G$75</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3871,8 +3996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3981,6 +4106,26 @@
         <v>118</v>
       </c>
     </row>
+    <row r="6" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>99</v>
@@ -4043,12 +4188,12 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A5">
+  <conditionalFormatting sqref="A2:A6">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F5">
+  <conditionalFormatting sqref="F2:F6">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
@@ -4060,13 +4205,13 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E5" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E6" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
       <formula1>$D$28:$D$35</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A5" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A6" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
       <formula1>$A$28:$A$31</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F5" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
       <formula1>$F$28:$F$30</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Found new bugs, harper help pls
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA6F6C1-7559-46E1-A383-06EF9EDCC27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB5892E-07DE-4129-A0B8-626A2911AC6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="1245" windowWidth="21600" windowHeight="11235" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="1785" yWindow="1245" windowWidth="21600" windowHeight="11235" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="173">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -654,6 +654,12 @@
   </si>
   <si>
     <t>As stated</t>
+  </si>
+  <si>
+    <t>With the grid system, players stay snapped to grid between level transitions</t>
+  </si>
+  <si>
+    <t>Players have to effectively be deleted between levels to disconnect and restart, I think the respawn function can handle this easily, just needs to be activated in the right place</t>
   </si>
 </sst>
 </file>
@@ -1339,7 +1345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -3996,8 +4002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4126,6 +4132,26 @@
         <v>119</v>
       </c>
     </row>
+    <row r="7" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>99</v>
@@ -4188,12 +4214,12 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A6">
+  <conditionalFormatting sqref="A2:A7">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F6">
+  <conditionalFormatting sqref="F2:F7">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
@@ -4205,13 +4231,13 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E6" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E7" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
       <formula1>$D$28:$D$35</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A6" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A7" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
       <formula1>$A$28:$A$31</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F7" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
       <formula1>$F$28:$F$30</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
started on intro cinematic
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5511BD5B-09D1-4995-9193-CEFF3D2A6977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F8F355-1FDD-4D7D-BCF0-0D87CA17D241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -1354,8 +1354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2263,7 +2263,7 @@
         <v>93</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>158</v>
+        <v>95</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>66</v>
@@ -2317,7 +2317,7 @@
         <v>92</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>66</v>
@@ -4012,7 +4012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
implemented cutscene support and Intro cutscene
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F8F355-1FDD-4D7D-BCF0-0D87CA17D241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D5A082-53CE-4480-8FFF-6D3A84034F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="7215" yWindow="4605" windowWidth="24525" windowHeight="15495" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -1354,7 +1354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
@@ -2317,7 +2317,7 @@
         <v>92</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>66</v>
@@ -4012,7 +4012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Minor adjustments to line-swapping and minor changes
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Tim\Desktop\Git\strung-along6\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D5A082-53CE-4480-8FFF-6D3A84034F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E31810A-2363-4700-9872-96375465AEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7215" yWindow="4605" windowWidth="24525" windowHeight="15495" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="178">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -669,6 +669,12 @@
   </si>
   <si>
     <t>Finalized new levers, lots of refactoring and tidying up the workspace. Started on puppet ragdoll and begun integration of new grid system.</t>
+  </si>
+  <si>
+    <t>Small jump when switching between some lines</t>
+  </si>
+  <si>
+    <t>This only happens when moving in a negitive direction, either on X or Y, as the player jumps to a perpendicual line before continuing to travel along the one they are supposed to</t>
   </si>
 </sst>
 </file>
@@ -831,21 +837,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -894,7 +895,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -902,12 +903,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1354,7 +1349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
@@ -1380,10 +1375,10 @@
       <c r="C1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="5" t="s">
         <v>97</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -1413,7 +1408,7 @@
       <c r="N1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="O1" s="25" t="s">
         <v>47</v>
       </c>
       <c r="P1" s="2" t="s">
@@ -1436,10 +1431,10 @@
       <c r="C2" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>8</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
@@ -1484,14 +1479,14 @@
       <c r="A3" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>159</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>1</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>0.5</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1538,16 +1533,16 @@
       <c r="A4" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>145</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>1</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>0.5</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -1598,10 +1593,10 @@
         <v>160</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>1</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1652,10 +1647,10 @@
       <c r="C6" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>10</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="1" t="s">
         <v>70</v>
       </c>
@@ -1706,10 +1701,10 @@
       <c r="C7" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>4</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="1" t="s">
         <v>70</v>
       </c>
@@ -1760,10 +1755,10 @@
       <c r="C8" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>4</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="1" t="s">
         <v>70</v>
       </c>
@@ -1814,10 +1809,10 @@
       <c r="C9" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>4</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="1" t="s">
         <v>70</v>
       </c>
@@ -1868,10 +1863,10 @@
       <c r="C10" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>4</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="3"/>
       <c r="F10" s="1" t="s">
         <v>70</v>
       </c>
@@ -1922,10 +1917,10 @@
       <c r="C11" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>4</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="1" t="s">
         <v>70</v>
       </c>
@@ -1976,10 +1971,10 @@
       <c r="C12" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>4</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="3"/>
       <c r="F12" s="1" t="s">
         <v>70</v>
       </c>
@@ -2030,10 +2025,10 @@
       <c r="C13" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>4</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="3"/>
       <c r="F13" s="1" t="s">
         <v>70</v>
       </c>
@@ -2084,8 +2079,8 @@
       <c r="C14" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
       <c r="F14" s="1" t="s">
         <v>23</v>
       </c>
@@ -2126,23 +2121,23 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:18" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="1">
         <v>5</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="1">
         <v>6.5</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="24" t="s">
         <v>7</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -2183,10 +2178,10 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>169</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -2237,10 +2232,10 @@
       </c>
     </row>
     <row r="17" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>164</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -2291,10 +2286,10 @@
       </c>
     </row>
     <row r="18" spans="1:18" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>148</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -2345,10 +2340,10 @@
       </c>
     </row>
     <row r="19" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -2399,10 +2394,10 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>122</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -2456,10 +2451,10 @@
       <c r="A21" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="1">
@@ -2559,26 +2554,26 @@
       </c>
     </row>
     <row r="23" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>111</v>
       </c>
       <c r="D23" s="1">
         <v>4</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G23" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="H23" s="23" t="s">
+      <c r="G23" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="H23" s="20" t="s">
         <v>92</v>
       </c>
       <c r="I23" s="1" t="s">
@@ -2612,14 +2607,14 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D24" s="1">
@@ -2628,10 +2623,10 @@
       <c r="E24" s="1">
         <v>0.5</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="23" t="s">
+      <c r="G24" s="20" t="s">
         <v>93</v>
       </c>
       <c r="H24" s="1" t="s">
@@ -2668,20 +2663,20 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:18" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="1">
         <v>2</v>
       </c>
-      <c r="E25" s="5"/>
+      <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
         <v>7</v>
       </c>
@@ -2722,20 +2717,20 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="1">
         <v>2</v>
       </c>
-      <c r="E26" s="5"/>
+      <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
         <v>7</v>
       </c>
@@ -2777,20 +2772,20 @@
       </c>
     </row>
     <row r="27" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C27" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="1">
         <v>6</v>
       </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="25" t="s">
+      <c r="E27" s="1"/>
+      <c r="F27" s="22" t="s">
         <v>34</v>
       </c>
       <c r="G27" s="1" t="s">
@@ -2837,12 +2832,12 @@
       <c r="B28" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="21" t="s">
         <v>16</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="25" t="s">
+      <c r="F28" s="22" t="s">
         <v>23</v>
       </c>
       <c r="G28" s="1" t="s">
@@ -2937,10 +2932,10 @@
       </c>
     </row>
     <row r="30" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -2991,10 +2986,10 @@
       </c>
     </row>
     <row r="31" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>168</v>
       </c>
       <c r="C31" s="3"/>
@@ -3043,10 +3038,10 @@
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C32" s="3"/>
@@ -3095,20 +3090,20 @@
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="4"/>
+      <c r="C33" s="3"/>
       <c r="D33" s="1">
         <v>0.5</v>
       </c>
       <c r="E33" s="1">
         <v>0.5</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G33" s="1" t="s">
@@ -3149,20 +3144,20 @@
       </c>
     </row>
     <row r="34" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>154</v>
       </c>
       <c r="D34" s="1">
         <v>3</v>
       </c>
       <c r="E34" s="1"/>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G34" s="1" t="s">
@@ -3206,10 +3201,10 @@
       <c r="A35" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D35" s="1">
@@ -3260,10 +3255,10 @@
       <c r="A36" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D36" s="1">
@@ -3314,10 +3309,10 @@
       <c r="A37" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C37" s="4"/>
+      <c r="C37" s="3"/>
       <c r="D37" s="1">
         <v>2</v>
       </c>
@@ -3366,10 +3361,10 @@
       <c r="A38" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>133</v>
       </c>
       <c r="D38" s="1">
@@ -3420,10 +3415,10 @@
       <c r="A39" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="3" t="s">
         <v>134</v>
       </c>
       <c r="D39" s="1">
@@ -3692,10 +3687,10 @@
       <c r="C44" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D44" s="3">
         <v>0.5</v>
       </c>
-      <c r="E44" s="4"/>
+      <c r="E44" s="3"/>
       <c r="F44" s="1" t="s">
         <v>5</v>
       </c>
@@ -4012,8 +4007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4031,7 +4026,7 @@
       <c r="B1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="5" t="s">
         <v>113</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -4058,7 +4053,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>117</v>
       </c>
     </row>
@@ -4076,7 +4071,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>117</v>
       </c>
     </row>
@@ -4096,7 +4091,7 @@
       <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>119</v>
       </c>
     </row>
@@ -4116,7 +4111,7 @@
       <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>119</v>
       </c>
     </row>
@@ -4136,7 +4131,7 @@
       <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>119</v>
       </c>
     </row>
@@ -4156,7 +4151,7 @@
       <c r="E7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>119</v>
       </c>
     </row>
@@ -4176,8 +4171,26 @@
       <c r="E8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -4242,12 +4255,12 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A8">
+  <conditionalFormatting sqref="A2:A9">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F8">
+  <conditionalFormatting sqref="F2:F9">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
@@ -4259,13 +4272,13 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E8" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E9" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
       <formula1>$D$28:$D$35</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A8" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A9" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
       <formula1>$A$28:$A$31</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F8" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F9" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
       <formula1>$F$28:$F$30</formula1>
     </dataValidation>
   </dataValidations>
@@ -4283,273 +4296,273 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="16" customWidth="1"/>
-    <col min="4" max="5" width="17.85546875" style="16" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" style="17" customWidth="1"/>
-    <col min="7" max="11" width="17.85546875" style="16" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" style="16" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" style="16" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="16"/>
+    <col min="1" max="1" width="24.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="13" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="14" customWidth="1"/>
+    <col min="7" max="11" width="17.85546875" style="13" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="13" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="13" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9"/>
-      <c r="B1" s="33" t="s">
+    <row r="1" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6"/>
+      <c r="B1" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-    </row>
-    <row r="2" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+    </row>
+    <row r="2" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
     </row>
     <row r="4" spans="1:13" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
     </row>
     <row r="5" spans="1:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
     </row>
     <row r="6" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
     </row>
     <row r="7" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
     </row>
     <row r="8" spans="1:13" ht="180" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
     </row>
     <row r="9" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
     </row>
     <row r="10" spans="1:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
     </row>
     <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="18" t="s">
+      <c r="B11" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4571,317 +4584,317 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="9"/>
-      <c r="B1" s="33" t="s">
+      <c r="A1" s="6"/>
+      <c r="B1" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
fix pesky respawn bug
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DF4961-67BD-440D-99C6-0344CF9044E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778236EE-2BBA-4732-A202-0312BFD1719F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-21255" yWindow="-5910" windowWidth="20775" windowHeight="18075" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -1445,23 +1445,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R84"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.88671875" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" customWidth="1"/>
-    <col min="11" max="18" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="18" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>87</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>99</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>99</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>99</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>99</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>99</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>99</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>99</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>99</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>99</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>99</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>99</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>99</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>99</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>99</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>99</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>88</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>88</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>88</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>88</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>88</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>88</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>88</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>88</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>88</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>88</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>88</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>88</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>88</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>88</v>
       </c>
@@ -3091,7 +3091,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>88</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>89</v>
       </c>
@@ -3199,7 +3199,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>89</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>89</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>89</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>89</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>89</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>89</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>89</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>89</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>89</v>
       </c>
@@ -3679,7 +3679,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>89</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>89</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>90</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>90</v>
       </c>
@@ -3893,7 +3893,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>90</v>
       </c>
@@ -3947,7 +3947,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>90</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>90</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>90</v>
       </c>
@@ -4105,7 +4105,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>90</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>90</v>
       </c>
@@ -4213,7 +4213,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>90</v>
       </c>
@@ -4267,7 +4267,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>90</v>
       </c>
@@ -4321,22 +4321,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="K59" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="K60" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F76" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>99</v>
       </c>
@@ -4347,7 +4347,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>88</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>89</v>
       </c>
@@ -4369,7 +4369,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>90</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="81" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F81" t="s">
         <v>77</v>
       </c>
@@ -4388,7 +4388,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="82" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F82" t="s">
         <v>34</v>
       </c>
@@ -4396,12 +4396,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="83" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F83" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F84" t="s">
         <v>70</v>
       </c>
@@ -4490,18 +4490,18 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="48.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="48.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>87</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>99</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
@@ -4559,7 +4559,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>89</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>89</v>
       </c>
@@ -4597,7 +4597,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>89</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>88</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>99</v>
       </c>
@@ -4657,7 +4657,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>88</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>88</v>
       </c>
@@ -4697,7 +4697,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>99</v>
       </c>
@@ -4717,7 +4717,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>99</v>
       </c>
@@ -4737,7 +4737,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>99</v>
       </c>
@@ -4748,7 +4748,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -4759,7 +4759,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -4770,7 +4770,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -4778,22 +4778,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>70</v>
       </c>
@@ -4834,24 +4834,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB7A6BC1-ED0D-41E7-903B-B5F7393F73BD}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="13" customWidth="1"/>
-    <col min="4" max="5" width="17.88671875" style="13" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="14" customWidth="1"/>
-    <col min="7" max="11" width="17.88671875" style="13" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" style="13" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" style="13" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="13"/>
+    <col min="1" max="1" width="24.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="13" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="14" customWidth="1"/>
+    <col min="7" max="11" width="17.85546875" style="13" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="13" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="13" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="28" t="s">
         <v>37</v>
@@ -4868,7 +4868,7 @@
       <c r="L1" s="28"/>
       <c r="M1" s="28"/>
     </row>
-    <row r="2" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>86</v>
       </c>
@@ -4909,7 +4909,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>23</v>
       </c>
@@ -4934,7 +4934,7 @@
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
     </row>
-    <row r="4" spans="1:13" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>19</v>
       </c>
@@ -4959,7 +4959,7 @@
       <c r="L4" s="15"/>
       <c r="M4" s="15"/>
     </row>
-    <row r="5" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>5</v>
       </c>
@@ -4984,7 +4984,7 @@
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
     </row>
-    <row r="6" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>34</v>
       </c>
@@ -5009,7 +5009,7 @@
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
     </row>
-    <row r="7" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>77</v>
       </c>
@@ -5034,7 +5034,7 @@
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
     </row>
-    <row r="8" spans="1:13" ht="144" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>6</v>
       </c>
@@ -5059,7 +5059,7 @@
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
     </row>
-    <row r="9" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>7</v>
       </c>
@@ -5084,7 +5084,7 @@
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
     </row>
-    <row r="10" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>70</v>
       </c>
@@ -5109,7 +5109,7 @@
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
     </row>
-    <row r="11" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>67</v>
       </c>
@@ -5151,9 +5151,9 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="28" t="s">
         <v>37</v>
@@ -5170,7 +5170,7 @@
       <c r="L1" s="28"/>
       <c r="M1" s="28"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>38</v>
       </c>
@@ -5211,7 +5211,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>51</v>
       </c>
@@ -5228,7 +5228,7 @@
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>52</v>
       </c>
@@ -5245,7 +5245,7 @@
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>53</v>
       </c>
@@ -5262,7 +5262,7 @@
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>54</v>
       </c>
@@ -5279,7 +5279,7 @@
       <c r="L6" s="29"/>
       <c r="M6" s="29"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>55</v>
       </c>
@@ -5296,7 +5296,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>56</v>
       </c>
@@ -5313,7 +5313,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>57</v>
       </c>
@@ -5330,7 +5330,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>58</v>
       </c>
@@ -5347,7 +5347,7 @@
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>59</v>
       </c>
@@ -5364,7 +5364,7 @@
       <c r="L11" s="29"/>
       <c r="M11" s="29"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>60</v>
       </c>
@@ -5381,7 +5381,7 @@
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>61</v>
       </c>
@@ -5398,7 +5398,7 @@
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>62</v>
       </c>
@@ -5415,7 +5415,7 @@
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>63</v>
       </c>
@@ -5432,7 +5432,7 @@
       <c r="L15" s="29"/>
       <c r="M15" s="29"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>64</v>
       </c>
@@ -5449,7 +5449,7 @@
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
shrink water hazard killbox slightly
the flowy cloth looks great dylan :D
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778236EE-2BBA-4732-A202-0312BFD1719F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC4F058-932E-43E0-AA2E-A32BA585B4CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21255" yWindow="-5910" windowWidth="20775" windowHeight="18075" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
@@ -4490,7 +4490,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4538,7 +4538,7 @@
         <v>19</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Quit button now returns to title screen
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC4F058-932E-43E0-AA2E-A32BA585B4CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD317CE-B7A3-47B3-BF96-FA237C05545F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21255" yWindow="-5910" windowWidth="20775" windowHeight="18075" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="211">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -771,13 +771,16 @@
   </si>
   <si>
     <t>Continue working on the soundtrack and score</t>
+  </si>
+  <si>
+    <t>Finished Item</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -815,6 +818,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -933,14 +943,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -991,16 +998,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1008,6 +1007,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1445,8 +1458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,10 +1484,10 @@
       <c r="C1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>97</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -1504,7 +1517,7 @@
       <c r="N1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="O1" s="22" t="s">
         <v>47</v>
       </c>
       <c r="P1" s="2" t="s">
@@ -1517,221 +1530,221 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:18" s="27" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="26">
         <v>8</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="26"/>
+      <c r="F2" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="J2" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="O2" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="P2" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q2" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="R2" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="27" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26">
         <v>1</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="26">
         <v>0.5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="G3" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="K3" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="L3" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="M3" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="N3" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="O3" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="P3" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q3" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="R3" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" s="27" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="26">
         <v>1</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="26">
         <v>0.5</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="G4" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="K4" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="L4" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="M4" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="N4" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="O4" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="P4" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q4" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="R4" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" s="27" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3">
+      <c r="C5" s="26"/>
+      <c r="D5" s="26">
         <v>1</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="26">
         <v>1</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="G5" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R5" s="1" t="s">
+      <c r="K5" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="L5" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="M5" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="N5" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="O5" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="P5" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q5" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="R5" s="25" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1791,57 +1804,57 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:18" s="27" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="26">
         <v>10</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="1" t="s">
+      <c r="E7" s="26"/>
+      <c r="F7" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="G7" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R7" s="1" t="s">
+      <c r="K7" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="N7" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="O7" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="P7" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q7" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="R7" s="25" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2279,59 +2292,59 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:18" s="27" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="25">
         <v>5</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="25">
         <v>6.5</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H16" s="1" t="s">
+      <c r="G16" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H16" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J16" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R16" s="1" t="s">
+      <c r="K16" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="L16" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="M16" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="N16" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="O16" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="P16" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q16" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="R16" s="25" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2497,165 +2510,165 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:18" s="27" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="25">
         <v>1</v>
       </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J20" s="1" t="s">
+      <c r="E20" s="25"/>
+      <c r="F20" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="J20" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="K20" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="L20" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="M20" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="N20" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="O20" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="P20" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q20" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="R20" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" s="27" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="D21" s="25">
+        <v>4</v>
+      </c>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I21" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="K20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="J21" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="K21" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="L21" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="M21" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="N21" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="O21" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="P21" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q21" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="R21" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" s="27" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="D21" s="1">
-        <v>4</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1" t="s">
+      <c r="B22" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="D22" s="25">
+        <v>3</v>
+      </c>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I21" s="1" t="s">
+      <c r="G22" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I22" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="J22" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="K21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="D22" s="1">
-        <v>3</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R22" s="1" t="s">
+      <c r="K22" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="L22" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="M22" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="N22" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="O22" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="P22" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q22" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="R22" s="25" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2794,7 +2807,7 @@
         <v>92</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>66</v>
@@ -2890,10 +2903,10 @@
       <c r="F27" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G27" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="H27" s="20" t="s">
+      <c r="G27" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="H27" s="19" t="s">
         <v>92</v>
       </c>
       <c r="I27" s="1" t="s">
@@ -2927,59 +2940,59 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:18" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="25">
         <v>0.5</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="25">
         <v>0.5</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G28" s="20" t="s">
+      <c r="G28" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H28" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="I28" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R28" s="1" t="s">
+      <c r="J28" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="K28" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="L28" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="M28" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="N28" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="O28" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="P28" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q28" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="R28" s="25" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3152,14 +3165,14 @@
       <c r="B32" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="20" t="s">
         <v>188</v>
       </c>
       <c r="D32" s="1">
         <v>1</v>
       </c>
       <c r="E32" s="1"/>
-      <c r="F32" s="22" t="s">
+      <c r="F32" s="21" t="s">
         <v>77</v>
       </c>
       <c r="G32" s="1" t="s">
@@ -3206,14 +3219,14 @@
       <c r="B33" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="C33" s="20" t="s">
         <v>139</v>
       </c>
       <c r="D33" s="1">
         <v>6</v>
       </c>
       <c r="E33" s="1"/>
-      <c r="F33" s="22" t="s">
+      <c r="F33" s="21" t="s">
         <v>34</v>
       </c>
       <c r="G33" s="1" t="s">
@@ -3260,12 +3273,12 @@
       <c r="B34" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="22" t="s">
+      <c r="F34" s="21" t="s">
         <v>23</v>
       </c>
       <c r="G34" s="1" t="s">
@@ -3571,57 +3584,57 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:18" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="1">
+      <c r="C40" s="26"/>
+      <c r="D40" s="25">
         <v>0.5</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40" s="25">
         <v>0.5</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F40" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H40" s="1" t="s">
+      <c r="G40" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H40" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="I40" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="J40" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N40" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O40" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q40" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R40" s="1" t="s">
+      <c r="J40" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="K40" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="L40" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="M40" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="N40" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="O40" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="P40" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q40" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="R40" s="25" t="s">
         <v>66</v>
       </c>
     </row>
@@ -4334,6 +4347,9 @@
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F76" t="s">
         <v>67</v>
+      </c>
+      <c r="G76" s="27" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -4508,7 +4524,7 @@
       <c r="B1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>113</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -4835,304 +4851,304 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="13" customWidth="1"/>
-    <col min="4" max="5" width="17.85546875" style="13" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" style="14" customWidth="1"/>
-    <col min="7" max="11" width="17.85546875" style="13" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" style="13" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" style="13" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="13"/>
+    <col min="1" max="1" width="24.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="12" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="13" customWidth="1"/>
+    <col min="7" max="11" width="17.85546875" style="12" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="12" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="12" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="28" t="s">
+    <row r="1" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-    </row>
-    <row r="2" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+    </row>
+    <row r="2" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
     </row>
     <row r="4" spans="1:13" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
     </row>
     <row r="5" spans="1:13" ht="165" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
     </row>
     <row r="6" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
     </row>
     <row r="7" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
     </row>
     <row r="8" spans="1:13" ht="180" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
     </row>
     <row r="9" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
     </row>
     <row r="10" spans="1:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
     </row>
     <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="15" t="s">
+      <c r="B11" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
+      <c r="E11" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5154,317 +5170,317 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="28" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Added new pages to production doc
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB805DC7-F940-487A-82B4-115D9873F109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8459F123-6DC3-4C9B-A6C2-9FD8F0F202EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
     <sheet name="Bug Tracking" sheetId="2" r:id="rId2"/>
     <sheet name="Weekly Meeting Notes" sheetId="5" r:id="rId3"/>
-    <sheet name="Gantt Chart" sheetId="4" r:id="rId4"/>
+    <sheet name="Usability Testing" sheetId="6" r:id="rId4"/>
+    <sheet name="Performance Testing" sheetId="7" r:id="rId5"/>
+    <sheet name="Gantt Chart" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Task Tracking'!$A$1:$R$85</definedName>
@@ -144,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="215">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -777,6 +779,18 @@
   </si>
   <si>
     <t>Tim knows what to do</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing plan, plan what needs to be tested, iterate, </t>
+  </si>
+  <si>
+    <t>benchmark things like frames per second, structure a playtesting process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How many deaths per level, time taken, data driven decisions, what was favourite levels? </t>
+  </si>
+  <si>
+    <t>Least favourite levels, etc.</t>
   </si>
 </sst>
 </file>
@@ -1018,12 +1032,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1031,25 +1039,24 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="12">
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAF8A4"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1074,49 +1081,12 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAF8A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4FBA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAF8A4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1159,6 +1129,16 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEAF8A4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1174,46 +1154,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC4FBA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1545,8 +1485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S49" sqref="S49"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1897,23 +1837,23 @@
       <c r="A7" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="32">
         <v>10</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="35" t="s">
+      <c r="E7" s="32"/>
+      <c r="F7" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="H7" s="35" t="s">
+      <c r="G7" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" s="33" t="s">
         <v>92</v>
       </c>
       <c r="I7" s="23" t="s">
@@ -4514,21 +4454,21 @@
   </sheetData>
   <autoFilter ref="A1:R85" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}"/>
   <conditionalFormatting sqref="A2:A49 A52:A53">
-    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H77:R81 G62:R76 G61:H61 J61:R61 G82:R1048576 G78:G81 G1:R49 G52:R60 I50:J51">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"Done (Needs Review)"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",G1)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
       <formula>"Done (Needs Testing)"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
       <formula>"Started"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4543,13 +4483,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B28)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Done (Needs Testing)"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Started"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4923,18 +4863,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A12:A13 A2:A9">
-    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F13">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Unfixed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4957,7 +4897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB7A6BC1-ED0D-41E7-903B-B5F7393F73BD}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -4976,20 +4916,20 @@
   <sheetData>
     <row r="1" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
     </row>
     <row r="2" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -5267,6 +5207,55 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15B1403-352E-4AED-9F5F-27791D86941F}">
+  <dimension ref="C5:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="9" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF3DEBB8-1969-4CBE-B855-486715171A1F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05F207C-B898-4037-B135-7745119EBD21}">
   <dimension ref="A1:M17"/>
   <sheetViews>
@@ -5281,20 +5270,20 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -5338,21 +5327,21 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -5389,21 +5378,21 @@
       <c r="M5" s="10"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -5474,21 +5463,21 @@
       <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
@@ -5542,21 +5531,21 @@
       <c r="M14" s="9"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">

</xml_diff>

<commit_message>
update prod doc so i dont forget what im doing
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8459F123-6DC3-4C9B-A6C2-9FD8F0F202EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38588B8-1A25-4BFA-B431-8D243A9F1ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -31,12 +31,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -146,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="215">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -1485,8 +1482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R84"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3438,7 +3435,7 @@
         <v>92</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>66</v>
@@ -4535,7 +4532,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4579,9 +4576,11 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F2" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -5210,8 +5209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15B1403-352E-4AED-9F5F-27791D86941F}">
   <dimension ref="C5:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
better stage colliders, new light on intro cinematic
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38588B8-1A25-4BFA-B431-8D243A9F1ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1950C5F-E6F6-491B-95B3-E83F6D1D0C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-21195" yWindow="8190" windowWidth="20775" windowHeight="18075" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -1482,8 +1482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2829,7 +2829,9 @@
       <c r="D25" s="1">
         <v>2</v>
       </c>
-      <c r="E25" s="1"/>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
       <c r="F25" s="1" t="s">
         <v>19</v>
       </c>
@@ -2846,7 +2848,7 @@
         <v>93</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>66</v>
@@ -3421,7 +3423,9 @@
       <c r="D36" s="1">
         <v>2</v>
       </c>
-      <c r="E36" s="1"/>
+      <c r="E36" s="1">
+        <v>1</v>
+      </c>
       <c r="F36" s="1" t="s">
         <v>19</v>
       </c>
@@ -3438,7 +3442,7 @@
         <v>93</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>66</v>
+        <v>156</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>66</v>
@@ -3492,7 +3496,7 @@
         <v>92</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>66</v>
@@ -3544,7 +3548,7 @@
         <v>92</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>66</v>
@@ -3704,7 +3708,7 @@
         <v>93</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>66</v>
@@ -3972,7 +3976,7 @@
         <v>92</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>66</v>
@@ -4532,7 +4536,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4563,24 +4567,24 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" s="25" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>118</v>
+      <c r="F2" s="24" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add light to intro cinematic
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38588B8-1A25-4BFA-B431-8D243A9F1ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1950C5F-E6F6-491B-95B3-E83F6D1D0C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-21195" yWindow="8190" windowWidth="20775" windowHeight="18075" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -1482,8 +1482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2829,7 +2829,9 @@
       <c r="D25" s="1">
         <v>2</v>
       </c>
-      <c r="E25" s="1"/>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
       <c r="F25" s="1" t="s">
         <v>19</v>
       </c>
@@ -2846,7 +2848,7 @@
         <v>93</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>66</v>
@@ -3421,7 +3423,9 @@
       <c r="D36" s="1">
         <v>2</v>
       </c>
-      <c r="E36" s="1"/>
+      <c r="E36" s="1">
+        <v>1</v>
+      </c>
       <c r="F36" s="1" t="s">
         <v>19</v>
       </c>
@@ -3438,7 +3442,7 @@
         <v>93</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>66</v>
+        <v>156</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>66</v>
@@ -3492,7 +3496,7 @@
         <v>92</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>66</v>
@@ -3544,7 +3548,7 @@
         <v>92</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>66</v>
@@ -3704,7 +3708,7 @@
         <v>93</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>66</v>
@@ -3972,7 +3976,7 @@
         <v>92</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>66</v>
@@ -4532,7 +4536,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4563,24 +4567,24 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" s="25" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>118</v>
+      <c r="F2" s="24" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Outline Shader Package added and Implemented
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dennys\Documents\Strung Along\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC61F1EC-D914-41E4-9C8F-03A367030ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEAA6CC-066B-43F1-A99C-2E2606A4A980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
@@ -3916,7 +3916,7 @@
         <v>92</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>93</v>
+        <v>156</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
add functionality to move props from side and bottom
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dennys\Documents\Strung Along\strung-along\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEAA6CC-066B-43F1-A99C-2E2606A4A980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64B41C3-6F0C-4670-B0F2-F9B099E32AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="217">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -788,6 +788,12 @@
   </si>
   <si>
     <t>Least favourite levels, etc.</t>
+  </si>
+  <si>
+    <t>Add multiple directions stage props can move</t>
+  </si>
+  <si>
+    <t>All props move in from the top, add the option to move in from side and bottom</t>
   </si>
 </sst>
 </file>
@@ -1480,10 +1486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
-  <dimension ref="A1:R84"/>
+  <dimension ref="A1:R85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1495,7 +1501,10 @@
     <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" customWidth="1"/>
-    <col min="11" max="18" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" customWidth="1"/>
+    <col min="14" max="18" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -3255,17 +3264,19 @@
         <v>89</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>138</v>
+        <v>215</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>139</v>
+        <v>216</v>
       </c>
       <c r="D33" s="1">
-        <v>6</v>
-      </c>
-      <c r="E33" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
       <c r="F33" s="21" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>92</v>
@@ -3274,13 +3285,13 @@
         <v>92</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>66</v>
@@ -3304,20 +3315,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>4</v>
+        <v>138</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" s="1"/>
+        <v>139</v>
+      </c>
+      <c r="D34" s="1">
+        <v>6</v>
+      </c>
       <c r="E34" s="1"/>
       <c r="F34" s="21" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>92</v>
@@ -3326,10 +3339,10 @@
         <v>92</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>66</v>
@@ -3356,34 +3369,32 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D35" s="1">
         <v>4</v>
       </c>
+      <c r="C35" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="1" t="s">
-        <v>7</v>
+      <c r="F35" s="21" t="s">
+        <v>23</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>92</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>66</v>
@@ -3415,34 +3426,32 @@
         <v>89</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>177</v>
+        <v>3</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>178</v>
+        <v>109</v>
       </c>
       <c r="D36" s="1">
-        <v>2</v>
-      </c>
-      <c r="E36" s="1">
-        <v>1</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>92</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>93</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>156</v>
+        <v>66</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>66</v>
@@ -3466,20 +3475,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>9</v>
+        <v>177</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>27</v>
+        <v>178</v>
       </c>
       <c r="D37" s="1">
-        <v>4</v>
-      </c>
-      <c r="E37" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1</v>
+      </c>
       <c r="F37" s="1" t="s">
         <v>19</v>
       </c>
@@ -3493,10 +3504,10 @@
         <v>92</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>66</v>
@@ -3520,14 +3531,16 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C38" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="D38" s="1">
         <v>4</v>
       </c>
@@ -3572,143 +3585,141 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>10</v>
+        <v>166</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="1">
+        <v>8</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J39" s="1" t="s">
+      <c r="G40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J40" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R39" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="23" t="s">
+      <c r="K40" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L40" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="M40" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="N40" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="O40" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="P40" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q40" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="R40" s="23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="B40" s="28" t="s">
+      <c r="B41" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="24"/>
-      <c r="D40" s="23">
+      <c r="C41" s="24"/>
+      <c r="D41" s="23">
         <v>0.5</v>
       </c>
-      <c r="E40" s="23">
+      <c r="E41" s="23">
         <v>0.5</v>
       </c>
-      <c r="F40" s="23" t="s">
+      <c r="F41" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="G40" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="H40" s="23" t="s">
+      <c r="G41" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H41" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="I40" s="23" t="s">
+      <c r="I41" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="J40" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="K40" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="L40" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="M40" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="N40" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="O40" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="P40" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q40" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="R40" s="23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D41" s="1">
-        <v>3</v>
-      </c>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>93</v>
+      <c r="J41" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="K41" s="23" t="s">
+        <v>66</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>66</v>
@@ -3732,22 +3743,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>22</v>
+        <v>153</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>24</v>
+        <v>154</v>
       </c>
       <c r="D42" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>92</v>
@@ -3756,13 +3767,13 @@
         <v>92</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>66</v>
@@ -3786,22 +3797,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D43" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>92</v>
@@ -3813,7 +3824,7 @@
         <v>92</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>66</v>
@@ -3840,20 +3851,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C44" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="D44" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>92</v>
@@ -3862,7 +3875,7 @@
         <v>92</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>156</v>
+        <v>92</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>66</v>
@@ -3892,16 +3905,14 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>133</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="C45" s="3"/>
       <c r="D45" s="1">
         <v>2</v>
       </c>
@@ -3946,22 +3957,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D46" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>92</v>
@@ -3970,13 +3981,13 @@
         <v>92</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>66</v>
@@ -4000,20 +4011,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C47" s="3"/>
+        <v>135</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>134</v>
+      </c>
       <c r="D47" s="1">
         <v>1</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>92</v>
@@ -4025,10 +4038,10 @@
         <v>92</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="L47" s="1" t="s">
         <v>66</v>
@@ -4057,15 +4070,15 @@
         <v>90</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>92</v>
@@ -4109,85 +4122,83 @@
         <v>90</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>98</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C49" s="3"/>
       <c r="D49" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R49" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D50" s="1">
+        <v>2</v>
+      </c>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G49" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I49" s="1" t="s">
+      <c r="G50" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I50" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J49" s="1" t="s">
+      <c r="J50" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K49" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L49" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M49" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N49" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O49" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P49" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q49" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R49" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="B50" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="C50" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="D50" s="24">
-        <v>3</v>
-      </c>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="G50" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="H50" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K50" s="24" t="s">
+      <c r="K50" s="1" t="s">
         <v>66</v>
       </c>
       <c r="L50" s="24" t="s">
@@ -4212,18 +4223,18 @@
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="24" t="s">
         <v>90</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>13</v>
+        <v>150</v>
       </c>
       <c r="D51" s="24">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="E51" s="24"/>
       <c r="F51" s="24" t="s">
@@ -4266,36 +4277,36 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D52" s="1">
+      <c r="B52" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="24">
         <v>0.5</v>
       </c>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1" t="s">
+      <c r="E52" s="24"/>
+      <c r="F52" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G52" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H52" s="1" t="s">
+      <c r="G52" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="H52" s="24" t="s">
         <v>92</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="K52" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K52" s="24" t="s">
         <v>66</v>
       </c>
       <c r="L52" s="1" t="s">
@@ -4325,141 +4336,174 @@
         <v>90</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D53" s="1">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N53" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O53" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P53" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q53" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R53" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="1">
+        <v>3</v>
+      </c>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G53" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J53" s="1" t="s">
+      <c r="G54" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J54" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K53" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L53" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M53" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N53" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O53" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P53" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q53" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R53" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F76" t="s">
+      <c r="K54" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F77" t="s">
         <v>67</v>
       </c>
-      <c r="G76" s="25" t="s">
+      <c r="G77" s="25" t="s">
         <v>207</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>99</v>
-      </c>
-      <c r="F77" t="s">
-        <v>7</v>
-      </c>
-      <c r="G77" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="F78" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="G78" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F79" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G79" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>89</v>
+      </c>
+      <c r="F80" t="s">
+        <v>23</v>
+      </c>
+      <c r="G80" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>90</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F81" t="s">
         <v>5</v>
       </c>
-      <c r="G80" t="s">
+      <c r="G81" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="81" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F81" t="s">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F82" t="s">
         <v>77</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G82" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="82" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F82" t="s">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F83" t="s">
         <v>34</v>
       </c>
-      <c r="G82" t="s">
+      <c r="G83" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="83" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F83" t="s">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F84" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F84" t="s">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F85" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:R85" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}"/>
-  <conditionalFormatting sqref="A2:A49 A52:A53">
+  <conditionalFormatting sqref="A53:A54 A2:A50">
     <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H77:R81 G62:R76 G61:H61 J61:R61 G82:R1048576 G78:G81 G1:R49 G52:R60 I50:J51">
+  <conditionalFormatting sqref="G62:H62 G79:G82 I51:J52 H78:K82 G63:K77 J62:K62 G83:K1048576 G1:R31 L32:R49 L52:R1048576 G53:K61 G32:K50">
     <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"Done (Needs Review)"</formula>
     </cfRule>
@@ -4504,7 +4548,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8:R49 G52:R53 I50:J51">
+  <conditionalFormatting sqref="I51:J52 G8:R31 L32:R49 L52:R53 G53:K54 G32:K50">
     <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
@@ -4515,14 +4559,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A53" xr:uid="{D3DB8CA4-CF09-459F-A4BC-4F324FE8B47E}">
-      <formula1>$A$77:$A$80</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A54" xr:uid="{D3DB8CA4-CF09-459F-A4BC-4F324FE8B47E}">
+      <formula1>$A$78:$A$81</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F53" xr:uid="{8F276E49-902F-4BBD-9E0B-A51B9A15EC6B}">
-      <formula1>$F$76:$F$84</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F54" xr:uid="{8F276E49-902F-4BBD-9E0B-A51B9A15EC6B}">
+      <formula1>$F$77:$F$85</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:R53" xr:uid="{74781059-03CD-4747-BF6A-E35BF8F2BF2E}">
-      <formula1>$G$77:$G$82</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:R31 L32:R53 G32:K54" xr:uid="{74781059-03CD-4747-BF6A-E35BF8F2BF2E}">
+      <formula1>$G$78:$G$83</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Minor changes, added left or right as slide in options
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAD48E2-B293-492A-B3BF-CA58770A7B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040E2C8C-5FC1-4879-810D-2A12A3AAA5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <sheet name="Gantt Chart" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Task Tracking'!$A$1:$R$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Task Tracking'!$A$1:$R$88</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="233">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -815,6 +815,33 @@
   </si>
   <si>
     <t>Choose which items should be brought on sideways</t>
+  </si>
+  <si>
+    <t>Consider using slower flicker script for stage lights</t>
+  </si>
+  <si>
+    <t>Use the script Dylan made for the into screen, currently light flicker is too fast and random</t>
+  </si>
+  <si>
+    <t>Collider is like a pentagon hexagon thing, we should aim for a cylinder if possible.</t>
+  </si>
+  <si>
+    <t>Can walk underneath table edge in first level</t>
+  </si>
+  <si>
+    <t>Same as above for mushrooms</t>
+  </si>
+  <si>
+    <t>These are cones, not as bad cause it does kind of deflect the jump backwards, but worth checking if we want cylinders</t>
+  </si>
+  <si>
+    <t>They kind of extend into the skull making the effect look strange when idle, consider extending outwards around the sides of the mask when idle: Perhaps even make the eyes slightly translucent and put a point light inside them to make the particle effects blend with the eyeball better</t>
+  </si>
+  <si>
+    <t>Consider which way the particles should be extending by default on the eyes</t>
+  </si>
+  <si>
+    <t>Add left or right option for where they can come in from for extra dynamics</t>
   </si>
 </sst>
 </file>
@@ -1507,10 +1534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
-  <dimension ref="A1:R87"/>
+  <dimension ref="A1:R88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2471,11 +2498,9 @@
         <v>220</v>
       </c>
       <c r="D18" s="1">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
         <v>7</v>
       </c>
@@ -2524,13 +2549,13 @@
         <v>223</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="D19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>7</v>
@@ -2545,7 +2570,7 @@
         <v>91</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>91</v>
+        <v>154</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>65</v>
@@ -4518,125 +4543,179 @@
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>2</v>
+        <v>224</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D56" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N56" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P56" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q56" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R56" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D57" s="1">
+        <v>3</v>
+      </c>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G56" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J56" s="1" t="s">
+      <c r="G57" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J57" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K56" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F79" t="s">
+      <c r="K57" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="80" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F80" t="s">
         <v>66</v>
       </c>
-      <c r="G79" s="25" t="s">
+      <c r="G80" s="25" t="s">
         <v>205</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>98</v>
-      </c>
-      <c r="F80" t="s">
-        <v>7</v>
-      </c>
-      <c r="G80" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="F81" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G81" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F82" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G82" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>88</v>
+      </c>
+      <c r="F83" t="s">
+        <v>22</v>
+      </c>
+      <c r="G83" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>89</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F84" t="s">
         <v>5</v>
       </c>
-      <c r="G83" t="s">
+      <c r="G84" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F84" t="s">
-        <v>76</v>
-      </c>
-      <c r="G84" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F85" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="G85" t="s">
-        <v>94</v>
+        <v>154</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F86" t="s">
-        <v>6</v>
+        <v>33</v>
+      </c>
+      <c r="G86" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F87" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F88" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R87" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}"/>
-  <conditionalFormatting sqref="A55:A56 A2:A52">
+  <autoFilter ref="A1:R88" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}"/>
+  <conditionalFormatting sqref="A2:A52 A55:A57">
     <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G64:H64 G81:G84 I53:J54 H80:K84 G65:K79 J64:K64 G85:K1048576 L34:R51 L54:R1048576 G55:K63 G34:K52 G1:R33">
+  <conditionalFormatting sqref="G65:H65 G82:G85 I53:J54 H81:K85 G66:K80 J65:K65 G86:K1048576 L34:R51 L54:R55 G55:K55 G34:K52 G1:R33 G57:K64 L57:R1048576 G56:R56">
     <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"Done (Needs Review)"</formula>
     </cfRule>
@@ -4681,7 +4760,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I53:J54 L34:R51 L54:R55 G55:K56 G34:K52 G8:R33">
+  <conditionalFormatting sqref="I53:J54 L34:R51 L54:R55 G55:K55 G34:K52 G8:R33 G57:K57 G56:R56">
     <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
@@ -4692,14 +4771,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A56" xr:uid="{D3DB8CA4-CF09-459F-A4BC-4F324FE8B47E}">
-      <formula1>$A$80:$A$83</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A57" xr:uid="{D3DB8CA4-CF09-459F-A4BC-4F324FE8B47E}">
+      <formula1>$A$81:$A$84</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F56" xr:uid="{8F276E49-902F-4BBD-9E0B-A51B9A15EC6B}">
-      <formula1>$F$79:$F$87</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F57" xr:uid="{8F276E49-902F-4BBD-9E0B-A51B9A15EC6B}">
+      <formula1>$F$80:$F$88</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L34:R55 G34:K56 G2:R33" xr:uid="{74781059-03CD-4747-BF6A-E35BF8F2BF2E}">
-      <formula1>$G$80:$G$85</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:R33 G34:K57 L34:R56" xr:uid="{74781059-03CD-4747-BF6A-E35BF8F2BF2E}">
+      <formula1>$G$81:$G$86</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4710,10 +4789,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4784,73 +4863,73 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="25" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>206</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>207</v>
-      </c>
-      <c r="D4" s="23" t="s">
+      <c r="B4" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="D5" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="24" t="s">
-        <v>18</v>
-      </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>111</v>
+        <v>227</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>113</v>
+        <v>226</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="F6" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>119</v>
+        <v>228</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>120</v>
+        <v>229</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>7</v>
@@ -4860,95 +4939,93 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>180</v>
+        <v>119</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>172</v>
+        <v>120</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
-        <v>87</v>
-      </c>
       <c r="B12" s="24" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>7</v>
@@ -4960,21 +5037,21 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
-        <v>87</v>
+    <row r="13" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>118</v>
@@ -4985,10 +5062,10 @@
         <v>98</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D14" s="24" t="s">
         <v>7</v>
@@ -5000,15 +5077,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>169</v>
+        <v>126</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>170</v>
+        <v>127</v>
       </c>
       <c r="D15" s="24" t="s">
         <v>7</v>
@@ -5020,74 +5097,134 @@
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>98</v>
-      </c>
-      <c r="D33" t="s">
+    <row r="16" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="F33" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="E16" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="D34" t="s">
+      <c r="B17" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="25" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="F34" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>88</v>
-      </c>
-      <c r="D35" t="s">
-        <v>22</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="F18" s="24" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>89</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D39" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A14:A15 A2:A11">
+  <conditionalFormatting sqref="A18 A2:A15">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F15">
+  <conditionalFormatting sqref="F2:F18">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
@@ -5099,14 +5236,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E15" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
-      <formula1>$D$33:$D$40</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E18" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
+      <formula1>$D$36:$D$43</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A15" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
-      <formula1>$A$33:$A$36</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A18" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
+      <formula1>$A$36:$A$39</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F15" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
-      <formula1>$F$33:$F$35</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F18" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
+      <formula1>$F$36:$F$38</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
more collider fixes on wells, mushrooms
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D956F9BE-6542-47C9-AB6A-60FC1F0BA0C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC73F59-62CA-46D2-9F50-8E0C72E759EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="1950" windowWidth="20775" windowHeight="18075" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -1536,8 +1536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R88"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3015,7 +3015,7 @@
         <v>92</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>93</v>
+        <v>154</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>65</v>
@@ -3449,7 +3449,7 @@
         <v>91</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>93</v>
+        <v>154</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>65</v>
@@ -4791,8 +4791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4918,7 +4918,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4938,7 +4938,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
First (broken) attempt at a line ghost thingy
A whole lot of a mess, but probably gonna redo anyway because wow is it bad for performance.
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Tim\Desktop\Git\strung-along6\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FB1D7F-966D-4211-9EEB-C7C85E077030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC3073F-3BFB-47C8-9B51-85F087539E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -1529,8 +1529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2344,7 +2344,7 @@
         <v>154</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>65</v>
+        <v>154</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>65</v>
@@ -2676,7 +2676,7 @@
         <v>91</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>65</v>
@@ -4784,8 +4784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4873,7 +4873,7 @@
         <v>22</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4969,7 +4969,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update prod doc, stealing line visuals from Tim
hehehehehehgheheghe
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Tim\Desktop\Git\strung-along6\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102730451\Desktop\udrjkdf\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC3073F-3BFB-47C8-9B51-85F087539E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7902640-AFF1-4C21-B432-F01F861D8CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1529,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R88"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3963,7 +3962,7 @@
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>91</v>
@@ -3978,7 +3977,7 @@
         <v>91</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>65</v>
@@ -4784,7 +4783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Prod doc recommit of shame...
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4421AA1E-5662-4B66-A42E-36CED2E0CABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C14D2F-FE90-4D77-A1BD-CE996A50CAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Gantt Chart" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Task Tracking'!$A$1:$R$89</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Task Tracking'!$A$1:$R$88</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="244">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -726,9 +726,6 @@
     <t>Working on fixing a bug which involves movement issues, still working on making edge snapping more tolerant, slingshotting mechanic</t>
   </si>
   <si>
-    <t>Make a clairvoyant mini grid around the characters</t>
-  </si>
-  <si>
     <t>Displays the grid lines wherever they are even if raised in the y axis</t>
   </si>
   <si>
@@ -874,6 +871,9 @@
   </si>
   <si>
     <t>Can't climb any more, holding grab button in air will hold puppet in vertical position infinitely, allowing them to swing, reintroduce the curved base while holding in air. As an extra thing, pressing grab button on the ground will have no effect, only if puppet is in the air.</t>
+  </si>
+  <si>
+    <t>Make the magic shadow grid which renders on every level of the y axis</t>
   </si>
 </sst>
 </file>
@@ -1559,28 +1559,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
-  <dimension ref="A1:R89"/>
+  <dimension ref="A1:R88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.88671875" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" customWidth="1"/>
-    <col min="13" max="13" width="15.5546875" customWidth="1"/>
-    <col min="14" max="18" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" customWidth="1"/>
+    <col min="14" max="18" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>86</v>
       </c>
@@ -1636,15 +1636,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>243</v>
       </c>
       <c r="D2" s="1">
         <v>5</v>
@@ -1690,15 +1690,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="25" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" s="25" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>98</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D3" s="29">
         <v>10</v>
@@ -1744,7 +1744,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>98</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>98</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>98</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>98</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>98</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>98</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>98</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>98</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:18" s="25" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" s="25" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>98</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="25" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" s="25" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>98</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:18" s="25" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" s="25" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>98</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:18" s="25" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" s="25" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>98</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>98</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="25" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>98</v>
       </c>
@@ -2510,15 +2510,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>220</v>
       </c>
       <c r="D18" s="1">
         <v>3</v>
@@ -2537,10 +2537,10 @@
         <v>91</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>65</v>
+        <v>154</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>65</v>
@@ -2564,15 +2564,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
@@ -2620,71 +2620,71 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:18" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="24">
         <v>1</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="24">
         <v>0.5</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I20" s="1" t="s">
+      <c r="G20" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="I20" s="24" t="s">
         <v>91</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>154</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+      <c r="L20" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="M20" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="N20" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="O20" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="P20" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q20" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="R20" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>195</v>
       </c>
       <c r="D21" s="1">
         <v>5</v>
@@ -2730,7 +2730,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
         <v>87</v>
       </c>
@@ -2786,7 +2786,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:18" s="25" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" s="25" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
         <v>87</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:18" s="25" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
         <v>87</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:18" s="25" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" s="25" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
         <v>87</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="72" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>87</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>124</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D26" s="1">
         <v>12</v>
@@ -3008,7 +3008,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>87</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>87</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>87</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>87</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
         <v>87</v>
       </c>
@@ -3280,7 +3280,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>87</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>87</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>87</v>
       </c>
@@ -3442,69 +3442,69 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="24" t="s">
         <v>183</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="24">
         <v>1</v>
       </c>
-      <c r="E35" s="1"/>
-      <c r="F35" s="21" t="s">
+      <c r="E35" s="24"/>
+      <c r="F35" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="G35" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I35" s="1" t="s">
+      <c r="G35" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="H35" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="I35" s="24" t="s">
         <v>91</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>92</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="N35" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="O35" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P35" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q35" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="R35" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+      <c r="L35" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="M35" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="N35" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="O35" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="P35" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q35" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="R35" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C36" s="20" t="s">
         <v>213</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>214</v>
       </c>
       <c r="D36" s="1">
         <v>1</v>
@@ -3552,7 +3552,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>88</v>
       </c>
@@ -3606,7 +3606,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>88</v>
       </c>
@@ -3658,7 +3658,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>88</v>
       </c>
@@ -3712,7 +3712,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>88</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>88</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>88</v>
       </c>
@@ -3874,7 +3874,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" s="25" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>88</v>
       </c>
@@ -3926,7 +3926,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
         <v>88</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>88</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>88</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>88</v>
       </c>
@@ -4142,7 +4142,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>89</v>
       </c>
@@ -4194,7 +4194,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>89</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>89</v>
       </c>
@@ -4302,7 +4302,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>89</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>89</v>
       </c>
@@ -4406,7 +4406,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>89</v>
       </c>
@@ -4460,7 +4460,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
         <v>89</v>
       </c>
@@ -4514,7 +4514,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
         <v>89</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>89</v>
       </c>
@@ -4622,15 +4622,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>224</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>225</v>
       </c>
       <c r="D57" s="1">
         <v>1</v>
@@ -4676,7 +4676,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>89</v>
       </c>
@@ -4684,7 +4684,7 @@
         <v>2</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D58" s="1">
         <v>3</v>
@@ -4708,108 +4708,129 @@
       <c r="K58" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="L58" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O58" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P58" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q58" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R58" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="80" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F80" t="s">
+        <v>66</v>
+      </c>
+      <c r="G80" s="25" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>98</v>
+      </c>
       <c r="F81" t="s">
-        <v>66</v>
-      </c>
-      <c r="G81" s="25" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="G81" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="F82" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="G82" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F83" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G83" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F84" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="G84" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>89</v>
-      </c>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F85" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="G85" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F86" t="s">
-        <v>76</v>
+        <v>33</v>
       </c>
       <c r="G86" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F87" t="s">
-        <v>33</v>
-      </c>
-      <c r="G87" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F88" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F89" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R89" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}"/>
-  <conditionalFormatting sqref="A56:A58 A2:A53">
-    <cfRule type="cellIs" dxfId="11" priority="18" operator="equal">
+  <autoFilter ref="A1:R88" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}"/>
+  <conditionalFormatting sqref="A2:A19 A36:A53 A21:A34 A56:A58">
+    <cfRule type="cellIs" dxfId="11" priority="19" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G66:H66 G83:G86 I54:J55 H82:K86 G67:K81 J66:K66 G87:K1048576 L35:R52 L55:R56 G56:K56 G35:K53 G58:K65 L58:R1048576 G57:R57 G1:R34">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+  <conditionalFormatting sqref="G65:H65 G82:G85 I54:J55 H81:K85 G66:K80 J65:K65 G86:K1048576 L36:R52 L55:R56 G56:K56 G36:K53 G1:R19 J35:K35 G21:R34 J20:K20 L59:R1048576 G59:K64 G57:R58">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>"Done (Needs Review)"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",G1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="14" operator="equal">
       <formula>"Done (Needs Testing)"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="15" operator="equal">
       <formula>"Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4819,28 +4840,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B31)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"Done (Needs Testing)"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>"Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:R15 G3:R3 I16:R16">
-    <cfRule type="colorScale" priority="44">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J22:K22 I54:J55 L35:R52 L55:R56 G56:K56 G35:K53 G58:K58 G57:R57 G4:R11 G17:R21 G2:R2 G23:R34">
-    <cfRule type="colorScale" priority="55">
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4850,6 +4861,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:R3">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G58:R58">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -4859,15 +4880,25 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J22:K22 I54:J55 L36:R52 L55:R56 G56:K56 G36:K53 G4:R11 G17:R19 G2:R2 G23:R34 J35:K35 G21:R21 J20:K20 G57:R57">
+    <cfRule type="colorScale" priority="67">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G35:K58 G2:R34 L35:R57" xr:uid="{74781059-03CD-4747-BF6A-E35BF8F2BF2E}">
-      <formula1>$G$82:$G$87</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:R58" xr:uid="{74781059-03CD-4747-BF6A-E35BF8F2BF2E}">
+      <formula1>$G$81:$G$86</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A58" xr:uid="{D3DB8CA4-CF09-459F-A4BC-4F324FE8B47E}">
-      <formula1>$A$82:$A$85</formula1>
+      <formula1>$A$81:$A$84</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F58" xr:uid="{8F276E49-902F-4BBD-9E0B-A51B9A15EC6B}">
-      <formula1>$F$81:$F$89</formula1>
+      <formula1>$F$80:$F$88</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4884,15 +4915,15 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="48.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="48.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>86</v>
       </c>
@@ -4912,15 +4943,15 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="25" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="25" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>98</v>
       </c>
       <c r="B2" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2" s="24" t="s">
         <v>215</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>216</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>7</v>
@@ -4932,15 +4963,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="111.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>218</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>7</v>
@@ -4952,7 +4983,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>87</v>
       </c>
@@ -4972,7 +5003,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>87</v>
       </c>
@@ -4990,15 +5021,15 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
@@ -5010,15 +5041,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>228</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>229</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>7</v>
@@ -5030,7 +5061,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>88</v>
       </c>
@@ -5048,7 +5079,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>88</v>
       </c>
@@ -5068,7 +5099,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>88</v>
       </c>
@@ -5088,15 +5119,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>7</v>
@@ -5108,7 +5139,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>98</v>
       </c>
@@ -5128,7 +5159,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>98</v>
       </c>
@@ -5148,7 +5179,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>98</v>
       </c>
@@ -5168,7 +5199,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>98</v>
       </c>
@@ -5188,7 +5219,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>87</v>
       </c>
@@ -5208,7 +5239,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
         <v>87</v>
       </c>
@@ -5228,15 +5259,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="25" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="25" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>87</v>
       </c>
       <c r="B18" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="C18" s="24" t="s">
         <v>206</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>207</v>
       </c>
       <c r="D18" s="23" t="s">
         <v>7</v>
@@ -5248,7 +5279,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>98</v>
       </c>
@@ -5259,7 +5290,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>87</v>
       </c>
@@ -5270,7 +5301,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>88</v>
       </c>
@@ -5281,7 +5312,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>89</v>
       </c>
@@ -5289,22 +5320,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>69</v>
       </c>
@@ -5349,20 +5380,20 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="12" customWidth="1"/>
-    <col min="4" max="5" width="17.88671875" style="12" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="13" customWidth="1"/>
-    <col min="7" max="11" width="17.88671875" style="12" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" style="12" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" style="12" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="12"/>
+    <col min="1" max="1" width="24.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="12" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="13" customWidth="1"/>
+    <col min="7" max="11" width="17.85546875" style="12" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="12" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="12" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="31" t="s">
         <v>36</v>
@@ -5379,7 +5410,7 @@
       <c r="L1" s="31"/>
       <c r="M1" s="31"/>
     </row>
-    <row r="2" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>85</v>
       </c>
@@ -5420,7 +5451,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="216" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>22</v>
       </c>
@@ -5437,7 +5468,7 @@
         <v>193</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
@@ -5447,7 +5478,7 @@
       <c r="L3" s="14"/>
       <c r="M3" s="14"/>
     </row>
-    <row r="4" spans="1:13" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>18</v>
       </c>
@@ -5461,10 +5492,10 @@
         <v>171</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
@@ -5474,7 +5505,7 @@
       <c r="L4" s="14"/>
       <c r="M4" s="14"/>
     </row>
-    <row r="5" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>5</v>
       </c>
@@ -5491,7 +5522,7 @@
         <v>191</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
@@ -5501,7 +5532,7 @@
       <c r="L5" s="14"/>
       <c r="M5" s="14"/>
     </row>
-    <row r="6" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>33</v>
       </c>
@@ -5515,10 +5546,10 @@
         <v>135</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
@@ -5528,7 +5559,7 @@
       <c r="L6" s="14"/>
       <c r="M6" s="14"/>
     </row>
-    <row r="7" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>76</v>
       </c>
@@ -5542,10 +5573,10 @@
         <v>128</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -5555,7 +5586,7 @@
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
     </row>
-    <row r="8" spans="1:13" ht="144" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>6</v>
       </c>
@@ -5566,13 +5597,13 @@
         <v>72</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
@@ -5582,7 +5613,7 @@
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
     </row>
-    <row r="9" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>7</v>
       </c>
@@ -5593,13 +5624,13 @@
         <v>70</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -5609,7 +5640,7 @@
       <c r="L9" s="14"/>
       <c r="M9" s="14"/>
     </row>
-    <row r="10" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>69</v>
       </c>
@@ -5623,10 +5654,10 @@
         <v>192</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -5636,7 +5667,7 @@
       <c r="L10" s="14"/>
       <c r="M10" s="14"/>
     </row>
-    <row r="11" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>66</v>
       </c>
@@ -5653,7 +5684,7 @@
         <v>65</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -5680,26 +5711,26 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
+    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
+    <row r="9" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>211</v>
-      </c>
-    </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
-        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -5715,7 +5746,7 @@
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5729,12 +5760,12 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="31" t="s">
         <v>36</v>
@@ -5751,7 +5782,7 @@
       <c r="L1" s="31"/>
       <c r="M1" s="31"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>37</v>
       </c>
@@ -5792,7 +5823,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>50</v>
       </c>
@@ -5809,7 +5840,7 @@
       <c r="L3" s="32"/>
       <c r="M3" s="32"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>51</v>
       </c>
@@ -5826,7 +5857,7 @@
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>52</v>
       </c>
@@ -5843,7 +5874,7 @@
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
         <v>53</v>
       </c>
@@ -5860,7 +5891,7 @@
       <c r="L6" s="32"/>
       <c r="M6" s="32"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>54</v>
       </c>
@@ -5877,7 +5908,7 @@
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>55</v>
       </c>
@@ -5894,7 +5925,7 @@
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>56</v>
       </c>
@@ -5911,7 +5942,7 @@
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>57</v>
       </c>
@@ -5928,7 +5959,7 @@
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
         <v>58</v>
       </c>
@@ -5945,7 +5976,7 @@
       <c r="L11" s="32"/>
       <c r="M11" s="32"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>59</v>
       </c>
@@ -5962,7 +5993,7 @@
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>60</v>
       </c>
@@ -5979,7 +6010,7 @@
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>61</v>
       </c>
@@ -5996,7 +6027,7 @@
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>62</v>
       </c>
@@ -6013,7 +6044,7 @@
       <c r="L15" s="32"/>
       <c r="M15" s="32"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>63</v>
       </c>
@@ -6030,7 +6061,7 @@
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
More animations added + some PFX
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dennys\Documents\Strung Along\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B95B41-D78F-4E4F-B4FB-02CDF3DB7FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6527C5E9-C3C4-4772-B35C-F7347FB54145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -1262,14 +1262,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1851,8 +1851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3851,7 +3851,7 @@
       <c r="B37" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="C37" s="29" t="s">
+      <c r="C37" s="27" t="s">
         <v>209</v>
       </c>
       <c r="D37" s="17">
@@ -3860,7 +3860,7 @@
       <c r="E37" s="17">
         <v>1</v>
       </c>
-      <c r="F37" s="29" t="s">
+      <c r="F37" s="27" t="s">
         <v>18</v>
       </c>
       <c r="G37" s="17" t="s">
@@ -4730,7 +4730,7 @@
         <v>91</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>91</v>
+        <v>154</v>
       </c>
       <c r="L53" s="1" t="s">
         <v>65</v>
@@ -5961,20 +5961,20 @@
   <sheetData>
     <row r="1" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
     </row>
     <row r="2" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6733,20 +6733,20 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6790,21 +6790,21 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -6841,21 +6841,21 @@
       <c r="M5" s="7"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -6926,21 +6926,21 @@
       <c r="M10" s="6"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -6994,21 +6994,21 @@
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">

</xml_diff>

<commit_message>
more cinematics, basic act change animated
not implemented yet, but that's the easy bit
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dennys\Documents\Strung Along\strung-along\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6527C5E9-C3C4-4772-B35C-F7347FB54145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB21360-5E32-4E0D-9859-752512FEFD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="2" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -1851,8 +1851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K53" sqref="K53"/>
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5412,7 +5412,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5466,23 +5466,23 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:7" s="24" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="17" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5942,7 +5942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB7A6BC1-ED0D-41E7-903B-B5F7393F73BD}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Grabbing puppet who is grabbing you now cancels the grab (plus prod doc bug report)
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Tim\Desktop\Git\strung-along6\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB21360-5E32-4E0D-9859-752512FEFD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927E76C6-593F-4E5D-8ECD-E78BCD4D0F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="2" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1324" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="292">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -1013,6 +1013,12 @@
   </si>
   <si>
     <t>Curtains come in, flashy lights, etc</t>
+  </si>
+  <si>
+    <t>Inconsistant tangle changes when jumping over</t>
+  </si>
+  <si>
+    <t>Jumping over the other puppet while tangled provides somewhat inconsistant results, sometimes it updates the tangle by 1, other times it doesn't, leading to strange tangling behavior.</t>
   </si>
 </sst>
 </file>
@@ -1851,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R89"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5409,10 +5415,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5585,64 +5591,64 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+    <row r="9" spans="1:7" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B10" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C10" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E10" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F10" s="17" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D11" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>18</v>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -5650,10 +5656,10 @@
         <v>98</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="D12" s="17" t="s">
         <v>7</v>
@@ -5670,10 +5676,10 @@
         <v>98</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>7</v>
@@ -5690,10 +5696,10 @@
         <v>98</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>126</v>
+        <v>169</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>127</v>
+        <v>170</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>7</v>
@@ -5706,14 +5712,14 @@
       </c>
     </row>
     <row r="15" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>210</v>
+        <v>126</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>211</v>
+        <v>127</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>7</v>
@@ -5721,19 +5727,19 @@
       <c r="E15" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="1" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>157</v>
+        <v>210</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>158</v>
+        <v>211</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>7</v>
@@ -5741,7 +5747,7 @@
       <c r="E16" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="17" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5750,16 +5756,16 @@
         <v>87</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>118</v>
@@ -5770,30 +5776,30 @@
         <v>87</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>205</v>
+        <v>162</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>206</v>
+        <v>163</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>7</v>
@@ -5801,19 +5807,19 @@
       <c r="E19" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>7</v>
@@ -5825,94 +5831,114 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>181</v>
+        <v>221</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>182</v>
+        <v>222</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="22" t="s">
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="D40" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F39" s="22" t="s">
+      <c r="F40" s="22" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="22" t="s">
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D40" s="22" t="s">
+      <c r="D41" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="F40" s="22" t="s">
+      <c r="F41" s="22" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D41" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F41" s="22" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F42" s="22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="D42" s="22" t="s">
+      <c r="D43" s="22" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D43" s="22" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D44" s="22" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D45" s="22" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D46" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D47" s="22" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A18:A21 A2:A15">
+  <conditionalFormatting sqref="A19:A22 A2:A16">
     <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F21">
+  <conditionalFormatting sqref="F2:F22">
     <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
@@ -5924,14 +5950,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E21" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
-      <formula1>$D$39:$D$46</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E22" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
+      <formula1>$D$40:$D$47</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A21" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
-      <formula1>$A$39:$A$42</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A22" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
+      <formula1>$A$40:$A$43</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F21" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
-      <formula1>$F$39:$F$41</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F22" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
+      <formula1>$F$40:$F$42</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5942,7 +5968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB7A6BC1-ED0D-41E7-903B-B5F7393F73BD}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed the snapping when going between lines
So much code for such a small thing lmao, but it does make fixing the other line problems easier
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Tim\Desktop\Git\strung-along6\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927E76C6-593F-4E5D-8ECD-E78BCD4D0F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B831A2C2-25C8-4C87-B595-D6B9A507A96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1331" uniqueCount="292">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -1857,7 +1857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -5417,8 +5417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5566,7 +5566,9 @@
       <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="F7" s="1" t="s">
         <v>116</v>
       </c>
@@ -5588,7 +5590,7 @@
         <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Prod doc bug report
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Tim\Desktop\Git\strung-along6\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3F02CF-4EE1-4720-ACE2-9A04CC73659D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E3E9BD-F1F8-4882-B869-1017A9A8E655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="296">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -1025,6 +1025,12 @@
   </si>
   <si>
     <t>Make switching lines smoother and respond to the player's predicted intentions rather than their literal inputs better</t>
+  </si>
+  <si>
+    <t>Very, very small reverse snapping when switching between some lines</t>
+  </si>
+  <si>
+    <t>So ok hear me out, we no longer have snapping, we have *reverse snapping*, it's very small and scales with the directionChangeBoost, still something to do with the order of points, I can not figure it out</t>
   </si>
 </sst>
 </file>
@@ -1863,8 +1869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L49" sqref="L49"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1973,7 +1979,7 @@
         <v>92</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>65</v>
@@ -5477,10 +5483,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5675,64 +5681,64 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B11" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C11" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D11" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E11" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F11" s="17" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D12" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="17" t="s">
-        <v>18</v>
+      <c r="E12" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -5740,10 +5746,10 @@
         <v>98</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>7</v>
@@ -5760,10 +5766,10 @@
         <v>98</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>7</v>
@@ -5780,10 +5786,10 @@
         <v>98</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>126</v>
+        <v>169</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>127</v>
+        <v>170</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>7</v>
@@ -5796,14 +5802,14 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>210</v>
+        <v>126</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>211</v>
+        <v>127</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>7</v>
@@ -5811,19 +5817,19 @@
       <c r="E16" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="1" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>157</v>
+        <v>210</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>158</v>
+        <v>211</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>7</v>
@@ -5831,7 +5837,7 @@
       <c r="E17" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="17" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5840,16 +5846,16 @@
         <v>87</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>118</v>
@@ -5860,30 +5866,30 @@
         <v>87</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>205</v>
+        <v>162</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>206</v>
+        <v>163</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>7</v>
@@ -5891,19 +5897,19 @@
       <c r="E20" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>7</v>
@@ -5915,94 +5921,114 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>181</v>
+        <v>221</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>182</v>
+        <v>222</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="22" t="s">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="22" t="s">
+      <c r="D41" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F40" s="22" t="s">
+      <c r="F41" s="22" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="22" t="s">
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D41" s="22" t="s">
+      <c r="D42" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="F41" s="22" t="s">
+      <c r="F42" s="22" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D42" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F42" s="22" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D43" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F43" s="22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="D43" s="22" t="s">
+      <c r="D44" s="22" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D44" s="22" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D45" s="22" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D46" s="22" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D47" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D48" s="22" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A19:A22 A2:A16">
+  <conditionalFormatting sqref="A20:A23 A2:A17">
     <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F22">
+  <conditionalFormatting sqref="F2:F23">
     <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
@@ -6014,14 +6040,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E22" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
-      <formula1>$D$40:$D$47</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E23" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
+      <formula1>$D$41:$D$48</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A22" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
-      <formula1>$A$40:$A$43</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A23" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
+      <formula1>$A$41:$A$44</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F22" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
-      <formula1>$F$40:$F$42</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F23" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
+      <formula1>$F$41:$F$43</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Moving off grid bug fixed
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Tim\Desktop\Git\strung-along6\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E3E9BD-F1F8-4882-B869-1017A9A8E655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887807F0-30A5-42E9-B810-AD7297844FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
@@ -1027,10 +1027,10 @@
     <t>Make switching lines smoother and respond to the player's predicted intentions rather than their literal inputs better</t>
   </si>
   <si>
-    <t>Very, very small reverse snapping when switching between some lines</t>
-  </si>
-  <si>
     <t>So ok hear me out, we no longer have snapping, we have *reverse snapping*, it's very small and scales with the directionChangeBoost, still something to do with the order of points, I can not figure it out</t>
+  </si>
+  <si>
+    <t>Very small reverse snapping when switching between some lines</t>
   </si>
 </sst>
 </file>
@@ -5486,7 +5486,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5600,7 +5600,7 @@
         <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5683,13 +5683,13 @@
     </row>
     <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>295</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
level transition skip added
its so fast the puppets fall into water hazards before the tiles can save them
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67E62E2-F493-499E-AC15-92D35D7AE67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408515AC-FDB9-4386-9168-B37FBC3E1B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="2" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -1905,28 +1905,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L62" sqref="L62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.44140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.88671875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="22"/>
-    <col min="5" max="5" width="10.109375" style="22" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="20.44140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="22"/>
+    <col min="5" max="5" width="10.140625" style="22" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="20.42578125" style="22" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" style="22" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" style="22" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" style="22" customWidth="1"/>
-    <col min="13" max="13" width="15.5546875" style="22" customWidth="1"/>
-    <col min="14" max="18" width="11.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.109375" style="22"/>
+    <col min="11" max="11" width="19.7109375" style="22" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="22" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" style="22" customWidth="1"/>
+    <col min="14" max="18" width="11.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>86</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>98</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>98</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>98</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>98</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>98</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>98</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>98</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>98</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>98</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>98</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>98</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>98</v>
       </c>
@@ -2630,7 +2630,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>98</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>98</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>98</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>98</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>98</v>
       </c>
@@ -2906,7 +2906,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>98</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:18" s="24" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>98</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>87</v>
       </c>
@@ -3074,7 +3074,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>87</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>87</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>87</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>87</v>
       </c>
@@ -3294,7 +3294,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>87</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:18" s="24" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" s="24" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>87</v>
       </c>
@@ -3406,7 +3406,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:18" s="24" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>87</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:18" s="24" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>87</v>
       </c>
@@ -3518,7 +3518,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="72" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>87</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>87</v>
       </c>
@@ -3626,7 +3626,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:18" s="24" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>87</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>87</v>
       </c>
@@ -3734,7 +3734,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>87</v>
       </c>
@@ -3788,7 +3788,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:18" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>87</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>87</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>87</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>87</v>
       </c>
@@ -4006,7 +4006,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>88</v>
       </c>
@@ -4060,7 +4060,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:18" s="24" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>88</v>
       </c>
@@ -4116,7 +4116,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>88</v>
       </c>
@@ -4170,7 +4170,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>88</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>88</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:18" s="24" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>88</v>
       </c>
@@ -4332,7 +4332,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>88</v>
       </c>
@@ -4386,7 +4386,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>88</v>
       </c>
@@ -4438,7 +4438,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>88</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
         <v>88</v>
       </c>
@@ -4544,7 +4544,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>88</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>88</v>
       </c>
@@ -4613,7 +4613,7 @@
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>91</v>
@@ -4652,7 +4652,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>88</v>
       </c>
@@ -4706,7 +4706,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>88</v>
       </c>
@@ -4762,7 +4762,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
         <v>89</v>
       </c>
@@ -4814,7 +4814,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
         <v>89</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>89</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>89</v>
       </c>
@@ -4974,7 +4974,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>89</v>
       </c>
@@ -5026,7 +5026,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>89</v>
       </c>
@@ -5080,7 +5080,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
         <v>89</v>
       </c>
@@ -5134,7 +5134,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
         <v>89</v>
       </c>
@@ -5188,7 +5188,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
         <v>89</v>
       </c>
@@ -5242,7 +5242,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>89</v>
       </c>
@@ -5296,7 +5296,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>89</v>
       </c>
@@ -5350,7 +5350,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>89</v>
       </c>
@@ -5404,7 +5404,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>89</v>
       </c>
@@ -5458,7 +5458,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F85" s="22" t="s">
         <v>66</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="22" t="s">
         <v>98</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="22" t="s">
         <v>87</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="22" t="s">
         <v>88</v>
       </c>
@@ -5499,7 +5499,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="22" t="s">
         <v>89</v>
       </c>
@@ -5510,7 +5510,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="F90" s="22" t="s">
         <v>76</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F91" s="22" t="s">
         <v>33</v>
       </c>
@@ -5526,12 +5526,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F92" s="22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F93" s="22" t="s">
         <v>69</v>
       </c>
@@ -5687,18 +5687,18 @@
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="22"/>
-    <col min="2" max="3" width="48.88671875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="22"/>
+    <col min="2" max="3" width="48.85546875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="21.5546875" style="22" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="22"/>
+    <col min="6" max="6" width="11.28515625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" style="22" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>86</v>
       </c>
@@ -5718,7 +5718,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>87</v>
       </c>
@@ -5738,7 +5738,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="24" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="24" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>87</v>
       </c>
@@ -5758,7 +5758,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="111.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>87</v>
       </c>
@@ -5778,7 +5778,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>87</v>
       </c>
@@ -5798,7 +5798,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>87</v>
       </c>
@@ -5816,7 +5816,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>88</v>
       </c>
@@ -5836,7 +5836,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>88</v>
       </c>
@@ -5856,7 +5856,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="24" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>87</v>
       </c>
@@ -5876,7 +5876,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>88</v>
       </c>
@@ -5896,7 +5896,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>88</v>
       </c>
@@ -5916,7 +5916,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>88</v>
       </c>
@@ -5936,7 +5936,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>98</v>
       </c>
@@ -5956,7 +5956,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>98</v>
       </c>
@@ -5976,7 +5976,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>98</v>
       </c>
@@ -5996,7 +5996,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>98</v>
       </c>
@@ -6016,7 +6016,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>98</v>
       </c>
@@ -6036,7 +6036,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>87</v>
       </c>
@@ -6056,7 +6056,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>87</v>
       </c>
@@ -6076,7 +6076,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>87</v>
       </c>
@@ -6096,7 +6096,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>88</v>
       </c>
@@ -6116,7 +6116,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>88</v>
       </c>
@@ -6136,7 +6136,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>88</v>
       </c>
@@ -6156,7 +6156,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
         <v>98</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
         <v>87</v>
       </c>
@@ -6178,7 +6178,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
         <v>88</v>
       </c>
@@ -6189,7 +6189,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
         <v>89</v>
       </c>
@@ -6197,22 +6197,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D45" s="22" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D46" s="22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D47" s="22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D48" s="22" t="s">
         <v>69</v>
       </c>
@@ -6253,24 +6253,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB7A6BC1-ED0D-41E7-903B-B5F7393F73BD}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="9" customWidth="1"/>
-    <col min="4" max="5" width="17.88671875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="10" customWidth="1"/>
-    <col min="7" max="11" width="17.88671875" style="9" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" style="9" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" style="9" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="24.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="9" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="10" customWidth="1"/>
+    <col min="7" max="11" width="17.85546875" style="9" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="9" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="9" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="28" t="s">
         <v>36</v>
@@ -6287,7 +6287,7 @@
       <c r="L1" s="28"/>
       <c r="M1" s="28"/>
     </row>
-    <row r="2" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>85</v>
       </c>
@@ -6328,7 +6328,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="216" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>22</v>
       </c>
@@ -6357,7 +6357,7 @@
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
     </row>
-    <row r="4" spans="1:13" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>18</v>
       </c>
@@ -6386,7 +6386,7 @@
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
     </row>
-    <row r="5" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
@@ -6415,7 +6415,7 @@
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
     </row>
-    <row r="6" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>33</v>
       </c>
@@ -6444,7 +6444,7 @@
       <c r="L6" s="11"/>
       <c r="M6" s="11"/>
     </row>
-    <row r="7" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>76</v>
       </c>
@@ -6473,7 +6473,7 @@
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="1:13" ht="144" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -6502,7 +6502,7 @@
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
     </row>
-    <row r="9" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>7</v>
       </c>
@@ -6531,7 +6531,7 @@
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>69</v>
       </c>
@@ -6560,7 +6560,7 @@
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>66</v>
       </c>
@@ -6606,19 +6606,19 @@
       <selection activeCell="F10" sqref="F10:G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="22"/>
-    <col min="2" max="2" width="38.33203125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="59.88671875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="22" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.44140625" style="22" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="22"/>
+    <col min="2" max="2" width="38.28515625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="59.85546875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" style="22" customWidth="1"/>
     <col min="7" max="7" width="18" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="22"/>
+    <col min="8" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>86</v>
       </c>
@@ -6641,7 +6641,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>98</v>
       </c>
@@ -6664,7 +6664,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>98</v>
       </c>
@@ -6687,7 +6687,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>87</v>
       </c>
@@ -6710,7 +6710,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>87</v>
       </c>
@@ -6733,7 +6733,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>87</v>
       </c>
@@ -6756,7 +6756,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>87</v>
       </c>
@@ -6779,7 +6779,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>98</v>
       </c>
@@ -6790,7 +6790,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>87</v>
       </c>
@@ -6801,7 +6801,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>88</v>
       </c>
@@ -6809,7 +6809,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>89</v>
       </c>
@@ -6864,19 +6864,19 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="22"/>
-    <col min="2" max="2" width="38.33203125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="59.88671875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="22" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.44140625" style="22" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="22"/>
+    <col min="2" max="2" width="38.28515625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="59.85546875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" style="22" customWidth="1"/>
     <col min="7" max="7" width="18" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="22"/>
+    <col min="8" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>86</v>
       </c>
@@ -6899,7 +6899,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>98</v>
       </c>
@@ -6922,7 +6922,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>87</v>
       </c>
@@ -6945,7 +6945,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>87</v>
       </c>
@@ -6953,7 +6953,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>87</v>
       </c>
@@ -6964,7 +6964,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>87</v>
       </c>
@@ -6972,7 +6972,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>87</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>98</v>
       </c>
@@ -6991,7 +6991,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>87</v>
       </c>
@@ -7002,7 +7002,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>88</v>
       </c>
@@ -7010,7 +7010,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>89</v>
       </c>
@@ -7055,12 +7055,12 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="28" t="s">
         <v>36</v>
@@ -7077,7 +7077,7 @@
       <c r="L1" s="28"/>
       <c r="M1" s="28"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -7118,7 +7118,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>50</v>
       </c>
@@ -7135,7 +7135,7 @@
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>51</v>
       </c>
@@ -7152,7 +7152,7 @@
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>52</v>
       </c>
@@ -7169,7 +7169,7 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>53</v>
       </c>
@@ -7186,7 +7186,7 @@
       <c r="L6" s="29"/>
       <c r="M6" s="29"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>54</v>
       </c>
@@ -7203,7 +7203,7 @@
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>55</v>
       </c>
@@ -7220,7 +7220,7 @@
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>56</v>
       </c>
@@ -7237,7 +7237,7 @@
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>57</v>
       </c>
@@ -7254,7 +7254,7 @@
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>58</v>
       </c>
@@ -7271,7 +7271,7 @@
       <c r="L11" s="29"/>
       <c r="M11" s="29"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>59</v>
       </c>
@@ -7288,7 +7288,7 @@
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>60</v>
       </c>
@@ -7305,7 +7305,7 @@
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>61</v>
       </c>
@@ -7322,7 +7322,7 @@
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>62</v>
       </c>
@@ -7339,7 +7339,7 @@
       <c r="L15" s="29"/>
       <c r="M15" s="29"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>63</v>
       </c>
@@ -7356,7 +7356,7 @@
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
framework for breakable props
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408515AC-FDB9-4386-9168-B37FBC3E1B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CBD4FB-15E9-458B-801B-FE6433531E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="2" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -1073,7 +1073,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1122,8 +1122,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1158,6 +1165,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -1233,10 +1245,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1325,8 +1338,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="26">
@@ -1905,8 +1922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R93"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L62" sqref="L62"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2122,8 +2139,8 @@
       <c r="K4" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="L4" s="19" t="s">
-        <v>91</v>
+      <c r="L4" s="30" t="s">
+        <v>92</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>65</v>
@@ -6253,8 +6270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB7A6BC1-ED0D-41E7-903B-B5F7393F73BD}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
god damnit prod doc update
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B9E387-A512-499C-A597-C48452C83C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965035E9-76D4-48BD-A421-1D65721D8D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -1073,7 +1073,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1122,15 +1122,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1165,11 +1158,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -1245,11 +1233,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1332,9 +1319,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1342,11 +1326,10 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="30">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1591,6 +1574,46 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEAF8A4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC4FBA9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1922,8 +1945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S63" sqref="S63"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2120,7 +2143,9 @@
       <c r="D4" s="19">
         <v>4</v>
       </c>
-      <c r="E4" s="19"/>
+      <c r="E4" s="19">
+        <v>4</v>
+      </c>
       <c r="F4" s="19" t="s">
         <v>18</v>
       </c>
@@ -2139,11 +2164,11 @@
       <c r="K4" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="L4" s="28" t="s">
+      <c r="L4" s="17" t="s">
         <v>92</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>65</v>
@@ -5556,26 +5581,26 @@
   </sheetData>
   <autoFilter ref="A1:R93" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}"/>
   <conditionalFormatting sqref="A25:A38 A55:A58 A62:A64 A40:A50 A2:A20 A22:A23">
-    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G70:H70 G87:G90 I59:J60 H86:K90 G71:K85 J70:K70 G91:K1048576 J61 J39:K39 J24:K24 G66:K69 G55:K58 L55:R57 G25:R38 I53:J54 G62:R64 G1:R2 G15:R20 I14:R14 I3:R3 M4:R6 G22:R23 J21:R21 G7:R13 G40:R50 J51:R51 L52:R52 L66:R1048576 L65">
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="15" operator="equal">
       <formula>"Done (Needs Review)"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="20" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",G1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
       <formula>"Done (Needs Testing)"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
       <formula>"Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="colorScale" priority="15">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5585,18 +5610,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="containsText" dxfId="24" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="24" priority="17" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B35)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="18" operator="equal">
       <formula>"Done (Needs Testing)"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="19" operator="equal">
       <formula>"Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:R18 I19:R19 I3:R3 M4:R6">
-    <cfRule type="colorScale" priority="52">
+    <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5606,7 +5631,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:R3 M4:R6">
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5616,7 +5641,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G63:R63">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5626,7 +5651,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26:K26 I59:J60 J61 G2:R2 J39:K39 G25:R25 J24:K24 G55:K58 L55:R57 G27:R38 I53:J54 G62:R62 G20:R20 I14:R14 G22:R23 J21:R21 G7:R13 G40:R50 J51:R51 L52:R52">
-    <cfRule type="colorScale" priority="74">
+    <cfRule type="colorScale" priority="79">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5636,7 +5661,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G64:R64">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5646,7 +5671,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L65">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5656,20 +5681,44 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L58">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="6" operator="equal">
       <formula>"Done (Needs Review)"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="2" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="20" priority="7" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",L58)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
       <formula>"Done (Needs Testing)"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
       <formula>"Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L58">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Done (Needs Review)"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",L4)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"Done (Needs Testing)"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+      <formula>"Started"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -5700,7 +5749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -6289,20 +6338,20 @@
   <sheetData>
     <row r="1" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
     </row>
     <row r="2" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -7079,20 +7128,20 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -7136,21 +7185,21 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -7187,21 +7236,21 @@
       <c r="M5" s="7"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -7272,21 +7321,21 @@
       <c r="M10" s="6"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -7340,21 +7389,21 @@
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">

</xml_diff>

<commit_message>
Stage fog added and ambient particles fixed
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dennys\Documents\Strung Along\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965035E9-76D4-48BD-A421-1D65721D8D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CA9DF8-ECDF-4324-BE7E-642895EA6A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -1332,46 +1332,6 @@
   <dxfs count="30">
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAF8A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4FBA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1507,6 +1467,46 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEAF8A4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC4FBA9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1945,8 +1945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L64" sqref="L64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4532,7 +4532,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
         <v>88</v>
       </c>
@@ -5425,7 +5425,7 @@
         <v>91</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>91</v>
+        <v>154</v>
       </c>
       <c r="M64" s="1" t="s">
         <v>65</v>
@@ -5705,16 +5705,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
       <formula>"Done (Needs Review)"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",L4)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>"Done (Needs Testing)"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>"Started"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6285,18 +6285,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A20:A23 A2:A3 A6:A7 A9:A17">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F23">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>"Unfixed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6319,7 +6319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB7A6BC1-ED0D-41E7-903B-B5F7393F73BD}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -6882,28 +6882,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A7">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G7">
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"More Data Needed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"Acceptable"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"Unacceptable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7083,18 +7083,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A7">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G3">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"More Data Needed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Acceptable"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Unacceptable"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Line display applied to stage scene and sinking fixed?
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Tim\Desktop\Git\strung-along6\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE29AF2-002E-4BA4-89B7-FA8775110E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F37A2B3-A9D3-4AF2-9260-681834F0FB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="309">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -1067,6 +1067,9 @@
   </si>
   <si>
     <t>Reformatted act 1 levels, boiled it down to 3. Implemented act 2 level 1 and 2, bulk out the levels.</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -1945,7 +1948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
@@ -5747,10 +5750,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5764,7 +5767,7 @@
     <col min="8" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>86</v>
       </c>
@@ -5784,7 +5787,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>87</v>
       </c>
@@ -5804,7 +5807,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="24" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="24" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>87</v>
       </c>
@@ -5824,7 +5827,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>87</v>
       </c>
@@ -5844,7 +5847,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>87</v>
       </c>
@@ -5864,7 +5867,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>87</v>
       </c>
@@ -5877,12 +5880,17 @@
       <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="F6" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>88</v>
       </c>
@@ -5902,7 +5910,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>88</v>
       </c>
@@ -5922,7 +5930,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>87</v>
       </c>
@@ -5942,7 +5950,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>88</v>
       </c>
@@ -5962,7 +5970,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>88</v>
       </c>
@@ -5982,7 +5990,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>88</v>
       </c>
@@ -6002,7 +6010,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>98</v>
       </c>
@@ -6022,7 +6030,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>98</v>
       </c>
@@ -6042,7 +6050,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>98</v>
       </c>
@@ -6062,7 +6070,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
Redid UI with buttons
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Tim\Desktop\Git\strung-along6\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F37A2B3-A9D3-4AF2-9260-681834F0FB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C1CEC4-E8EE-48F9-842E-CD278DA51396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="313">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -1070,6 +1070,18 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>Puppets maintaining position when respawning</t>
+  </si>
+  <si>
+    <t>Seems to happen if input controols are held down while respawning</t>
+  </si>
+  <si>
+    <t>Level select button raycasting completely cooked</t>
+  </si>
+  <si>
+    <t>Can't seem to fix for some reason rip</t>
   </si>
 </sst>
 </file>
@@ -1948,8 +1960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R93"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3321,7 +3333,7 @@
         <v>92</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>93</v>
+        <v>154</v>
       </c>
       <c r="N25" s="1" t="s">
         <v>65</v>
@@ -4303,7 +4315,7 @@
         <v>92</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>65</v>
+        <v>154</v>
       </c>
       <c r="N43" s="1" t="s">
         <v>65</v>
@@ -5750,10 +5762,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5807,101 +5819,98 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="24" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>238</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>241</v>
-      </c>
-      <c r="D3" s="17" t="s">
+      <c r="B3" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="F3" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>239</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="D4" s="17" t="s">
+      <c r="B4" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>18</v>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D5" s="17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>111</v>
+        <v>289</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>113</v>
+        <v>290</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>119</v>
+        <v>294</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>120</v>
+        <v>293</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>22</v>
@@ -5910,75 +5919,75 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>22</v>
+      <c r="B8" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>22</v>
+        <v>98</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>18</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>88</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>240</v>
+        <v>169</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>242</v>
+        <v>170</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>7</v>
@@ -5986,39 +5995,39 @@
       <c r="E11" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>5</v>
+      <c r="E12" s="17" t="s">
+        <v>18</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
         <v>98</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>177</v>
+        <v>210</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>178</v>
+        <v>211</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>7</v>
@@ -6026,19 +6035,19 @@
       <c r="E13" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>98</v>
+    <row r="14" spans="1:7" s="24" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>87</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>167</v>
+        <v>238</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>168</v>
+        <v>241</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>7</v>
@@ -6046,39 +6055,42 @@
       <c r="E14" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>98</v>
+    <row r="15" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>87</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>169</v>
+        <v>111</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>170</v>
+        <v>113</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>98</v>
+      <c r="G15" s="22" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>87</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>126</v>
+        <v>239</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>127</v>
+        <v>212</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>7</v>
@@ -6090,23 +6102,23 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>210</v>
+        <v>179</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>211</v>
+        <v>174</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>118</v>
       </c>
     </row>
@@ -6190,15 +6202,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>7</v>
@@ -6206,22 +6218,22 @@
       <c r="E22" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E23" s="17" t="s">
         <v>22</v>
@@ -6230,74 +6242,114 @@
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="D41" s="22" t="s">
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="D24" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F41" s="22" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D42" s="22" t="s">
+      <c r="E24" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F42" s="22" t="s">
-        <v>117</v>
+      <c r="F24" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" s="22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="D43" s="22" t="s">
+      <c r="D45" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F43" s="22" t="s">
+      <c r="F45" s="22" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="22" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="D44" s="22" t="s">
+      <c r="D46" s="22" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D45" s="22" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D46" s="22" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D47" s="22" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D48" s="22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="22" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A20:A23 A2:A3 A6:A7 A9:A17">
+  <conditionalFormatting sqref="A20:A25 A2:A17">
     <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F23">
+  <conditionalFormatting sqref="F2:F25">
     <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
@@ -6309,14 +6361,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E23" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
-      <formula1>$D$41:$D$48</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E25" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
+      <formula1>$D$43:$D$50</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A23" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
-      <formula1>$A$41:$A$44</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A25" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
+      <formula1>$A$43:$A$46</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F23" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
-      <formula1>$F$41:$F$43</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F25" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
+      <formula1>$F$43:$F$45</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
breakable object prefabs, fixed incorrect breakable wall setups
im mad
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD280C12-9EB2-4020-BF3D-B5E1B43C52AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF94077-DE51-44B9-BF76-268FD6578EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -2014,28 +2014,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R93"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36:L37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.44140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.88671875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="22"/>
-    <col min="5" max="5" width="10.109375" style="22" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="20.44140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="22"/>
+    <col min="5" max="5" width="10.140625" style="22" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="20.42578125" style="22" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" style="22" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" style="22" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" style="22" customWidth="1"/>
-    <col min="13" max="13" width="15.5546875" style="22" customWidth="1"/>
-    <col min="14" max="18" width="11.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.109375" style="22"/>
+    <col min="11" max="11" width="19.7109375" style="22" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="22" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" style="22" customWidth="1"/>
+    <col min="14" max="18" width="11.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>86</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>98</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>98</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>98</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>98</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>98</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>98</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>98</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>98</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>98</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>98</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>98</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>98</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>98</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>98</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>98</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>98</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>98</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>98</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:18" s="24" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>98</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>87</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>87</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>92</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>65</v>
+        <v>154</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>65</v>
@@ -3239,7 +3239,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>87</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>87</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>87</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>87</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:18" s="24" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" s="24" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>87</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:18" s="24" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>87</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:18" s="24" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>87</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="72" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>87</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>87</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:18" s="24" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>87</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>87</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>87</v>
       </c>
@@ -3899,7 +3899,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:18" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>87</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>87</v>
       </c>
@@ -4009,7 +4009,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>87</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>87</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>88</v>
       </c>
@@ -4171,7 +4171,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:18" s="24" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>88</v>
       </c>
@@ -4227,7 +4227,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>88</v>
       </c>
@@ -4281,7 +4281,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>88</v>
       </c>
@@ -4333,7 +4333,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>88</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:18" s="24" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>88</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>88</v>
       </c>
@@ -4497,7 +4497,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>88</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>88</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
         <v>88</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>88</v>
       </c>
@@ -4709,7 +4709,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>88</v>
       </c>
@@ -4763,7 +4763,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
         <v>88</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
         <v>88</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
         <v>89</v>
       </c>
@@ -4925,7 +4925,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
         <v>89</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>89</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>89</v>
       </c>
@@ -5085,7 +5085,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>89</v>
       </c>
@@ -5137,7 +5137,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>89</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
         <v>89</v>
       </c>
@@ -5245,7 +5245,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
         <v>89</v>
       </c>
@@ -5299,7 +5299,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
         <v>89</v>
       </c>
@@ -5353,7 +5353,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>89</v>
       </c>
@@ -5407,7 +5407,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
         <v>89</v>
       </c>
@@ -5461,7 +5461,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>89</v>
       </c>
@@ -5515,7 +5515,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="17" t="s">
         <v>89</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F85" s="22" t="s">
         <v>66</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="22" t="s">
         <v>98</v>
       </c>
@@ -5588,7 +5588,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="22" t="s">
         <v>87</v>
       </c>
@@ -5599,7 +5599,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="22" t="s">
         <v>88</v>
       </c>
@@ -5610,7 +5610,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="22" t="s">
         <v>89</v>
       </c>
@@ -5621,7 +5621,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="F90" s="22" t="s">
         <v>76</v>
       </c>
@@ -5629,7 +5629,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F91" s="22" t="s">
         <v>33</v>
       </c>
@@ -5637,12 +5637,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F92" s="22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F93" s="22" t="s">
         <v>69</v>
       </c>
@@ -5818,22 +5818,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="22"/>
-    <col min="2" max="3" width="48.88671875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="22"/>
+    <col min="2" max="3" width="48.85546875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="21.5546875" style="22" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="22"/>
+    <col min="6" max="6" width="11.28515625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" style="22" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>86</v>
       </c>
@@ -5853,7 +5853,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>98</v>
       </c>
@@ -5873,27 +5873,27 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:6" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="17" t="s">
         <v>320</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="17" t="s">
         <v>321</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F3" s="17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>87</v>
       </c>
@@ -5913,7 +5913,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>87</v>
       </c>
@@ -5933,7 +5933,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>87</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>87</v>
       </c>
@@ -5973,7 +5973,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>87</v>
       </c>
@@ -5993,7 +5993,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="24" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>87</v>
       </c>
@@ -6013,7 +6013,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>87</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>87</v>
       </c>
@@ -6053,7 +6053,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>87</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>88</v>
       </c>
@@ -6093,7 +6093,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="24" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>87</v>
       </c>
@@ -6113,7 +6113,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>88</v>
       </c>
@@ -6133,7 +6133,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>88</v>
       </c>
@@ -6153,7 +6153,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>89</v>
       </c>
@@ -6173,7 +6173,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>98</v>
       </c>
@@ -6193,7 +6193,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>98</v>
       </c>
@@ -6213,7 +6213,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>98</v>
       </c>
@@ -6233,7 +6233,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>98</v>
       </c>
@@ -6253,7 +6253,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>98</v>
       </c>
@@ -6273,7 +6273,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="24" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" s="24" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>87</v>
       </c>
@@ -6293,7 +6293,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>87</v>
       </c>
@@ -6316,7 +6316,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="111.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>87</v>
       </c>
@@ -6336,7 +6336,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>87</v>
       </c>
@@ -6356,7 +6356,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>87</v>
       </c>
@@ -6376,7 +6376,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>87</v>
       </c>
@@ -6396,7 +6396,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>87</v>
       </c>
@@ -6416,7 +6416,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>88</v>
       </c>
@@ -6436,7 +6436,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>88</v>
       </c>
@@ -6456,7 +6456,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>88</v>
       </c>
@@ -6476,7 +6476,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>88</v>
       </c>
@@ -6496,7 +6496,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>88</v>
       </c>
@@ -6516,7 +6516,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
         <v>98</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="22" t="s">
         <v>87</v>
       </c>
@@ -6538,7 +6538,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="22" t="s">
         <v>88</v>
       </c>
@@ -6549,7 +6549,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="s">
         <v>89</v>
       </c>
@@ -6557,22 +6557,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D56" s="22" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D57" s="22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D58" s="22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D59" s="22" t="s">
         <v>69</v>
       </c>
@@ -6617,20 +6617,20 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="9" customWidth="1"/>
-    <col min="4" max="5" width="17.88671875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="10" customWidth="1"/>
-    <col min="7" max="11" width="17.88671875" style="9" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" style="9" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" style="9" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="24.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="9" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="10" customWidth="1"/>
+    <col min="7" max="11" width="17.85546875" style="9" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="9" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="9" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="28" t="s">
         <v>36</v>
@@ -6647,7 +6647,7 @@
       <c r="L1" s="28"/>
       <c r="M1" s="28"/>
     </row>
-    <row r="2" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>85</v>
       </c>
@@ -6688,7 +6688,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="216" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>22</v>
       </c>
@@ -6717,7 +6717,7 @@
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
     </row>
-    <row r="4" spans="1:13" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>18</v>
       </c>
@@ -6746,7 +6746,7 @@
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
     </row>
-    <row r="5" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
@@ -6775,7 +6775,7 @@
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
     </row>
-    <row r="6" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>33</v>
       </c>
@@ -6804,7 +6804,7 @@
       <c r="L6" s="11"/>
       <c r="M6" s="11"/>
     </row>
-    <row r="7" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>76</v>
       </c>
@@ -6833,7 +6833,7 @@
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="1:13" ht="144" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -6862,7 +6862,7 @@
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
     </row>
-    <row r="9" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>7</v>
       </c>
@@ -6891,7 +6891,7 @@
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>69</v>
       </c>
@@ -6920,7 +6920,7 @@
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>66</v>
       </c>
@@ -6966,19 +6966,19 @@
       <selection activeCell="F10" sqref="F10:G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="22"/>
-    <col min="2" max="2" width="38.33203125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="59.88671875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="22" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.44140625" style="22" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="22"/>
+    <col min="2" max="2" width="38.28515625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="59.85546875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" style="22" customWidth="1"/>
     <col min="7" max="7" width="18" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="22"/>
+    <col min="8" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>86</v>
       </c>
@@ -7001,7 +7001,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>98</v>
       </c>
@@ -7024,7 +7024,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>98</v>
       </c>
@@ -7047,7 +7047,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>87</v>
       </c>
@@ -7070,7 +7070,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>87</v>
       </c>
@@ -7093,7 +7093,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>87</v>
       </c>
@@ -7116,7 +7116,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>87</v>
       </c>
@@ -7139,7 +7139,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>98</v>
       </c>
@@ -7150,7 +7150,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>87</v>
       </c>
@@ -7161,7 +7161,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>88</v>
       </c>
@@ -7169,7 +7169,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>89</v>
       </c>
@@ -7224,19 +7224,19 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="22"/>
-    <col min="2" max="2" width="38.33203125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="59.88671875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="22" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.44140625" style="22" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="22"/>
+    <col min="2" max="2" width="38.28515625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="59.85546875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" style="22" customWidth="1"/>
     <col min="7" max="7" width="18" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="22"/>
+    <col min="8" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>86</v>
       </c>
@@ -7259,7 +7259,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>98</v>
       </c>
@@ -7282,7 +7282,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>87</v>
       </c>
@@ -7305,7 +7305,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>87</v>
       </c>
@@ -7313,7 +7313,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>87</v>
       </c>
@@ -7324,7 +7324,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>87</v>
       </c>
@@ -7332,7 +7332,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>87</v>
       </c>
@@ -7340,7 +7340,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>98</v>
       </c>
@@ -7351,7 +7351,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>87</v>
       </c>
@@ -7362,7 +7362,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>88</v>
       </c>
@@ -7370,7 +7370,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>89</v>
       </c>
@@ -7415,12 +7415,12 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="28" t="s">
         <v>36</v>
@@ -7437,7 +7437,7 @@
       <c r="L1" s="28"/>
       <c r="M1" s="28"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -7478,7 +7478,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>50</v>
       </c>
@@ -7495,7 +7495,7 @@
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>51</v>
       </c>
@@ -7512,7 +7512,7 @@
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>52</v>
       </c>
@@ -7529,7 +7529,7 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>53</v>
       </c>
@@ -7546,7 +7546,7 @@
       <c r="L6" s="29"/>
       <c r="M6" s="29"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>54</v>
       </c>
@@ -7563,7 +7563,7 @@
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>55</v>
       </c>
@@ -7580,7 +7580,7 @@
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>56</v>
       </c>
@@ -7597,7 +7597,7 @@
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>57</v>
       </c>
@@ -7614,7 +7614,7 @@
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>58</v>
       </c>
@@ -7631,7 +7631,7 @@
       <c r="L11" s="29"/>
       <c r="M11" s="29"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>59</v>
       </c>
@@ -7648,7 +7648,7 @@
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>60</v>
       </c>
@@ -7665,7 +7665,7 @@
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>61</v>
       </c>
@@ -7682,7 +7682,7 @@
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>62</v>
       </c>
@@ -7699,7 +7699,7 @@
       <c r="L15" s="29"/>
       <c r="M15" s="29"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>63</v>
       </c>
@@ -7716,7 +7716,7 @@
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
levers are now crank and forget
no longer need to require holding them after cranking
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF94077-DE51-44B9-BF76-268FD6578EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AAACDC-CB48-4E00-A209-C6D643C3405F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -2014,7 +2014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
@@ -5818,8 +5818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6033,24 +6033,24 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:6" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="17" t="s">
         <v>314</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="17" t="s">
         <v>325</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>117</v>
+      <c r="F11" s="17" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update prod doc with some of the bugs from 23-09-2022 playtest
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AAACDC-CB48-4E00-A209-C6D643C3405F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F390A6BD-C1ED-480F-9CBD-112B88A030CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="335">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -886,9 +886,6 @@
     <t>Make the fire more realistic</t>
   </si>
   <si>
-    <t>Puppets not returning to grid after death</t>
-  </si>
-  <si>
     <t>Test Item</t>
   </si>
   <si>
@@ -1069,9 +1066,6 @@
     <t>?</t>
   </si>
   <si>
-    <t>Puppets maintaining position when respawning</t>
-  </si>
-  <si>
     <t>Level select button raycasting completely cooked</t>
   </si>
   <si>
@@ -1084,9 +1078,6 @@
     <t>Pressing jump while holding onto string makes you go around the world</t>
   </si>
   <si>
-    <t>Seems to happen if input controls are held down while respawning</t>
-  </si>
-  <si>
     <t>Make levers one shot</t>
   </si>
   <si>
@@ -1102,9 +1093,6 @@
     <t>Untagling arrow gets difficult to see when raised cause its 2D</t>
   </si>
   <si>
-    <t>Pperhaps tilt it forward a few degrees</t>
-  </si>
-  <si>
     <t>Collider not being deleted after breakable prop is broken</t>
   </si>
   <si>
@@ -1132,10 +1120,34 @@
     <t>Enable the gravity so the boxes can fall into water and down cliffs. Make them kinematic so that bumping into them moves them a  little, helps with soft lock boxes blocking ledges and shit</t>
   </si>
   <si>
-    <t>Slingshotting walls need to be more breakable</t>
-  </si>
-  <si>
-    <t>Specifically 2:2, the wall refuses to break</t>
+    <t>Insides of broken walls are yellow</t>
+  </si>
+  <si>
+    <t>I can't believe Spongebob is fucking dead</t>
+  </si>
+  <si>
+    <t>Act 2 Scene 2 breakable wall isn't breakable</t>
+  </si>
+  <si>
+    <t>I think it's something to do with BreakableProp.cs angle calculation, as it's the only wall placed horizontally in the game. All the others are vertical and work fine.</t>
+  </si>
+  <si>
+    <t>Puppets position is not correctly set on respawn</t>
+  </si>
+  <si>
+    <t>Curtain doesn't close completely on Act Change</t>
+  </si>
+  <si>
+    <t>I'll make the cloth physics more weighty so they close properly.</t>
+  </si>
+  <si>
+    <t>End of Game prevents switching to previous levels</t>
+  </si>
+  <si>
+    <t>Just gotta add support for it in the state machine and we're juicy yfeel me</t>
+  </si>
+  <si>
+    <t>Pperhaps tilt it forward a few degrees, or make it a little pop-up like the contextual tutorials.</t>
   </si>
 </sst>
 </file>
@@ -2204,7 +2216,7 @@
         <v>98</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>207</v>
@@ -2260,10 +2272,10 @@
         <v>98</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>296</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>297</v>
       </c>
       <c r="D5" s="19">
         <v>4</v>
@@ -2314,10 +2326,10 @@
         <v>98</v>
       </c>
       <c r="B6" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>298</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>299</v>
       </c>
       <c r="D6" s="19">
         <v>4</v>
@@ -3190,10 +3202,10 @@
         <v>87</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>287</v>
       </c>
       <c r="D22" s="1">
         <v>4</v>
@@ -4822,10 +4834,10 @@
         <v>88</v>
       </c>
       <c r="B52" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="C52" s="17" t="s">
         <v>290</v>
-      </c>
-      <c r="C52" s="17" t="s">
-        <v>291</v>
       </c>
       <c r="D52" s="17">
         <v>2</v>
@@ -5361,7 +5373,7 @@
         <v>218</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D62" s="1">
         <v>2</v>
@@ -5816,10 +5828,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5858,10 +5870,10 @@
         <v>98</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -5873,44 +5885,44 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>320</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>321</v>
-      </c>
-      <c r="D3" s="17" t="s">
+      <c r="B3" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>316</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>317</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="17" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -5918,16 +5930,16 @@
         <v>87</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>116</v>
@@ -5938,10 +5950,10 @@
         <v>87</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>247</v>
+        <v>329</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
@@ -5958,19 +5970,19 @@
         <v>87</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -5978,10 +5990,10 @@
         <v>87</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>7</v>
@@ -5998,10 +6010,10 @@
         <v>87</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>7</v>
@@ -6013,78 +6025,78 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:6" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>314</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>325</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>309</v>
+        <v>119</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>310</v>
+        <v>120</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>119</v>
+        <v>287</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>120</v>
+        <v>288</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>22</v>
@@ -6093,15 +6105,15 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>22</v>
@@ -6113,115 +6125,115 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>293</v>
+        <v>332</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>292</v>
+        <v>333</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>224</v>
+        <v>325</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>223</v>
+        <v>326</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>318</v>
+        <v>224</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>319</v>
+        <v>223</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D18" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>18</v>
+      <c r="E19" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>7</v>
@@ -6238,10 +6250,10 @@
         <v>98</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>126</v>
+        <v>167</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>127</v>
+        <v>168</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>7</v>
@@ -6253,15 +6265,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
+    <row r="22" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>210</v>
+        <v>169</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>211</v>
+        <v>170</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>7</v>
@@ -6269,19 +6281,19 @@
       <c r="E22" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F22" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="24" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
-        <v>87</v>
+    <row r="23" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>238</v>
+        <v>126</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>241</v>
+        <v>127</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>7</v>
@@ -6289,42 +6301,39 @@
       <c r="E23" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="F23" s="1" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>111</v>
+        <v>210</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>113</v>
+        <v>211</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="G24" s="22" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:7" s="24" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>212</v>
+        <v>241</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>7</v>
@@ -6332,19 +6341,19 @@
       <c r="E25" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>179</v>
+        <v>111</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>174</v>
+        <v>113</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>7</v>
@@ -6355,16 +6364,19 @@
       <c r="F26" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G26" s="22" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>157</v>
+        <v>239</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>158</v>
+        <v>212</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>7</v>
@@ -6376,35 +6388,35 @@
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>205</v>
+        <v>157</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>206</v>
+        <v>158</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>7</v>
@@ -6412,39 +6424,39 @@
       <c r="E29" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F29" s="17" t="s">
+      <c r="F29" s="1" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>220</v>
+        <v>162</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>242</v>
+        <v>206</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>7</v>
@@ -6456,35 +6468,35 @@
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>172</v>
+        <v>219</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>7</v>
@@ -6492,22 +6504,22 @@
       <c r="E33" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E34" s="17" t="s">
         <v>22</v>
@@ -6516,74 +6528,114 @@
         <v>118</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="D52" s="22" t="s">
+    <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="D35" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F52" s="22" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D53" s="22" t="s">
+      <c r="E35" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F53" s="22" t="s">
-        <v>117</v>
+      <c r="F35" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D54" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" s="22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D55" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F55" s="22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="D54" s="22" t="s">
+      <c r="D56" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F54" s="22" t="s">
+      <c r="F56" s="22" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="22" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="D55" s="22" t="s">
+      <c r="D57" s="22" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D56" s="22" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D57" s="22" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D58" s="22" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D59" s="22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D60" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D61" s="22" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A29:A34 A2:A26">
+  <conditionalFormatting sqref="A31:A36 A2:A28">
     <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F34">
+  <conditionalFormatting sqref="F2:F36">
     <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
@@ -6595,14 +6647,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E34" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
-      <formula1>$D$52:$D$59</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E36" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
+      <formula1>$D$54:$D$61</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A34" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
-      <formula1>$A$52:$A$55</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A36" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
+      <formula1>$A$54:$A$57</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F34" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
-      <formula1>$F$52:$F$54</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F36" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
+      <formula1>$F$54:$F$56</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6708,7 +6760,7 @@
         <v>234</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
@@ -6737,7 +6789,7 @@
         <v>231</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
@@ -6766,7 +6818,7 @@
         <v>230</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
@@ -6795,7 +6847,7 @@
         <v>226</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
@@ -6824,7 +6876,7 @@
         <v>229</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
@@ -6853,7 +6905,7 @@
         <v>232</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
@@ -6882,7 +6934,7 @@
         <v>233</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
@@ -6911,7 +6963,7 @@
         <v>228</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
@@ -6983,19 +7035,19 @@
         <v>86</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C1" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>262</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>252</v>
-      </c>
       <c r="F1" s="20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G1" s="20" t="s">
         <v>115</v>
@@ -7006,22 +7058,22 @@
         <v>98</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7029,22 +7081,22 @@
         <v>98</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>266</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7052,22 +7104,22 @@
         <v>87</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7075,22 +7127,22 @@
         <v>87</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7098,22 +7150,22 @@
         <v>87</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7121,22 +7173,22 @@
         <v>87</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>277</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -7144,10 +7196,10 @@
         <v>98</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G22" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -7155,10 +7207,10 @@
         <v>87</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G23" s="22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -7166,7 +7218,7 @@
         <v>88</v>
       </c>
       <c r="G24" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -7241,19 +7293,19 @@
         <v>86</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C1" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>262</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>252</v>
-      </c>
       <c r="F1" s="20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G1" s="20" t="s">
         <v>115</v>
@@ -7264,22 +7316,22 @@
         <v>98</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>269</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7287,22 +7339,22 @@
         <v>87</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>272</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -7310,7 +7362,7 @@
         <v>87</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -7318,10 +7370,10 @@
         <v>87</v>
       </c>
       <c r="B5" s="22" t="s">
+        <v>283</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>284</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7329,7 +7381,7 @@
         <v>87</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -7337,7 +7389,7 @@
         <v>87</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -7345,10 +7397,10 @@
         <v>98</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -7356,10 +7408,10 @@
         <v>87</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G21" s="22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -7367,7 +7419,7 @@
         <v>88</v>
       </c>
       <c r="G22" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix insides of broken walls being yellow
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F390A6BD-C1ED-480F-9CBD-112B88A030CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7321A0-3E58-4D31-BBF8-1ADEF1F76289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
@@ -5831,7 +5831,7 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6145,7 +6145,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>88</v>
       </c>
@@ -6162,7 +6162,7 @@
         <v>18</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix softlock at end of game, now opens level select
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7321A0-3E58-4D31-BBF8-1ADEF1F76289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E7E19E-2FE3-4850-9379-BA370A1A5AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
@@ -5830,8 +5830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5962,7 +5962,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -6142,7 +6142,7 @@
         <v>18</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
eased required angle to break walls
from 45 degrees to 75 degrees. level 2-2 wall should break much more consistently!
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E7E19E-2FE3-4850-9379-BA370A1A5AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FB8BCB-657D-43F5-BFD9-00F8DC42BB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="336">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -1148,6 +1148,9 @@
   </si>
   <si>
     <t>Pperhaps tilt it forward a few degrees, or make it a little pop-up like the contextual tutorials.</t>
+  </si>
+  <si>
+    <t>Requires some testing</t>
   </si>
 </sst>
 </file>
@@ -5831,7 +5834,7 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5845,7 +5848,7 @@
     <col min="8" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>86</v>
       </c>
@@ -5865,7 +5868,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>98</v>
       </c>
@@ -5885,7 +5888,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>98</v>
       </c>
@@ -5902,10 +5905,13 @@
         <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>98</v>
       </c>
@@ -5925,7 +5931,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>87</v>
       </c>
@@ -5945,7 +5951,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>87</v>
       </c>
@@ -5965,7 +5971,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>87</v>
       </c>
@@ -5985,7 +5991,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>87</v>
       </c>
@@ -6005,7 +6011,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>87</v>
       </c>
@@ -6025,7 +6031,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>87</v>
       </c>
@@ -6045,7 +6051,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>87</v>
       </c>
@@ -6065,7 +6071,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>88</v>
       </c>
@@ -6085,7 +6091,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>87</v>
       </c>
@@ -6105,7 +6111,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>88</v>
       </c>
@@ -6125,7 +6131,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>88</v>
       </c>
@@ -6145,7 +6151,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
wall fragments shrink after breakage
much less chance of getting in the way of visibility and movement
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FB8BCB-657D-43F5-BFD9-00F8DC42BB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CA8246-B238-4F80-AF14-592D6097E565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="337">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -1151,6 +1151,9 @@
   </si>
   <si>
     <t>Requires some testing</t>
+  </si>
+  <si>
+    <t>Shards of broken walls can get in the way of visibility and movement</t>
   </si>
 </sst>
 </file>
@@ -5831,10 +5834,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6111,55 +6114,53 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>291</v>
-      </c>
+        <v>336</v>
+      </c>
+      <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>332</v>
+        <v>292</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>333</v>
+        <v>291</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>69</v>
@@ -6171,95 +6172,95 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>7</v>
@@ -6271,15 +6272,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>7</v>
@@ -6291,15 +6292,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>126</v>
+        <v>169</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>127</v>
+        <v>170</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>7</v>
@@ -6312,14 +6313,14 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>210</v>
+        <v>126</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>211</v>
+        <v>127</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>7</v>
@@ -6327,19 +6328,19 @@
       <c r="E24" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F24" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="24" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>241</v>
+        <v>211</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>7</v>
@@ -6351,104 +6352,104 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="24" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>111</v>
+        <v>238</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>113</v>
+        <v>241</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="G26" s="22" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>239</v>
+        <v>111</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>212</v>
+        <v>113</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G27" s="22" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>179</v>
+        <v>239</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>118</v>
@@ -6459,30 +6460,30 @@
         <v>87</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>205</v>
+        <v>162</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>206</v>
+        <v>163</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F31" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>7</v>
@@ -6490,19 +6491,19 @@
       <c r="E32" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F32" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>7</v>
@@ -6510,138 +6511,158 @@
       <c r="E33" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F33" s="17" t="s">
+      <c r="F33" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>172</v>
+        <v>242</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>221</v>
+        <v>180</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>222</v>
+        <v>172</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>181</v>
+        <v>221</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>182</v>
+        <v>222</v>
       </c>
       <c r="D36" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="22" t="s">
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="D54" s="22" t="s">
+      <c r="D55" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F54" s="22" t="s">
+      <c r="F55" s="22" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="22" t="s">
+    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D55" s="22" t="s">
+      <c r="D56" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="F55" s="22" t="s">
+      <c r="F56" s="22" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D56" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F56" s="22" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D57" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F57" s="22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="D57" s="22" t="s">
+      <c r="D58" s="22" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D58" s="22" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D59" s="22" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D60" s="22" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D61" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D62" s="22" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A31:A36 A2:A28">
+  <conditionalFormatting sqref="A32:A37 A2:A29">
     <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F36">
+  <conditionalFormatting sqref="F2:F37">
     <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
@@ -6653,14 +6674,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E36" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
-      <formula1>$D$54:$D$61</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E37" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
+      <formula1>$D$55:$D$62</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A36" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
-      <formula1>$A$54:$A$57</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A37" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
+      <formula1>$A$55:$A$58</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F36" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
-      <formula1>$F$54:$F$56</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F37" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
+      <formula1>$F$55:$F$57</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed raycasting bug for level select UI
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BECFE23-3754-489A-B67B-0BA57E275F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3EB0A6-99B5-478D-A9A8-46D9546B67B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="339">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -1144,9 +1144,6 @@
     <t>End of Game prevents switching to previous levels</t>
   </si>
   <si>
-    <t>Just gotta add support for it in the state machine and we're juicy yfeel me</t>
-  </si>
-  <si>
     <t>Pperhaps tilt it forward a few degrees, or make it a little pop-up like the contextual tutorials.</t>
   </si>
   <si>
@@ -1154,6 +1151,15 @@
   </si>
   <si>
     <t>Shards of broken walls can get in the way of visibility and movement</t>
+  </si>
+  <si>
+    <t>Just gotta add support for it in the state machine and we're juicy you feel me</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soft lock between books and chest of drawers </t>
+  </si>
+  <si>
+    <t>Level 2:1, leaves puppet in permanent fall state, books need to be moved slightly</t>
   </si>
 </sst>
 </file>
@@ -2032,8 +2038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R93"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5834,10 +5840,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5891,7 +5897,7 @@
         <v>118</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -5914,7 +5920,7 @@
         <v>118</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -5957,38 +5963,38 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>329</v>
+        <v>337</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>314</v>
+        <v>338</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>18</v>
@@ -5997,35 +6003,35 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>312</v>
+        <v>323</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>313</v>
+        <v>324</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>7</v>
@@ -6037,78 +6043,78 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+    <row r="10" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>311</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C11" s="17" t="s">
         <v>321</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D11" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E11" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F11" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>287</v>
+        <v>119</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>288</v>
+        <v>120</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>22</v>
@@ -6117,73 +6123,73 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="C14" s="1"/>
+        <v>287</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>288</v>
+      </c>
       <c r="D14" s="1" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>291</v>
-      </c>
+        <v>335</v>
+      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>332</v>
+        <v>292</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>333</v>
+        <v>291</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>69</v>
@@ -6195,95 +6201,95 @@
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>224</v>
+        <v>325</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>223</v>
+        <v>326</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>330</v>
+        <v>224</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>331</v>
+        <v>223</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="C21" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>7</v>
@@ -6295,15 +6301,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>7</v>
@@ -6315,15 +6321,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>126</v>
+        <v>169</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>127</v>
+        <v>170</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>7</v>
@@ -6336,14 +6342,14 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>210</v>
+        <v>126</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>211</v>
+        <v>127</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>7</v>
@@ -6351,19 +6357,19 @@
       <c r="E25" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="F25" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="24" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>241</v>
+        <v>211</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>7</v>
@@ -6375,104 +6381,104 @@
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" s="24" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>111</v>
+        <v>238</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>113</v>
+        <v>241</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="G27" s="22" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>239</v>
+        <v>111</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>212</v>
+        <v>113</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G28" s="22" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>179</v>
+        <v>239</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>118</v>
@@ -6483,30 +6489,30 @@
         <v>87</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>205</v>
+        <v>162</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>206</v>
+        <v>163</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F32" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>7</v>
@@ -6514,19 +6520,19 @@
       <c r="E33" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
       <c r="D34" s="17" t="s">
         <v>7</v>
@@ -6534,138 +6540,158 @@
       <c r="E34" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F34" s="17" t="s">
+      <c r="F34" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>172</v>
+        <v>242</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>221</v>
+        <v>180</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>222</v>
+        <v>172</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>181</v>
+        <v>221</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>182</v>
+        <v>222</v>
       </c>
       <c r="D37" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="22" t="s">
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="D55" s="22" t="s">
+      <c r="D56" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F55" s="22" t="s">
+      <c r="F56" s="22" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="22" t="s">
+    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D56" s="22" t="s">
+      <c r="D57" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="F56" s="22" t="s">
+      <c r="F57" s="22" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D57" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F57" s="22" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D58" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F58" s="22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="D58" s="22" t="s">
+      <c r="D59" s="22" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D59" s="22" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D60" s="22" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D61" s="22" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D62" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D63" s="22" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A32:A37 A2:A29">
+  <conditionalFormatting sqref="A33:A38 A2:A30">
     <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F37">
+  <conditionalFormatting sqref="F2:F38">
     <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
@@ -6677,14 +6703,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E37" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
-      <formula1>$D$55:$D$62</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E38" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
+      <formula1>$D$56:$D$63</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A37" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
-      <formula1>$A$55:$A$58</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A38" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
+      <formula1>$A$56:$A$59</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F37" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
-      <formula1>$F$55:$F$57</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F38" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
+      <formula1>$F$56:$F$58</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
prod doc bug tracking update
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Tim\Desktop\Git\strung-along-again\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACC6E97-54F6-4EC7-BBF5-706FC0BE8D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667AED8D-DB18-44D5-A31D-54F65594BF8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="344">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -1169,6 +1169,12 @@
   </si>
   <si>
     <t>Prevents soft lock, especially in the case where both levers are supposed to be pulled at the same time.</t>
+  </si>
+  <si>
+    <t>Pulling the levers makes the hooks wiggle before going to their intended position</t>
+  </si>
+  <si>
+    <t>Uhhh, so when I pull the level the hook wiggles for a while before moving, and you can't like, move it only a little bit anymore, it does it with all the levels in the stage scene</t>
   </si>
 </sst>
 </file>
@@ -1418,14 +1424,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2047,8 +2053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2217,7 +2223,7 @@
         <v>93</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>65</v>
@@ -5985,10 +5991,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6041,7 +6047,7 @@
       <c r="F2" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="27" t="s">
         <v>334</v>
       </c>
     </row>
@@ -6064,7 +6070,7 @@
       <c r="F3" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="27" t="s">
         <v>334</v>
       </c>
     </row>
@@ -6168,7 +6174,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>87</v>
       </c>
@@ -6185,7 +6191,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6202,10 +6208,10 @@
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -6248,38 +6254,38 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>119</v>
+        <v>342</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>120</v>
+        <v>343</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>287</v>
+        <v>119</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>288</v>
+        <v>120</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>22</v>
@@ -6288,73 +6294,73 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+    <row r="15" spans="1:7" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B16" s="17" t="s">
         <v>335</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17" t="s">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E16" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F16" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>332</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>336</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>69</v>
@@ -6366,95 +6372,95 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>325</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>326</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+    <row r="21" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B21" s="17" t="s">
         <v>330</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C21" s="17" t="s">
         <v>331</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D21" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E21" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F21" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>18</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>7</v>
@@ -6466,15 +6472,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>7</v>
@@ -6486,15 +6492,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>126</v>
+        <v>169</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>127</v>
+        <v>170</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>7</v>
@@ -6507,14 +6513,14 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>210</v>
+        <v>126</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>211</v>
+        <v>127</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>7</v>
@@ -6522,19 +6528,19 @@
       <c r="E26" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="24" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>241</v>
+        <v>211</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>7</v>
@@ -6546,104 +6552,104 @@
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" s="24" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>111</v>
+        <v>238</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>113</v>
+        <v>241</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="G28" s="22" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>239</v>
+        <v>111</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>212</v>
+        <v>113</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G29" s="22" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>179</v>
+        <v>239</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>118</v>
@@ -6654,30 +6660,30 @@
         <v>87</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>205</v>
+        <v>162</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>206</v>
+        <v>163</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F33" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="D34" s="17" t="s">
         <v>7</v>
@@ -6685,19 +6691,19 @@
       <c r="E34" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F34" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
       <c r="D35" s="17" t="s">
         <v>7</v>
@@ -6705,138 +6711,158 @@
       <c r="E35" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F35" s="17" t="s">
+      <c r="F35" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>172</v>
+        <v>242</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>221</v>
+        <v>180</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>222</v>
+        <v>172</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>181</v>
+        <v>221</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>182</v>
+        <v>222</v>
       </c>
       <c r="D38" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="22" t="s">
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="D56" s="22" t="s">
+      <c r="D57" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F56" s="22" t="s">
+      <c r="F57" s="22" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="22" t="s">
+    <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D57" s="22" t="s">
+      <c r="D58" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="F57" s="22" t="s">
+      <c r="F58" s="22" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F58" s="22" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F59" s="22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="D59" s="22" t="s">
+      <c r="D60" s="22" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D60" s="22" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D61" s="22" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D62" s="22" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D63" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D64" s="22" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A33:A38 A2:A30">
+  <conditionalFormatting sqref="A34:A39 A2:A31">
     <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F38">
+  <conditionalFormatting sqref="F2:F39">
     <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
@@ -6848,14 +6874,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E38" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
-      <formula1>$D$56:$D$63</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E39" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
+      <formula1>$D$57:$D$64</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A38" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
-      <formula1>$A$56:$A$59</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A39" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
+      <formula1>$A$57:$A$60</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F38" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
-      <formula1>$F$56:$F$58</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F39" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
+      <formula1>$F$57:$F$59</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6886,20 +6912,20 @@
   <sheetData>
     <row r="1" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
     </row>
     <row r="2" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -7676,20 +7702,20 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -7733,21 +7759,21 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -7784,21 +7810,21 @@
       <c r="M5" s="7"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -7869,21 +7895,21 @@
       <c r="M10" s="6"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -7937,21 +7963,21 @@
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">

</xml_diff>

<commit_message>
Prefab change for strings
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Tim\Desktop\Git\strung-along-again\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667AED8D-DB18-44D5-A31D-54F65594BF8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE01EA9-CAFF-418F-86BE-9800E506A58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="342">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -1169,12 +1169,6 @@
   </si>
   <si>
     <t>Prevents soft lock, especially in the case where both levers are supposed to be pulled at the same time.</t>
-  </si>
-  <si>
-    <t>Pulling the levers makes the hooks wiggle before going to their intended position</t>
-  </si>
-  <si>
-    <t>Uhhh, so when I pull the level the hook wiggles for a while before moving, and you can't like, move it only a little bit anymore, it does it with all the levels in the stage scene</t>
   </si>
 </sst>
 </file>
@@ -5991,10 +5985,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6254,113 +6248,113 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>342</v>
+        <v>119</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>343</v>
+        <v>120</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>119</v>
+        <v>287</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>120</v>
+        <v>288</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>335</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+    <row r="17" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>335</v>
-      </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17" t="s">
+      <c r="B17" s="17" t="s">
+        <v>332</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>336</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E17" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F17" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>69</v>
@@ -6372,95 +6366,95 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>325</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>326</v>
-      </c>
-      <c r="D19" s="17" t="s">
+    <row r="19" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>331</v>
+      </c>
+      <c r="D20" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E20" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F20" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="B21" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>330</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>331</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="F22" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>7</v>
@@ -6472,15 +6466,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>7</v>
@@ -6492,15 +6486,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>169</v>
+        <v>126</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>170</v>
+        <v>127</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>7</v>
@@ -6513,14 +6507,14 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="17" t="s">
         <v>98</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>126</v>
+        <v>210</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>127</v>
+        <v>211</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>7</v>
@@ -6528,19 +6522,19 @@
       <c r="E26" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" s="24" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>210</v>
+        <v>238</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>211</v>
+        <v>241</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>7</v>
@@ -6552,104 +6546,104 @@
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="24" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>238</v>
+        <v>111</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>241</v>
+        <v>113</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G28" s="22" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>111</v>
+        <v>239</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>113</v>
+        <v>212</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G29" s="22" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>239</v>
+        <v>179</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>212</v>
+        <v>174</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>118</v>
@@ -6660,30 +6654,30 @@
         <v>87</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>162</v>
+        <v>205</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>163</v>
+        <v>206</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="17" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="D34" s="17" t="s">
         <v>7</v>
@@ -6691,19 +6685,19 @@
       <c r="E34" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F34" s="17" t="s">
+      <c r="F34" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>219</v>
+        <v>242</v>
       </c>
       <c r="D35" s="17" t="s">
         <v>7</v>
@@ -6711,158 +6705,138 @@
       <c r="E35" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F35" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>240</v>
+        <v>180</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>242</v>
+        <v>172</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F36" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>180</v>
+        <v>221</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>172</v>
+        <v>222</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>221</v>
+        <v>181</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>222</v>
+        <v>182</v>
       </c>
       <c r="D38" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D56" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" s="22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D57" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F57" s="22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="B39" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="17" t="s">
+      <c r="D58" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F58" s="22" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="D57" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="F57" s="22" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F58" s="22" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="22" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F59" s="22" t="s">
-        <v>118</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="22" t="s">
-        <v>89</v>
-      </c>
       <c r="D60" s="22" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D61" s="22" t="s">
-        <v>76</v>
+        <v>33</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D62" s="22" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D63" s="22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D64" s="22" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A34:A39 A2:A31">
+  <conditionalFormatting sqref="A33:A38 A2:A30">
     <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F39">
+  <conditionalFormatting sqref="F2:F38">
     <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
@@ -6874,14 +6848,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E39" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
-      <formula1>$D$57:$D$64</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E38" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
+      <formula1>$D$56:$D$63</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A39" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
-      <formula1>$A$57:$A$60</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A38" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
+      <formula1>$A$56:$A$59</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F39" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
-      <formula1>$F$57:$F$59</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F38" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
+      <formula1>$F$56:$F$58</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Found some bugs, updated prod doc
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB60D63C-D008-4A7E-ABC1-6469FCA8E42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF136A7-F2DC-4375-9BF3-5FB9DB788000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11235" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1532" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="346">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -463,9 +463,6 @@
     <t>Create Act 3 level 3</t>
   </si>
   <si>
-    <t>Levels are to demonstrate more complexity, also requiring final capabilities</t>
-  </si>
-  <si>
     <t>Do as said</t>
   </si>
   <si>
@@ -1166,6 +1163,24 @@
   </si>
   <si>
     <t>Replace anchor point placeholder models with completed ones</t>
+  </si>
+  <si>
+    <t>Grid ded</t>
+  </si>
+  <si>
+    <t>First level can be beaten by just walking along ground</t>
+  </si>
+  <si>
+    <t>Shorten strings, otherwise I prefer it without hazards, it's nice</t>
+  </si>
+  <si>
+    <t>Level 2:2 has a strange issue where you can beat the level by doing a cheeky string extension on player 1</t>
+  </si>
+  <si>
+    <t>Underlying issue here is that you can move further than your normal string radius after you tangle. Not sure if this is localised to 1 level or a fundamnetal problem, but worth a look for sure</t>
+  </si>
+  <si>
+    <t>Assets need to be placed</t>
   </si>
 </sst>
 </file>
@@ -1335,7 +1350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1413,9 +1428,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2084,8 +2096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="C55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N64" sqref="N64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2166,15 +2178,17 @@
         <v>98</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>336</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>337</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>338</v>
       </c>
       <c r="D2" s="17">
         <v>2</v>
       </c>
-      <c r="E2" s="17"/>
+      <c r="E2" s="17">
+        <v>1.5</v>
+      </c>
       <c r="F2" s="17" t="s">
         <v>18</v>
       </c>
@@ -2220,10 +2234,10 @@
         <v>98</v>
       </c>
       <c r="B3" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>235</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>236</v>
       </c>
       <c r="D3" s="17">
         <v>5</v>
@@ -2276,15 +2290,17 @@
         <v>98</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D4" s="17">
         <v>10</v>
       </c>
-      <c r="E4" s="17"/>
+      <c r="E4" s="17">
+        <v>8.5</v>
+      </c>
       <c r="F4" s="17" t="s">
         <v>22</v>
       </c>
@@ -2330,10 +2346,10 @@
         <v>98</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D5" s="17">
         <v>4</v>
@@ -2413,10 +2429,10 @@
         <v>92</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>94</v>
@@ -2469,10 +2485,10 @@
         <v>92</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>94</v>
@@ -2525,10 +2541,10 @@
         <v>92</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>94</v>
@@ -2557,7 +2573,7 @@
         <v>103</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>106</v>
+        <v>345</v>
       </c>
       <c r="D9" s="1">
         <v>4</v>
@@ -2611,7 +2627,7 @@
         <v>104</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>106</v>
+        <v>345</v>
       </c>
       <c r="D10" s="1">
         <v>4</v>
@@ -2665,7 +2681,7 @@
         <v>105</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>106</v>
+        <v>345</v>
       </c>
       <c r="D11" s="1">
         <v>4</v>
@@ -2716,10 +2732,10 @@
         <v>98</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12" s="17">
         <v>4</v>
@@ -2743,10 +2759,10 @@
         <v>92</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>94</v>
@@ -2772,10 +2788,10 @@
         <v>98</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D13" s="17">
         <v>3</v>
@@ -2796,10 +2812,10 @@
         <v>92</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>94</v>
@@ -2828,10 +2844,10 @@
         <v>98</v>
       </c>
       <c r="B14" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>140</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>141</v>
       </c>
       <c r="D14" s="17">
         <v>8</v>
@@ -2884,7 +2900,7 @@
         <v>98</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17">
@@ -2938,10 +2954,10 @@
         <v>98</v>
       </c>
       <c r="B16" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>144</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>145</v>
       </c>
       <c r="D16" s="17">
         <v>1</v>
@@ -2959,7 +2975,7 @@
         <v>91</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J16" s="17" t="s">
         <v>94</v>
@@ -2994,7 +3010,7 @@
         <v>98</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17">
@@ -3048,10 +3064,10 @@
         <v>98</v>
       </c>
       <c r="B18" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>142</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>143</v>
       </c>
       <c r="D18" s="17">
         <v>6</v>
@@ -3072,7 +3088,7 @@
         <v>92</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>94</v>
@@ -3107,7 +3123,7 @@
         <v>27</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D19" s="17">
         <v>5</v>
@@ -3125,7 +3141,7 @@
         <v>92</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J19" s="17" t="s">
         <v>94</v>
@@ -3160,10 +3176,10 @@
         <v>87</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D20" s="19">
         <v>4</v>
@@ -3210,36 +3226,38 @@
       </c>
     </row>
     <row r="21" spans="1:18" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>340</v>
-      </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19">
+      <c r="B21" s="17" t="s">
+        <v>339</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17">
         <v>1</v>
       </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19" t="s">
+      <c r="E21" s="17">
+        <v>1</v>
+      </c>
+      <c r="F21" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="H21" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="I21" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="J21" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="K21" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="L21" s="19" t="s">
+      <c r="G21" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="K21" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="L21" s="17" t="s">
         <v>91</v>
       </c>
       <c r="M21" s="1" t="s">
@@ -3248,16 +3266,16 @@
       <c r="N21" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="O21" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="R21" s="1" t="s">
+      <c r="O21" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="P21" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q21" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="R21" s="17" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3266,10 +3284,10 @@
         <v>87</v>
       </c>
       <c r="B22" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>213</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>214</v>
       </c>
       <c r="D22" s="17">
         <v>3</v>
@@ -3293,27 +3311,27 @@
         <v>92</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="R22" s="1" t="s">
+      <c r="M22" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="N22" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="O22" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="P22" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q22" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="R22" s="17" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3322,10 +3340,10 @@
         <v>87</v>
       </c>
       <c r="B23" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="C23" s="17" t="s">
         <v>285</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>286</v>
       </c>
       <c r="D23" s="17">
         <v>4</v>
@@ -3353,7 +3371,7 @@
         <v>92</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>94</v>
@@ -3372,58 +3390,58 @@
       </c>
     </row>
     <row r="24" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D24" s="1">
+      <c r="B24" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="D24" s="17">
         <v>1</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="17">
         <v>1</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I24" s="1" t="s">
+      <c r="G24" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="I24" s="17" t="s">
         <v>91</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="R24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N24" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="O24" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="P24" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q24" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="R24" s="17" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3432,10 +3450,10 @@
         <v>87</v>
       </c>
       <c r="B25" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="C25" s="17" t="s">
         <v>187</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>188</v>
       </c>
       <c r="D25" s="17">
         <v>1</v>
@@ -3456,7 +3474,7 @@
         <v>91</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>94</v>
@@ -3484,56 +3502,58 @@
       </c>
     </row>
     <row r="26" spans="1:18" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D26" s="1">
+      <c r="B26" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="D26" s="17">
         <v>5</v>
       </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1" t="s">
+      <c r="E26" s="17">
+        <v>5.5</v>
+      </c>
+      <c r="F26" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J26" s="1" t="s">
+      <c r="G26" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="I26" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="J26" s="17" t="s">
         <v>91</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>92</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q26" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="R26" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N26" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="O26" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="P26" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q26" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="R26" s="17" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3542,10 +3562,10 @@
         <v>87</v>
       </c>
       <c r="B27" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="C27" s="18" t="s">
         <v>185</v>
-      </c>
-      <c r="C27" s="18" t="s">
-        <v>186</v>
       </c>
       <c r="D27" s="18">
         <v>1</v>
@@ -3566,7 +3586,7 @@
         <v>91</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>94</v>
@@ -3598,10 +3618,10 @@
         <v>87</v>
       </c>
       <c r="B28" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C28" s="17" t="s">
         <v>165</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>166</v>
       </c>
       <c r="D28" s="17">
         <v>1</v>
@@ -3654,10 +3674,10 @@
         <v>87</v>
       </c>
       <c r="B29" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C29" s="17" t="s">
         <v>160</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>161</v>
       </c>
       <c r="D29" s="17">
         <v>4</v>
@@ -3710,10 +3730,10 @@
         <v>87</v>
       </c>
       <c r="B30" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C30" s="17" t="s">
         <v>146</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>147</v>
       </c>
       <c r="D30" s="17">
         <v>3</v>
@@ -3766,10 +3786,10 @@
         <v>87</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D31" s="1">
         <v>12</v>
@@ -3788,13 +3808,13 @@
         <v>91</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M31" s="1" t="s">
         <v>65</v>
@@ -3820,10 +3840,10 @@
         <v>87</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="D32" s="1">
         <v>12</v>
@@ -3982,10 +4002,10 @@
         <v>87</v>
       </c>
       <c r="B35" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" s="17" t="s">
         <v>109</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>110</v>
       </c>
       <c r="D35" s="17">
         <v>4</v>
@@ -4094,7 +4114,7 @@
         <v>87</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>29</v>
@@ -4116,10 +4136,10 @@
         <v>92</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>65</v>
@@ -4148,10 +4168,10 @@
         <v>87</v>
       </c>
       <c r="B38" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="C38" s="17" t="s">
         <v>189</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>190</v>
       </c>
       <c r="D38" s="17">
         <v>2</v>
@@ -4256,10 +4276,10 @@
         <v>88</v>
       </c>
       <c r="B40" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C40" s="17" t="s">
         <v>183</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>184</v>
       </c>
       <c r="D40" s="17">
         <v>1</v>
@@ -4310,10 +4330,10 @@
         <v>88</v>
       </c>
       <c r="B41" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="C41" s="26" t="s">
         <v>208</v>
-      </c>
-      <c r="C41" s="26" t="s">
-        <v>209</v>
       </c>
       <c r="D41" s="17">
         <v>1</v>
@@ -4337,7 +4357,7 @@
         <v>91</v>
       </c>
       <c r="K41" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L41" s="17" t="s">
         <v>94</v>
@@ -4366,10 +4386,10 @@
         <v>88</v>
       </c>
       <c r="B42" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C42" s="17" t="s">
         <v>137</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>138</v>
       </c>
       <c r="D42" s="17">
         <v>8</v>
@@ -4396,7 +4416,7 @@
         <v>92</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M42" s="1" t="s">
         <v>94</v>
@@ -4422,7 +4442,7 @@
         <v>88</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1">
@@ -4529,7 +4549,7 @@
         <v>3</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D45" s="17">
         <v>4</v>
@@ -4559,7 +4579,7 @@
         <v>92</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N45" s="1" t="s">
         <v>94</v>
@@ -4582,10 +4602,10 @@
         <v>88</v>
       </c>
       <c r="B46" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C46" s="17" t="s">
         <v>175</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>176</v>
       </c>
       <c r="D46" s="17">
         <v>2</v>
@@ -4609,7 +4629,7 @@
         <v>92</v>
       </c>
       <c r="K46" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L46" s="17" t="s">
         <v>94</v>
@@ -4692,7 +4712,7 @@
         <v>88</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1">
@@ -4850,10 +4870,10 @@
         <v>88</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="D51" s="1">
         <v>3</v>
@@ -4983,7 +5003,7 @@
         <v>92</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L53" s="1" t="s">
         <v>94</v>
@@ -5012,10 +5032,10 @@
         <v>88</v>
       </c>
       <c r="B54" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="C54" s="17" t="s">
         <v>289</v>
-      </c>
-      <c r="C54" s="17" t="s">
-        <v>290</v>
       </c>
       <c r="D54" s="17">
         <v>2</v>
@@ -5068,7 +5088,7 @@
         <v>89</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C55" s="17"/>
       <c r="D55" s="17">
@@ -5085,7 +5105,7 @@
         <v>91</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>94</v>
@@ -5120,10 +5140,10 @@
         <v>89</v>
       </c>
       <c r="B56" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="C56" s="17" t="s">
         <v>131</v>
-      </c>
-      <c r="C56" s="17" t="s">
-        <v>132</v>
       </c>
       <c r="D56" s="17">
         <v>2</v>
@@ -5139,7 +5159,7 @@
         <v>91</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>94</v>
@@ -5174,10 +5194,10 @@
         <v>89</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D57" s="1">
         <v>1</v>
@@ -5303,10 +5323,10 @@
         <v>91</v>
       </c>
       <c r="K59" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L59" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M59" s="17" t="s">
         <v>94</v>
@@ -5386,10 +5406,10 @@
         <v>89</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D61" s="17">
         <v>3</v>
@@ -5405,7 +5425,7 @@
         <v>91</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>94</v>
@@ -5459,7 +5479,7 @@
         <v>91</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J62" s="1" t="s">
         <v>94</v>
@@ -5548,10 +5568,10 @@
         <v>89</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D64" s="1">
         <v>2</v>
@@ -5605,7 +5625,7 @@
         <v>2</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D65" s="17">
         <v>3</v>
@@ -5629,7 +5649,7 @@
         <v>92</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>94</v>
@@ -5658,10 +5678,10 @@
         <v>89</v>
       </c>
       <c r="B66" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="C66" s="17" t="s">
         <v>243</v>
-      </c>
-      <c r="C66" s="17" t="s">
-        <v>244</v>
       </c>
       <c r="D66" s="17">
         <v>1</v>
@@ -5688,7 +5708,7 @@
         <v>91</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M66" s="1" t="s">
         <v>94</v>
@@ -5714,10 +5734,10 @@
         <v>89</v>
       </c>
       <c r="B67" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="C67" s="17" t="s">
         <v>245</v>
-      </c>
-      <c r="C67" s="17" t="s">
-        <v>246</v>
       </c>
       <c r="D67" s="17">
         <v>1</v>
@@ -5770,7 +5790,7 @@
         <v>66</v>
       </c>
       <c r="G87" s="24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -5822,7 +5842,7 @@
         <v>76</v>
       </c>
       <c r="G92" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -5845,12 +5865,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:R95" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}"/>
-  <conditionalFormatting sqref="A26:A34 A57:A60 A64 A23:A24 A36:A37 A39 A44 A46:A52 A41 A2:A21">
+  <conditionalFormatting sqref="A27:A34 A57:A60 A64 A23 A36:A37 A39 A44 A46:A52 A41 A2:A20">
     <cfRule type="cellIs" dxfId="33" priority="38" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G72:H72 G89:G92 I61:J62 H88:K92 G73:K87 J72:K72 G93:K1048576 J63 J40:K40 J25:K25 G68:K71 G57:K60 L57:R59 G26:R34 I55:J56 G64:R64 I13:L13 I4:L4 J22:R22 J53:R53 L54:R54 L68:R1048576 L67 L66:R66 J65:R65 G36:R37 I35:R35 G39:R39 J38:R38 G44:R44 I42:R42 N43:R43 G46:R52 I45:R45 M5:N5 G9:R11 J12:M12 G6:M8 G1:R2 G23:R24 F3:R3 G41:R41 G14:R21">
+  <conditionalFormatting sqref="G72:H72 G89:G92 I61:J62 H88:K92 G73:K87 J72:K72 G93:K1048576 J63 J40:K40 J25:K25 G68:K71 G57:K60 L57:R59 G27:R34 I55:J56 G64:R64 I13:L13 I4:L4 J22:L22 J53:R53 L54:R54 L68:R1048576 L67 L66:R66 J65:R65 G36:R37 I35:R35 G39:R39 J38:R38 G44:R44 I42:R42 N43:R43 G46:R52 I45:R45 M5:N5 G9:R11 J12:M12 G6:M8 G1:R2 J24:M24 F3:R3 G41:R41 G14:R20 M21:N21 G23:N23 K26:M26">
     <cfRule type="cellIs" dxfId="32" priority="22" operator="equal">
       <formula>"Done (Needs Review)"</formula>
     </cfRule>
@@ -5885,7 +5905,7 @@
       <formula>"Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M20:R21 G14:R17 I18:R18 I4:L4 M5:N5">
+  <conditionalFormatting sqref="M20:R20 G14:R17 I18:R18 I4:L4 M5:N5 M21:N21">
     <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
@@ -5895,7 +5915,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M20:R21 L4 M5:N5">
+  <conditionalFormatting sqref="M20:R20 L4 M5:N5 M21:N21">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -5915,7 +5935,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I61:J62 J27:K27 J63 J40:K40 G26:R26 J25:K25 G57:K60 L57:R59 G28:R34 I55:J56 G64:R64 G19:R19 I13:L13 J22:R22 G41:R41 J53:R53 L54:R54 G36:R37 I35:R35 G39:R39 J38:R38 G44:R44 I42:R42 N43:R43 G46:R52 I45:R45 K3:R3 G9:R11 J12:M12 G6:M8 G23:R24">
+  <conditionalFormatting sqref="I61:J62 J27:K27 J63 J40:K40 K26:M26 J25:K25 G57:K60 L57:R59 G28:R34 I55:J56 G64:R64 G19:R19 I13:L13 J22:L22 G41:R41 J53:R53 L54:R54 G36:R37 I35:R35 G39:R39 J38:R38 G44:R44 I42:R42 N43:R43 G46:R52 I45:R45 K3:R3 G9:R11 J12:M12 G6:M8 J24:M24 G23:N23">
     <cfRule type="colorScale" priority="86">
       <colorScale>
         <cfvo type="min"/>
@@ -6056,10 +6076,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6081,56 +6101,56 @@
         <v>90</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D1" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>315</v>
+        <v>343</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>316</v>
+        <v>344</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>334</v>
+        <v>314</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>335</v>
+        <v>315</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6138,79 +6158,79 @@
         <v>87</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>309</v>
+        <v>341</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>310</v>
+        <v>342</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>119</v>
+        <v>333</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>120</v>
+        <v>334</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>288</v>
+        <v>309</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>292</v>
+        <v>118</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>291</v>
+        <v>119</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6218,10 +6238,10 @@
         <v>89</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>7</v>
@@ -6230,7 +6250,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6238,10 +6258,10 @@
         <v>89</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>7</v>
@@ -6250,7 +6270,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6258,10 +6278,10 @@
         <v>98</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>7</v>
@@ -6270,7 +6290,7 @@
         <v>18</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -6278,10 +6298,10 @@
         <v>98</v>
       </c>
       <c r="B11" s="17" t="s">
+        <v>323</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>324</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>325</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>7</v>
@@ -6290,10 +6310,10 @@
         <v>18</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="G11" s="27" t="s">
-        <v>331</v>
+        <v>117</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -6301,10 +6321,10 @@
         <v>98</v>
       </c>
       <c r="B12" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>313</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>314</v>
       </c>
       <c r="D12" s="17" t="s">
         <v>7</v>
@@ -6313,10 +6333,10 @@
         <v>18</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="G12" s="27" t="s">
-        <v>331</v>
+        <v>117</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -6324,10 +6344,10 @@
         <v>98</v>
       </c>
       <c r="B13" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>177</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>178</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>7</v>
@@ -6336,7 +6356,7 @@
         <v>18</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -6344,10 +6364,10 @@
         <v>98</v>
       </c>
       <c r="B14" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>167</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>168</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>7</v>
@@ -6356,7 +6376,7 @@
         <v>18</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6364,10 +6384,10 @@
         <v>98</v>
       </c>
       <c r="B15" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>169</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>170</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>7</v>
@@ -6376,7 +6396,7 @@
         <v>18</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="24" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -6384,10 +6404,10 @@
         <v>98</v>
       </c>
       <c r="B16" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>126</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>127</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>7</v>
@@ -6396,7 +6416,7 @@
         <v>18</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6404,10 +6424,10 @@
         <v>98</v>
       </c>
       <c r="B17" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>210</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>211</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>7</v>
@@ -6416,7 +6436,7 @@
         <v>18</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6424,10 +6444,10 @@
         <v>87</v>
       </c>
       <c r="B18" s="17" t="s">
+        <v>305</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>306</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>307</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>7</v>
@@ -6436,58 +6456,64 @@
         <v>18</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>308</v>
+        <v>286</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>318</v>
+        <v>287</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>326</v>
+        <v>307</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>7</v>
@@ -6496,38 +6522,38 @@
         <v>18</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="24" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>238</v>
+        <v>325</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>241</v>
+        <v>310</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>7</v>
@@ -6536,38 +6562,38 @@
         <v>18</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>111</v>
+        <v>319</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>113</v>
+        <v>320</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="24" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>212</v>
+        <v>240</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>7</v>
@@ -6575,22 +6601,19 @@
       <c r="E25" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G25" s="22" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F25" s="17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>179</v>
+        <v>110</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>174</v>
+        <v>112</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>7</v>
@@ -6599,18 +6622,18 @@
         <v>22</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>157</v>
+        <v>238</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>158</v>
+        <v>211</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>7</v>
@@ -6619,27 +6642,30 @@
         <v>18</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>87</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6647,10 +6673,10 @@
         <v>87</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>205</v>
+        <v>156</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>206</v>
+        <v>157</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>7</v>
@@ -6658,77 +6684,79 @@
       <c r="E29" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F29" s="17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F29" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>220</v>
+        <v>161</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>219</v>
+        <v>162</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>329</v>
+        <v>204</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>333</v>
+        <v>205</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="E31" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>332</v>
-      </c>
-      <c r="C32" s="17"/>
+        <v>219</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>218</v>
+      </c>
       <c r="D32" s="17" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="E32" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F32" s="17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F32" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>69</v>
@@ -6737,7 +6765,7 @@
         <v>18</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6745,50 +6773,48 @@
         <v>88</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>240</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>242</v>
-      </c>
+        <v>331</v>
+      </c>
+      <c r="C34" s="17"/>
       <c r="D34" s="17" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="E34" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>180</v>
+        <v>321</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>172</v>
+        <v>322</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>221</v>
+        <v>239</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>222</v>
+        <v>241</v>
       </c>
       <c r="D36" s="17" t="s">
         <v>7</v>
@@ -6796,118 +6822,158 @@
       <c r="E36" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F36" s="17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E37" s="17" t="s">
         <v>22</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>327</v>
+        <v>220</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>328</v>
+        <v>221</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="E38" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F38" s="17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="D56" s="22" t="s">
+      <c r="F38" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D39" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F56" s="22" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D57" s="22" t="s">
+      <c r="E39" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>326</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>327</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F57" s="22" t="s">
+      <c r="F40" s="17" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D58" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F58" s="22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F59" s="22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="D58" s="22" t="s">
+      <c r="D60" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F58" s="22" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="22" t="s">
+      <c r="F60" s="22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="D59" s="22" t="s">
+      <c r="D61" s="22" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D60" s="22" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D61" s="22" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D62" s="22" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D63" s="22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D64" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="22" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A26 A29:A38">
+  <conditionalFormatting sqref="A31:A40 A2:A28">
     <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F38">
+  <conditionalFormatting sqref="F2:F40">
     <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
@@ -6919,14 +6985,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E38" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
-      <formula1>$D$56:$D$63</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E40" xr:uid="{154ECC09-7D67-45A6-90DF-1961A685E627}">
+      <formula1>$D$58:$D$65</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A38" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
-      <formula1>$A$56:$A$59</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A40" xr:uid="{72EC6FF7-955E-4ED7-9B0B-51830424EBF6}">
+      <formula1>$A$58:$A$61</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F38" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
-      <formula1>$F$56:$F$58</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F40" xr:uid="{F81763E8-DE35-4D24-BE53-2E916D17EE9E}">
+      <formula1>$F$58:$F$60</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6957,20 +7023,20 @@
   <sheetData>
     <row r="1" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
     </row>
     <row r="2" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -7024,16 +7090,16 @@
         <v>83</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
@@ -7053,16 +7119,16 @@
         <v>81</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
@@ -7082,16 +7148,16 @@
         <v>79</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
@@ -7111,16 +7177,16 @@
         <v>77</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
@@ -7140,16 +7206,16 @@
         <v>74</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
@@ -7169,16 +7235,16 @@
         <v>72</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
@@ -7198,16 +7264,16 @@
         <v>70</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
@@ -7227,16 +7293,16 @@
         <v>67</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
@@ -7256,13 +7322,13 @@
         <v>65</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>65</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>65</v>
@@ -7308,22 +7374,22 @@
         <v>86</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C1" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>250</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>261</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>251</v>
-      </c>
       <c r="F1" s="20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7331,22 +7397,22 @@
         <v>98</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7354,22 +7420,22 @@
         <v>98</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>265</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7377,22 +7443,22 @@
         <v>87</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7400,22 +7466,22 @@
         <v>87</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7423,22 +7489,22 @@
         <v>87</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7446,22 +7512,22 @@
         <v>87</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>276</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -7469,10 +7535,10 @@
         <v>98</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G22" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -7480,10 +7546,10 @@
         <v>87</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G23" s="22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -7491,7 +7557,7 @@
         <v>88</v>
       </c>
       <c r="G24" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -7566,22 +7632,22 @@
         <v>86</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C1" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>250</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>261</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>251</v>
-      </c>
       <c r="F1" s="20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7589,22 +7655,22 @@
         <v>98</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>268</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7612,22 +7678,22 @@
         <v>87</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>271</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -7635,7 +7701,7 @@
         <v>87</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -7643,10 +7709,10 @@
         <v>87</v>
       </c>
       <c r="B5" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>283</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7654,7 +7720,7 @@
         <v>87</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -7662,7 +7728,7 @@
         <v>87</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -7670,10 +7736,10 @@
         <v>98</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -7681,10 +7747,10 @@
         <v>87</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G21" s="22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -7692,7 +7758,7 @@
         <v>88</v>
       </c>
       <c r="G22" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -7747,20 +7813,20 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -7804,21 +7870,21 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -7855,21 +7921,21 @@
       <c r="M5" s="7"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -7940,21 +8006,21 @@
       <c r="M10" s="6"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -8008,21 +8074,21 @@
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">

</xml_diff>

<commit_message>
fix using rat head as a footstool
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102730451\Desktop\sdffsdfs\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2247CF2-3722-41A8-B998-8E82C755A4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2B750D-E27D-4C8D-B8C4-B92CE1B99BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
@@ -1497,56 +1497,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="73">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAF8A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4FBA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1914,6 +1864,56 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEAF8A4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC4FBA9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6848,21 +6848,21 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="5" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:R6">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
       <formula>"Done (Needs Review)"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="40" priority="2" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",G6)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
       <formula>"Done (Needs Testing)"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
       <formula>"Started"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6898,7 +6898,7 @@
   <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7012,24 +7012,24 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:7" s="24" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="17" t="s">
         <v>355</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>116</v>
+      <c r="F6" s="17" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -7906,114 +7906,114 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A37:A46 A4 A8:A34">
-    <cfRule type="cellIs" dxfId="42" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="28" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4 F8:F46">
-    <cfRule type="cellIs" dxfId="41" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="25" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="26" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="27" operator="equal">
       <formula>"Unfixed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="cellIs" dxfId="38" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="24" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="37" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="21" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="22" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="23" operator="equal">
       <formula>"Unfixed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="cellIs" dxfId="34" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="20" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="33" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="17" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="18" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="19" operator="equal">
       <formula>"Unfixed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9">
-    <cfRule type="cellIs" dxfId="30" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="16" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="29" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="13" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="14" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="15" operator="equal">
       <formula>"Unfixed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="12" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="9" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
       <formula>"Unfixed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="22" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>"Unfixed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"Working On"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>"Unfixed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8600,28 +8600,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A7">
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G7">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"More Data Needed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"Acceptable"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"Unacceptable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8801,18 +8801,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A7">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G3">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"More Data Needed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Acceptable"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Unacceptable"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Finally fixed that stupid teleportation glitch when tangling when strings are held
It was the stupidest problem and the solution was somehow ever stupider, I hated every moment I spent on this problem, and I feel like a worse person afterwards
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102730451\Desktop\sdffsdfs\strung-along\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Tim\Desktop\Git\strung-along-again\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537BBF0F-300A-4CF2-A285-21B6877AC76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF442030-CD12-48DC-99BF-6730DA3AEC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -2542,7 +2542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A56" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -6897,8 +6897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6989,7 +6989,7 @@
         <v>22</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
lil' funny small changes
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Tim\Desktop\Git\strung-along-again\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF442030-CD12-48DC-99BF-6730DA3AEC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92586750-85DD-49E3-AF16-223E9292B157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
@@ -6898,7 +6898,7 @@
   <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6969,7 +6969,7 @@
         <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
making changes based on the excel doc
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University 2022\Game Design Capstone\Game Repo\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE00B69-D57A-4256-8F42-27100BBBC879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249B1D1C-2F8C-4AC2-A830-0674165B411E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -2699,28 +2699,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.44140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.88671875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="22"/>
-    <col min="5" max="5" width="10.109375" style="22" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="20.44140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="22"/>
+    <col min="5" max="5" width="10.140625" style="22" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="20.42578125" style="22" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" style="22" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" style="22" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" style="22" customWidth="1"/>
-    <col min="13" max="13" width="15.5546875" style="22" customWidth="1"/>
-    <col min="14" max="18" width="11.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.109375" style="22"/>
+    <col min="11" max="11" width="19.7109375" style="22" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="22" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" style="22" customWidth="1"/>
+    <col min="14" max="18" width="11.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>85</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>86</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>86</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>86</v>
       </c>
@@ -2938,7 +2938,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>86</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>86</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>86</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>86</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>86</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>86</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>86</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>90</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="Q11" s="1" t="s">
         <v>64</v>
@@ -3316,7 +3316,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>86</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>90</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>64</v>
@@ -3370,7 +3370,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>86</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>90</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>64</v>
@@ -3478,7 +3478,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>86</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>86</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>87</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>87</v>
       </c>
@@ -3694,7 +3694,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>87</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>87</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>87</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>87</v>
       </c>
@@ -3910,7 +3910,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>87</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:18" s="23" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" s="23" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>87</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>87</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>87</v>
       </c>
@@ -4122,7 +4122,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>87</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>87</v>
       </c>
@@ -4230,7 +4230,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>87</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>88</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>88</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>88</v>
       </c>
@@ -4444,7 +4444,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>88</v>
       </c>
@@ -4498,7 +4498,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:18" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>88</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:18" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>97</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="72" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>97</v>
       </c>
@@ -4666,7 +4666,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:18" s="23" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" s="23" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>97</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:18" s="23" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" s="23" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>97</v>
       </c>
@@ -4778,7 +4778,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>97</v>
       </c>
@@ -4834,7 +4834,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>97</v>
       </c>
@@ -4890,7 +4890,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>97</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>97</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>97</v>
       </c>
@@ -5054,7 +5054,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>97</v>
       </c>
@@ -5108,7 +5108,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>97</v>
       </c>
@@ -5164,7 +5164,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>97</v>
       </c>
@@ -5220,7 +5220,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="47" spans="1:18" s="23" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" s="23" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
         <v>97</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:18" s="23" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" s="23" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
         <v>97</v>
       </c>
@@ -5330,7 +5330,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:18" s="23" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" s="23" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
         <v>97</v>
       </c>
@@ -5386,7 +5386,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="1:18" s="23" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" s="23" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
         <v>97</v>
       </c>
@@ -5440,7 +5440,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>97</v>
       </c>
@@ -5496,7 +5496,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:18" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
         <v>97</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:18" s="23" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" s="23" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
         <v>86</v>
       </c>
@@ -5608,7 +5608,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="54" spans="1:18" s="23" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" s="23" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
         <v>86</v>
       </c>
@@ -5662,7 +5662,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
         <v>86</v>
       </c>
@@ -5718,7 +5718,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
         <v>86</v>
       </c>
@@ -5772,7 +5772,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
         <v>86</v>
       </c>
@@ -5828,7 +5828,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
         <v>86</v>
       </c>
@@ -5884,7 +5884,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
         <v>86</v>
       </c>
@@ -5940,7 +5940,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
         <v>86</v>
       </c>
@@ -5996,7 +5996,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:18" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
         <v>86</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="62" spans="1:18" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
         <v>86</v>
       </c>
@@ -6108,7 +6108,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:18" s="23" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" s="23" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
         <v>86</v>
       </c>
@@ -6164,7 +6164,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="64" spans="1:18" ht="72" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="17" t="s">
         <v>86</v>
       </c>
@@ -6220,7 +6220,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="17" t="s">
         <v>86</v>
       </c>
@@ -6274,7 +6274,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:18" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:18" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="17" t="s">
         <v>86</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="17" t="s">
         <v>86</v>
       </c>
@@ -6382,7 +6382,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
         <v>86</v>
       </c>
@@ -6438,7 +6438,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:18" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:18" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="17" t="s">
         <v>86</v>
       </c>
@@ -6494,7 +6494,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="17" t="s">
         <v>86</v>
       </c>
@@ -6550,7 +6550,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="71" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="17" t="s">
         <v>86</v>
       </c>
@@ -6604,7 +6604,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="17" t="s">
         <v>87</v>
       </c>
@@ -6658,7 +6658,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="73" spans="1:18" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:18" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="17" t="s">
         <v>87</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="74" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="17" t="s">
         <v>87</v>
       </c>
@@ -6770,7 +6770,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="75" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="17" t="s">
         <v>87</v>
       </c>
@@ -6826,7 +6826,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="76" spans="1:18" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:18" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="17" t="s">
         <v>87</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="17" t="s">
         <v>87</v>
       </c>
@@ -6936,7 +6936,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="78" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="17" t="s">
         <v>87</v>
       </c>
@@ -6990,7 +6990,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="17" t="s">
         <v>87</v>
       </c>
@@ -7046,7 +7046,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="17" t="s">
         <v>88</v>
       </c>
@@ -7098,7 +7098,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="81" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="17" t="s">
         <v>88</v>
       </c>
@@ -7152,7 +7152,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="82" spans="1:18" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:18" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="17" t="s">
         <v>88</v>
       </c>
@@ -7204,7 +7204,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="83" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
         <v>88</v>
       </c>
@@ -7258,7 +7258,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="84" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="17" t="s">
         <v>88</v>
       </c>
@@ -7312,7 +7312,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="17" t="s">
         <v>88</v>
       </c>
@@ -7366,7 +7366,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="17" t="s">
         <v>88</v>
       </c>
@@ -7422,7 +7422,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="87" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="17" t="s">
         <v>88</v>
       </c>
@@ -7478,7 +7478,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="88" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="17" t="s">
         <v>88</v>
       </c>
@@ -7534,7 +7534,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F108" s="22" t="s">
         <v>65</v>
       </c>
@@ -7542,7 +7542,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="22" t="s">
         <v>97</v>
       </c>
@@ -7553,7 +7553,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="22" t="s">
         <v>86</v>
       </c>
@@ -7564,7 +7564,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="22" t="s">
         <v>87</v>
       </c>
@@ -7575,7 +7575,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="22" t="s">
         <v>88</v>
       </c>
@@ -7586,7 +7586,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="113" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="6:7" ht="30" x14ac:dyDescent="0.25">
       <c r="F113" s="22" t="s">
         <v>75</v>
       </c>
@@ -7594,7 +7594,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="114" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F114" s="22" t="s">
         <v>32</v>
       </c>
@@ -7602,12 +7602,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="115" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F115" s="22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="116" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F116" s="22" t="s">
         <v>68</v>
       </c>
@@ -7978,18 +7978,18 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="22"/>
-    <col min="2" max="3" width="48.88671875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="22"/>
+    <col min="2" max="3" width="48.85546875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="21.5546875" style="22" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="22"/>
+    <col min="6" max="6" width="11.28515625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" style="22" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>85</v>
       </c>
@@ -8009,7 +8009,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>86</v>
       </c>
@@ -8029,7 +8029,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>86</v>
       </c>
@@ -8049,7 +8049,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>86</v>
       </c>
@@ -8069,7 +8069,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>86</v>
       </c>
@@ -8089,7 +8089,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>86</v>
       </c>
@@ -8109,7 +8109,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>86</v>
       </c>
@@ -8129,7 +8129,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>87</v>
       </c>
@@ -8149,7 +8149,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>87</v>
       </c>
@@ -8169,7 +8169,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="23" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="23" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>87</v>
       </c>
@@ -8189,7 +8189,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>87</v>
       </c>
@@ -8209,7 +8209,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>87</v>
       </c>
@@ -8227,7 +8227,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>87</v>
       </c>
@@ -8247,7 +8247,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>88</v>
       </c>
@@ -8267,7 +8267,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>88</v>
       </c>
@@ -8287,7 +8287,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>97</v>
       </c>
@@ -8307,7 +8307,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>97</v>
       </c>
@@ -8327,7 +8327,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="23" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" s="23" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>97</v>
       </c>
@@ -8350,7 +8350,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="23" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" s="23" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>97</v>
       </c>
@@ -8373,7 +8373,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="23" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" s="23" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>97</v>
       </c>
@@ -8393,7 +8393,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>97</v>
       </c>
@@ -8413,7 +8413,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>97</v>
       </c>
@@ -8433,7 +8433,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="23" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" s="23" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>97</v>
       </c>
@@ -8453,7 +8453,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>97</v>
       </c>
@@ -8473,7 +8473,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>86</v>
       </c>
@@ -8493,7 +8493,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>86</v>
       </c>
@@ -8513,7 +8513,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>86</v>
       </c>
@@ -8533,7 +8533,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>86</v>
       </c>
@@ -8553,7 +8553,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="23" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" s="23" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>86</v>
       </c>
@@ -8576,7 +8576,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>87</v>
       </c>
@@ -8599,7 +8599,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>86</v>
       </c>
@@ -8619,7 +8619,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>86</v>
       </c>
@@ -8639,7 +8639,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>86</v>
       </c>
@@ -8659,7 +8659,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="23" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" s="23" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>86</v>
       </c>
@@ -8679,7 +8679,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="23" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" s="23" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>86</v>
       </c>
@@ -8699,7 +8699,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>86</v>
       </c>
@@ -8719,7 +8719,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>86</v>
       </c>
@@ -8742,7 +8742,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="111.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>86</v>
       </c>
@@ -8762,7 +8762,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>86</v>
       </c>
@@ -8782,7 +8782,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="23" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" s="23" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>86</v>
       </c>
@@ -8802,7 +8802,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
         <v>86</v>
       </c>
@@ -8822,7 +8822,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
         <v>87</v>
       </c>
@@ -8842,7 +8842,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>87</v>
       </c>
@@ -8862,7 +8862,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>87</v>
       </c>
@@ -8880,7 +8880,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
         <v>87</v>
       </c>
@@ -8900,7 +8900,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
         <v>87</v>
       </c>
@@ -8920,7 +8920,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
         <v>87</v>
       </c>
@@ -8940,7 +8940,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
         <v>87</v>
       </c>
@@ -8960,7 +8960,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
         <v>87</v>
       </c>
@@ -8980,7 +8980,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
         <v>88</v>
       </c>
@@ -9000,7 +9000,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="22" t="s">
         <v>97</v>
       </c>
@@ -9011,7 +9011,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="22" t="s">
         <v>86</v>
       </c>
@@ -9022,7 +9022,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="22" t="s">
         <v>87</v>
       </c>
@@ -9033,7 +9033,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="22" t="s">
         <v>88</v>
       </c>
@@ -9041,22 +9041,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D72" s="22" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D73" s="22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D74" s="22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D75" s="22" t="s">
         <v>68</v>
       </c>
@@ -9214,20 +9214,20 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="9" customWidth="1"/>
-    <col min="4" max="5" width="17.88671875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="10" customWidth="1"/>
-    <col min="7" max="11" width="17.88671875" style="9" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" style="9" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" style="9" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="24.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="9" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="10" customWidth="1"/>
+    <col min="7" max="11" width="17.85546875" style="9" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="9" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="9" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="26" t="s">
         <v>35</v>
@@ -9244,7 +9244,7 @@
       <c r="L1" s="26"/>
       <c r="M1" s="26"/>
     </row>
-    <row r="2" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>84</v>
       </c>
@@ -9285,7 +9285,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="216" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>22</v>
       </c>
@@ -9314,7 +9314,7 @@
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
     </row>
-    <row r="4" spans="1:13" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>18</v>
       </c>
@@ -9343,7 +9343,7 @@
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
     </row>
-    <row r="5" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
@@ -9372,7 +9372,7 @@
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
     </row>
-    <row r="6" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>32</v>
       </c>
@@ -9401,7 +9401,7 @@
       <c r="L6" s="11"/>
       <c r="M6" s="11"/>
     </row>
-    <row r="7" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>75</v>
       </c>
@@ -9430,7 +9430,7 @@
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="1:13" ht="144" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -9459,7 +9459,7 @@
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
     </row>
-    <row r="9" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>7</v>
       </c>
@@ -9488,7 +9488,7 @@
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>68</v>
       </c>
@@ -9517,7 +9517,7 @@
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>65</v>
       </c>
@@ -9563,19 +9563,19 @@
       <selection activeCell="F10" sqref="F10:G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="22"/>
-    <col min="2" max="2" width="38.33203125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="59.88671875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="22" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.44140625" style="22" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="22"/>
+    <col min="2" max="2" width="38.28515625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="59.85546875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" style="22" customWidth="1"/>
     <col min="7" max="7" width="18" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="22"/>
+    <col min="8" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>85</v>
       </c>
@@ -9598,7 +9598,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>97</v>
       </c>
@@ -9621,7 +9621,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>97</v>
       </c>
@@ -9644,7 +9644,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>86</v>
       </c>
@@ -9667,7 +9667,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>86</v>
       </c>
@@ -9690,7 +9690,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>86</v>
       </c>
@@ -9713,7 +9713,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>86</v>
       </c>
@@ -9736,7 +9736,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>97</v>
       </c>
@@ -9747,7 +9747,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>86</v>
       </c>
@@ -9758,7 +9758,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>87</v>
       </c>
@@ -9766,7 +9766,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>88</v>
       </c>
@@ -9821,19 +9821,19 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="22"/>
-    <col min="2" max="2" width="38.33203125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="59.88671875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="22" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.44140625" style="22" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="22"/>
+    <col min="2" max="2" width="38.28515625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="59.85546875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" style="22" customWidth="1"/>
     <col min="7" max="7" width="18" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="22"/>
+    <col min="8" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>85</v>
       </c>
@@ -9856,7 +9856,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>97</v>
       </c>
@@ -9879,7 +9879,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>86</v>
       </c>
@@ -9902,7 +9902,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>86</v>
       </c>
@@ -9910,7 +9910,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>86</v>
       </c>
@@ -9921,7 +9921,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>86</v>
       </c>
@@ -9929,7 +9929,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>86</v>
       </c>
@@ -9937,7 +9937,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>97</v>
       </c>
@@ -9948,7 +9948,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>86</v>
       </c>
@@ -9959,7 +9959,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>87</v>
       </c>
@@ -9967,7 +9967,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>88</v>
       </c>
@@ -10012,12 +10012,12 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="26" t="s">
         <v>35</v>
@@ -10034,7 +10034,7 @@
       <c r="L1" s="26"/>
       <c r="M1" s="26"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>36</v>
       </c>
@@ -10075,7 +10075,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>49</v>
       </c>
@@ -10092,7 +10092,7 @@
       <c r="L3" s="27"/>
       <c r="M3" s="27"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>50</v>
       </c>
@@ -10109,7 +10109,7 @@
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>51</v>
       </c>
@@ -10126,7 +10126,7 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>52</v>
       </c>
@@ -10143,7 +10143,7 @@
       <c r="L6" s="27"/>
       <c r="M6" s="27"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>53</v>
       </c>
@@ -10160,7 +10160,7 @@
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>54</v>
       </c>
@@ -10177,7 +10177,7 @@
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>55</v>
       </c>
@@ -10194,7 +10194,7 @@
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>56</v>
       </c>
@@ -10211,7 +10211,7 @@
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
         <v>57</v>
       </c>
@@ -10228,7 +10228,7 @@
       <c r="L11" s="27"/>
       <c r="M11" s="27"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>58</v>
       </c>
@@ -10245,7 +10245,7 @@
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>59</v>
       </c>
@@ -10262,7 +10262,7 @@
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>60</v>
       </c>
@@ -10279,7 +10279,7 @@
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>61</v>
       </c>
@@ -10296,7 +10296,7 @@
       <c r="L15" s="27"/>
       <c r="M15" s="27"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>62</v>
       </c>
@@ -10313,7 +10313,7 @@
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Fixed loose strings on swinging + object push/pull limited to one axis
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University 2022\Game Design Capstone\Game Repo\strung-along\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Tim\Desktop\Git\strung-along-again\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F60A1B-5B66-468A-A07E-097685690B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7861A4-0366-44FB-B96D-985ED852FD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -2699,8 +2699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3532,7 +3532,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>86</v>
       </c>
@@ -3577,7 +3577,7 @@
         <v>90</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>90</v>
+        <v>152</v>
       </c>
       <c r="Q16" s="1" t="s">
         <v>64</v>
@@ -4284,7 +4284,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>88</v>
       </c>
@@ -4327,7 +4327,7 @@
         <v>91</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>91</v>
+        <v>152</v>
       </c>
       <c r="Q30" s="1" t="s">
         <v>64</v>
@@ -7974,8 +7974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8166,7 +8166,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="23" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
lil' baby beep boop prod doc change :))
</commit_message>
<xml_diff>
--- a/Admin Files/The Prod Doc.xlsx
+++ b/Admin Files/The Prod Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Tim\Desktop\Git\strung-along-again\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7861A4-0366-44FB-B96D-985ED852FD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9A7748-04A1-4892-8172-6AD245E0EAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Tracking" sheetId="1" r:id="rId1"/>
@@ -2699,8 +2699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
   <dimension ref="A1:R116"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3577,10 +3577,10 @@
         <v>90</v>
       </c>
       <c r="P16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q16" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="R16" s="1" t="s">
         <v>64</v>
@@ -4327,10 +4327,10 @@
         <v>91</v>
       </c>
       <c r="P30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q30" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="Q30" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="R30" s="1" t="s">
         <v>64</v>
@@ -7974,7 +7974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>